<commit_message>
included user stories https://github.com/i-adopt/users_stories/issues/3 modified codes, domain areas and description of user stories https://github.com/i-adopt/users_stories/issues/15
</commit_message>
<xml_diff>
--- a/I-AdoptUserStoriesanalysis_25022020.xlsx
+++ b/I-AdoptUserStoriesanalysis_25022020.xlsx
@@ -5,7 +5,7 @@
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anusu\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anusu\python-workspace\usecase_analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -18,11 +18,9 @@
     <sheet name="Results_UseCases" sheetId="7" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Analysis_Coding!$D$2:$D$15</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Analysis_Coding!$D$2:$D$16</definedName>
     <definedName name="_xlchart.0" hidden="1">Results_UseCases!$B$16:$I$16</definedName>
     <definedName name="_xlchart.1" hidden="1">Results_UseCases!$B$1:$I$1</definedName>
-    <definedName name="_xlchart.2" hidden="1">Results_UseCases!$B$16:$I$16</definedName>
-    <definedName name="_xlchart.3" hidden="1">Results_UseCases!$B$1:$I$1</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -34,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="183">
   <si>
     <t>https://github.com/i-adopt/users_stories/issues/1</t>
   </si>
@@ -267,9 +265,6 @@
   </si>
   <si>
     <t>Animal Ecology, Biodiversity and Ecosystem Research</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Oceanography</t>
   </si>
   <si>
     <r>
@@ -2111,9 +2106,6 @@
     <t>Ecology of Agricultural Landscapes</t>
   </si>
   <si>
-    <t>use standaridzed terminologies mappings to improve data annotation.</t>
-  </si>
-  <si>
     <t>semantic modelling, terminology management</t>
   </si>
   <si>
@@ -2127,6 +2119,177 @@
   </si>
   <si>
     <t>N (number of user stories)</t>
+  </si>
+  <si>
+    <t>use agreed mappings or alignments between terminologies to improve data exchange and integration</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Oceanography (check with Gwen)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">terminology alignment terminology management, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>data integration and analysis, semantic data search, terminology search, and semantic modelling</t>
+    </r>
+  </si>
+  <si>
+    <t>https://github.com/i-adopt/users_stories/issues/3</t>
+  </si>
+  <si>
+    <t>Soil Data manager - Normalize data - Achievement of a standard</t>
+  </si>
+  <si>
+    <t>Soil data manager</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lbtgnn68 </t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>observableProperties (together with UnitsOfMeasure, and Processes</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">) would result in </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>unambiguous descriptions</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <t>Soil; Geographic information; Biology; Biochemistry; Microbiology; Chemistry; Mineralogy; Pedology; Physics; Hydrology; Micromorphology</t>
+  </si>
+  <si>
+    <t>Usually, relational databases store data according to a physical implementation into tables, records, and columns where tables partly identify natural entities, columns identify properties (parameters) and records the recorded data (semantic representation). Unnormalized structures are unfortunately characterized by different notations of the same parameter, or feature-of-interest, related to different natural entities. Searching for all properties related to nitrogen in an unnormalized database means checking manually all coding for every column and table (hundreds of fields). No query automatically implements such a simple search. Normalizing the database would allow for a simple query to enable such a search.
+The achievement of a standard goes through the normalizing step.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Natural Sciences </t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>normalize</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (both) the </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>collected (and collectable) soil</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> information in agreement with the </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>INSPIRE</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> directive (https://inspire.ec.europa.eu/id/document/tg/so; https://inspire.ec.europa.eu/data-model/approved/r4618-ir/html/ - Themes&gt;Annex III&gt;SO) ) according to the </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Observation and Measurement Standard </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">(https://www.opengeospatial.org/standards/om),
+</t>
+    </r>
+  </si>
+  <si>
+    <t>transform the representation of observable properties (&amp;related concepts) from inspire model to O&amp;M standard to enable their explicit descriptions</t>
   </si>
 </sst>
 </file>
@@ -2298,7 +2461,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -2310,9 +2473,6 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2391,6 +2551,24 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -3380,7 +3558,7 @@
   <dimension ref="A1:B20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A6"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3389,105 +3567,105 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
-        <v>92</v>
+      <c r="A1" s="8" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="10" t="s">
-        <v>118</v>
+      <c r="A2" s="9" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="10" t="s">
-        <v>117</v>
+      <c r="A3" s="9" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="10" t="s">
-        <v>96</v>
+      <c r="A4" s="9" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="10" t="s">
-        <v>158</v>
+      <c r="A5" s="9" t="s">
+        <v>157</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="10" t="s">
-        <v>109</v>
+      <c r="A6" s="9" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="10"/>
+      <c r="A7" s="9"/>
     </row>
     <row r="8" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="10"/>
+      <c r="A8" s="9"/>
     </row>
     <row r="9" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="13" t="s">
+      <c r="A9" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="B9" s="10" t="s">
         <v>104</v>
       </c>
-      <c r="B9" s="11" t="s">
-        <v>105</v>
-      </c>
     </row>
     <row r="10" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="13" t="s">
+      <c r="A10" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="B10" s="10" t="s">
         <v>113</v>
-      </c>
-      <c r="B10" s="11" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="22" t="s">
-        <v>125</v>
+      <c r="A12" s="21" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="22" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="22" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="23" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="23" t="s">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="22" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" s="23" t="s">
-        <v>128</v>
-      </c>
-    </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" s="23" t="s">
-        <v>139</v>
+      <c r="A17" s="22" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" s="23" t="s">
-        <v>153</v>
+      <c r="A18" s="22" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" s="23" t="s">
-        <v>88</v>
+      <c r="A19" s="22" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" s="23" t="s">
-        <v>83</v>
+      <c r="A20" s="22" t="s">
+        <v>82</v>
       </c>
     </row>
   </sheetData>
@@ -3501,18 +3679,18 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H16"/>
+  <dimension ref="A1:H17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
+    <sheetView zoomScale="64" zoomScaleNormal="64" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.5703125" style="1" customWidth="1"/>
     <col min="2" max="2" width="24.140625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="13.7109375" style="1" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="16.7109375" style="1" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="16.7109375" style="1" customWidth="1"/>
     <col min="5" max="5" width="21.28515625" style="1" customWidth="1"/>
     <col min="6" max="6" width="20.5703125" style="1" customWidth="1"/>
     <col min="7" max="7" width="14" style="1" customWidth="1"/>
@@ -3520,29 +3698,29 @@
     <col min="12" max="12" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
+    <row r="1" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="13" t="s">
         <v>65</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="13" t="s">
         <v>66</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="C1" s="13" t="s">
         <v>67</v>
       </c>
-      <c r="D1" s="14" t="s">
+      <c r="D1" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="E1" s="14" t="s">
+      <c r="E1" s="13" t="s">
         <v>69</v>
       </c>
-      <c r="F1" s="14" t="s">
+      <c r="F1" s="13" t="s">
         <v>70</v>
       </c>
-      <c r="G1" s="14" t="s">
+      <c r="G1" s="13" t="s">
         <v>71</v>
       </c>
-      <c r="H1" s="15" t="s">
+      <c r="H1" s="14" t="s">
         <v>72</v>
       </c>
     </row>
@@ -3550,7 +3728,7 @@
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="38" t="s">
         <v>3</v>
       </c>
       <c r="C2" s="4" t="s">
@@ -3559,388 +3737,415 @@
       <c r="D2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="E2" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="F2" s="6" t="s">
         <v>79</v>
-      </c>
-      <c r="F2" s="7" t="s">
-        <v>80</v>
       </c>
       <c r="G2" s="4" t="s">
         <v>2</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" ht="210" x14ac:dyDescent="0.25">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="333.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="B3" s="38" t="s">
+        <v>174</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>176</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>181</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>177</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="210" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B4" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C4" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D4" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E4" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="F4" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="F3" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="G3" s="6" t="s">
+      <c r="G4" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="H3" s="4" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="75" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
+      <c r="H4" s="4" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B5" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C5" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D5" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="F4" s="4" t="s">
+      <c r="E5" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="H5" s="4" t="s">
         <v>119</v>
       </c>
-      <c r="G4" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="H4" s="4" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="150" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
+    </row>
+    <row r="6" spans="1:8" ht="150" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B6" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C6" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D6" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="E6" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="F6" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="F5" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="G5" s="4" t="s">
+      <c r="G6" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="H5" s="4" t="s">
+      <c r="H6" s="4" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="105" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
+    <row r="7" spans="1:8" ht="105" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B7" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C7" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="D7" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="E7" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="F7" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="F6" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="G6" s="4" t="s">
+      <c r="G7" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="H6" s="4" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="300" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
+      <c r="H7" s="4" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="300" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B8" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C8" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="D8" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="E7" s="4" t="s">
+      <c r="E8" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="F8" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="F7" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="G7" s="4" t="s">
+      <c r="G8" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="H7" s="4" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" ht="150" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
+      <c r="H8" s="4" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="150" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B9" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C9" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="D8" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="E8" s="4" t="s">
+      <c r="D9" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="F8" s="4" t="s">
-        <v>137</v>
-      </c>
-      <c r="G8" s="4" t="s">
+      <c r="E9" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="G9" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="H8" s="4" t="s">
+      <c r="H9" s="4" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="243.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
+    <row r="10" spans="1:8" ht="243.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B10" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C10" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="D10" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="E9" s="4" t="s">
-        <v>141</v>
-      </c>
-      <c r="F9" s="4" t="s">
-        <v>143</v>
-      </c>
-      <c r="G9" s="4" t="s">
+      <c r="E10" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="G10" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="H9" s="4" t="s">
+      <c r="H10" s="4" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="165" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
+    <row r="11" spans="1:8" ht="165" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B11" s="4" t="s">
         <v>42</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="F10" s="4" t="s">
-        <v>100</v>
-      </c>
-      <c r="G10" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="H10" s="4"/>
-    </row>
-    <row r="11" spans="1:8" ht="90" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>46</v>
       </c>
       <c r="C11" s="4" t="s">
         <v>44</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>148</v>
+        <v>5</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>154</v>
+        <v>98</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="G11" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="H11" s="4"/>
+    </row>
+    <row r="12" spans="1:8" ht="90" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="G12" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="H11" s="4"/>
-    </row>
-    <row r="12" spans="1:8" ht="225" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
+      <c r="H12" s="4"/>
+    </row>
+    <row r="13" spans="1:8" ht="225" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="B13" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="C13" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="D12" s="4" t="s">
+      <c r="D13" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="E12" s="4" t="s">
+      <c r="E13" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="F13" s="4" t="s">
         <v>151</v>
       </c>
-      <c r="F12" s="4" t="s">
-        <v>152</v>
-      </c>
-      <c r="G12" s="4" t="s">
+      <c r="G13" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="H12" s="4" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" ht="406.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
+      <c r="H13" s="4" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="406.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="B13" s="4" t="s">
+      <c r="B14" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="C13" s="4" t="s">
+      <c r="C14" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="D13" s="4" t="s">
+      <c r="D14" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="E13" s="4" t="s">
-        <v>157</v>
-      </c>
-      <c r="F13" s="24" t="s">
+      <c r="E14" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="F14" s="23" t="s">
+        <v>159</v>
+      </c>
+      <c r="G14" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="H14" s="4" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="300" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="D15" s="4" t="s">
         <v>160</v>
       </c>
-      <c r="G13" s="4" t="s">
-        <v>159</v>
-      </c>
-      <c r="H13" s="4" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" ht="300" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="D14" s="4" t="s">
+      <c r="E15" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="G15" s="4" t="s">
         <v>161</v>
       </c>
-      <c r="E14" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="F14" s="4" t="s">
+      <c r="H15" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="G14" s="4" t="s">
+    </row>
+    <row r="16" spans="1:8" ht="90" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E16" s="4" t="s">
         <v>162</v>
       </c>
-      <c r="H14" s="4" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" ht="90" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="D15" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="E15" s="4" t="s">
-        <v>163</v>
-      </c>
-      <c r="F15" s="4" t="s">
+      <c r="F16" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="G15" s="4" t="s">
+      <c r="G16" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="H15" s="4"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="2"/>
-      <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
-      <c r="G16" s="2"/>
+      <c r="H16" s="4"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="2"/>
+      <c r="B17" s="2"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
+      <c r="G17" s="2"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1"/>
-    <hyperlink ref="A4" r:id="rId2"/>
-    <hyperlink ref="A5" r:id="rId3"/>
-    <hyperlink ref="A6" r:id="rId4"/>
-    <hyperlink ref="A7" r:id="rId5"/>
-    <hyperlink ref="A8" r:id="rId6"/>
-    <hyperlink ref="A9" r:id="rId7"/>
-    <hyperlink ref="A10" r:id="rId8"/>
-    <hyperlink ref="A11" r:id="rId9"/>
-    <hyperlink ref="A12" r:id="rId10"/>
-    <hyperlink ref="A13" r:id="rId11"/>
-    <hyperlink ref="A14" r:id="rId12"/>
-    <hyperlink ref="A15" r:id="rId13"/>
-    <hyperlink ref="A3" r:id="rId14"/>
+    <hyperlink ref="A5" r:id="rId2"/>
+    <hyperlink ref="A6" r:id="rId3"/>
+    <hyperlink ref="A7" r:id="rId4"/>
+    <hyperlink ref="A8" r:id="rId5"/>
+    <hyperlink ref="A9" r:id="rId6"/>
+    <hyperlink ref="A10" r:id="rId7"/>
+    <hyperlink ref="A11" r:id="rId8"/>
+    <hyperlink ref="A12" r:id="rId9"/>
+    <hyperlink ref="A13" r:id="rId10"/>
+    <hyperlink ref="A14" r:id="rId11"/>
+    <hyperlink ref="A15" r:id="rId12"/>
+    <hyperlink ref="A16" r:id="rId13"/>
+    <hyperlink ref="A4" r:id="rId14"/>
+    <hyperlink ref="A3" r:id="rId15"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId15"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId16"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N15"/>
+  <dimension ref="A1:N16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17:XFD24"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3960,526 +4165,566 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="63" x14ac:dyDescent="0.25">
-      <c r="A1" s="25" t="str">
+      <c r="A1" s="24" t="str">
         <f>GithubIssues!A1</f>
         <v>github_url</v>
       </c>
-      <c r="B1" s="25" t="str">
+      <c r="B1" s="24" t="str">
         <f>GithubIssues!B1</f>
         <v>issue_title</v>
       </c>
-      <c r="C1" s="27" t="s">
+      <c r="C1" s="26" t="s">
+        <v>105</v>
+      </c>
+      <c r="D1" s="26" t="s">
+        <v>114</v>
+      </c>
+      <c r="E1" s="26" t="s">
         <v>106</v>
       </c>
-      <c r="D1" s="27" t="s">
-        <v>115</v>
-      </c>
-      <c r="E1" s="27" t="s">
+      <c r="F1" s="27" t="s">
         <v>107</v>
       </c>
-      <c r="F1" s="28" t="s">
-        <v>108</v>
-      </c>
-      <c r="G1" s="30" t="s">
+      <c r="G1" s="29" t="s">
+        <v>125</v>
+      </c>
+      <c r="H1" s="29" t="s">
+        <v>134</v>
+      </c>
+      <c r="I1" s="29" t="s">
         <v>126</v>
       </c>
-      <c r="H1" s="30" t="s">
-        <v>135</v>
-      </c>
-      <c r="I1" s="30" t="s">
+      <c r="J1" s="29" t="s">
         <v>127</v>
       </c>
-      <c r="J1" s="30" t="s">
-        <v>128</v>
-      </c>
-      <c r="K1" s="30" t="s">
-        <v>139</v>
-      </c>
-      <c r="L1" s="30" t="s">
-        <v>153</v>
-      </c>
-      <c r="M1" s="30" t="s">
-        <v>88</v>
-      </c>
-      <c r="N1" s="30" t="s">
-        <v>83</v>
+      <c r="K1" s="29" t="s">
+        <v>138</v>
+      </c>
+      <c r="L1" s="29" t="s">
+        <v>152</v>
+      </c>
+      <c r="M1" s="29" t="s">
+        <v>87</v>
+      </c>
+      <c r="N1" s="29" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="2" spans="1:14" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="26" t="str">
+      <c r="A2" s="25" t="str">
         <f>GithubIssues!A2</f>
         <v>https://github.com/i-adopt/users_stories/issues/1</v>
       </c>
-      <c r="B2" s="26" t="str">
+      <c r="B2" s="25" t="str">
         <f>GithubIssues!B2</f>
         <v>Asset manager tracks nitrogen model changes to assess impact on related apps</v>
       </c>
-      <c r="C2" s="17" t="s">
-        <v>109</v>
-      </c>
-      <c r="D2" s="18" t="s">
-        <v>89</v>
-      </c>
-      <c r="E2" s="8" t="s">
+      <c r="C2" s="16" t="s">
+        <v>108</v>
+      </c>
+      <c r="D2" s="17" t="s">
+        <v>88</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="F2" s="11" t="s">
+        <v>165</v>
+      </c>
+      <c r="G2" s="30">
+        <v>1</v>
+      </c>
+      <c r="H2" s="30"/>
+      <c r="I2" s="31"/>
+      <c r="J2" s="31"/>
+      <c r="K2" s="31"/>
+      <c r="L2" s="31">
+        <v>1</v>
+      </c>
+      <c r="M2" s="31"/>
+      <c r="N2" s="31"/>
+    </row>
+    <row r="3" spans="1:14" ht="75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="25" t="str">
+        <f>GithubIssues!A3</f>
+        <v>https://github.com/i-adopt/users_stories/issues/3</v>
+      </c>
+      <c r="B3" s="25" t="str">
+        <f>GithubIssues!B3</f>
+        <v>Soil Data manager - Normalize data - Achievement of a standard</v>
+      </c>
+      <c r="C3" s="39" t="s">
+        <v>95</v>
+      </c>
+      <c r="D3" s="20" t="s">
+        <v>180</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>182</v>
+      </c>
+      <c r="F3" s="40" t="s">
+        <v>152</v>
+      </c>
+      <c r="G3" s="30"/>
+      <c r="H3" s="30"/>
+      <c r="I3" s="31"/>
+      <c r="J3" s="31"/>
+      <c r="K3" s="31"/>
+      <c r="L3" s="31">
+        <v>1</v>
+      </c>
+      <c r="M3" s="31"/>
+      <c r="N3" s="31"/>
+    </row>
+    <row r="4" spans="1:14" ht="68.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="25" t="str">
+        <f>GithubIssues!A4</f>
+        <v>https://github.com/i-adopt/users_stories/issues/4</v>
+      </c>
+      <c r="B4" s="25" t="str">
+        <f>GithubIssues!B4</f>
+        <v>eLTER nitrogen cycle research</v>
+      </c>
+      <c r="C4" s="16" t="s">
+        <v>122</v>
+      </c>
+      <c r="D4" s="18" t="s">
+        <v>115</v>
+      </c>
+      <c r="E4" s="7" t="s">
         <v>111</v>
       </c>
-      <c r="F2" s="12" t="s">
+      <c r="F4" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="G4" s="30"/>
+      <c r="H4" s="30">
+        <v>1</v>
+      </c>
+      <c r="I4" s="31">
+        <v>1</v>
+      </c>
+      <c r="J4" s="31"/>
+      <c r="K4" s="31"/>
+      <c r="L4" s="31"/>
+      <c r="M4" s="31"/>
+      <c r="N4" s="31"/>
+    </row>
+    <row r="5" spans="1:14" ht="55.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="25" t="str">
+        <f>GithubIssues!A5</f>
+        <v>https://github.com/i-adopt/users_stories/issues/5</v>
+      </c>
+      <c r="B5" s="25" t="str">
+        <f>GithubIssues!B5</f>
+        <v>Observer- Annotate observation in situ - interoperable descriptions from start</v>
+      </c>
+      <c r="C5" s="16" t="s">
+        <v>116</v>
+      </c>
+      <c r="D5" s="20" t="s">
+        <v>73</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="G5" s="30"/>
+      <c r="H5" s="30"/>
+      <c r="I5" s="31"/>
+      <c r="J5" s="31">
+        <v>1</v>
+      </c>
+      <c r="K5" s="31"/>
+      <c r="L5" s="31"/>
+      <c r="M5" s="31"/>
+      <c r="N5" s="31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="25" t="str">
+        <f>GithubIssues!A6</f>
+        <v>https://github.com/i-adopt/users_stories/issues/6</v>
+      </c>
+      <c r="B6" s="25" t="str">
+        <f>GithubIssues!B6</f>
+        <v>Vocabulary manager - Select the right URI for "nitrogen" - Better data integration and interoperability</v>
+      </c>
+      <c r="C6" s="16" t="s">
+        <v>108</v>
+      </c>
+      <c r="D6" s="17" t="s">
+        <v>88</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>166</v>
+      </c>
+      <c r="G6" s="30"/>
+      <c r="H6" s="30"/>
+      <c r="I6" s="31"/>
+      <c r="J6" s="31">
+        <v>1</v>
+      </c>
+      <c r="K6" s="31"/>
+      <c r="L6" s="31">
+        <v>1</v>
+      </c>
+      <c r="M6" s="31"/>
+      <c r="N6" s="31"/>
+    </row>
+    <row r="7" spans="1:14" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="25" t="str">
+        <f>GithubIssues!A7</f>
+        <v>https://github.com/i-adopt/users_stories/issues/7</v>
+      </c>
+      <c r="B7" s="25" t="str">
+        <f>GithubIssues!B7</f>
+        <v>Scientist - Integrate data - Efficient analysis</v>
+      </c>
+      <c r="C7" s="16" t="s">
+        <v>122</v>
+      </c>
+      <c r="D7" s="20" t="s">
+        <v>164</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="G7" s="30"/>
+      <c r="H7" s="30">
+        <v>1</v>
+      </c>
+      <c r="I7" s="31">
+        <v>1</v>
+      </c>
+      <c r="J7" s="31"/>
+      <c r="K7" s="31"/>
+      <c r="L7" s="31"/>
+      <c r="M7" s="31"/>
+      <c r="N7" s="31"/>
+    </row>
+    <row r="8" spans="1:14" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="25" t="str">
+        <f>GithubIssues!A8</f>
+        <v>https://github.com/i-adopt/users_stories/issues/8</v>
+      </c>
+      <c r="B8" s="25" t="str">
+        <f>GithubIssues!B8</f>
+        <v>Scientist - find data - to calculate a Nitrogen budget for an algal population</v>
+      </c>
+      <c r="C8" s="16" t="s">
+        <v>122</v>
+      </c>
+      <c r="D8" s="19" t="s">
+        <v>132</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="F8" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="G8" s="30"/>
+      <c r="H8" s="30">
+        <v>1</v>
+      </c>
+      <c r="I8" s="31">
+        <v>1</v>
+      </c>
+      <c r="J8" s="31"/>
+      <c r="K8" s="31"/>
+      <c r="L8" s="31"/>
+      <c r="M8" s="31"/>
+      <c r="N8" s="31"/>
+    </row>
+    <row r="9" spans="1:14" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="25" t="str">
+        <f>GithubIssues!A9</f>
+        <v>https://github.com/i-adopt/users_stories/issues/9</v>
+      </c>
+      <c r="B9" s="25" t="str">
+        <f>GithubIssues!B9</f>
+        <v>Scientist - clean data - (reproduce) elemental analysis of sample</v>
+      </c>
+      <c r="C9" s="16" t="s">
+        <v>122</v>
+      </c>
+      <c r="D9" s="17" t="s">
+        <v>137</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>139</v>
+      </c>
+      <c r="G9" s="30"/>
+      <c r="H9" s="30"/>
+      <c r="I9" s="31">
+        <v>1</v>
+      </c>
+      <c r="J9" s="31"/>
+      <c r="K9" s="31">
+        <v>1</v>
+      </c>
+      <c r="L9" s="31"/>
+      <c r="M9" s="31"/>
+      <c r="N9" s="31"/>
+    </row>
+    <row r="10" spans="1:14" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="25" t="str">
+        <f>GithubIssues!A10</f>
+        <v>https://github.com/i-adopt/users_stories/issues/10</v>
+      </c>
+      <c r="B10" s="25" t="str">
+        <f>GithubIssues!B10</f>
+        <v>Bio-loggingData - NormalizeDataMeasurements - Interoperability</v>
+      </c>
+      <c r="C10" s="16" t="s">
+        <v>95</v>
+      </c>
+      <c r="D10" s="17" t="s">
+        <v>75</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="F10" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="G10" s="30"/>
+      <c r="H10" s="30">
+        <v>1</v>
+      </c>
+      <c r="I10" s="31">
+        <v>1</v>
+      </c>
+      <c r="J10" s="31"/>
+      <c r="K10" s="31"/>
+      <c r="L10" s="31"/>
+      <c r="M10" s="31"/>
+      <c r="N10" s="31"/>
+    </row>
+    <row r="11" spans="1:14" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="25" t="str">
+        <f>GithubIssues!A11</f>
+        <v>https://github.com/i-adopt/users_stories/issues/11</v>
+      </c>
+      <c r="B11" s="25" t="str">
+        <f>GithubIssues!B11</f>
+        <v>scientist - N forms in water - N&lt;-&gt;phytoplankton / AnaEE_01</v>
+      </c>
+      <c r="C11" s="16" t="s">
+        <v>122</v>
+      </c>
+      <c r="D11" s="17" t="s">
+        <v>75</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>143</v>
+      </c>
+      <c r="F11" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="G11" s="30"/>
+      <c r="H11" s="30">
+        <v>1</v>
+      </c>
+      <c r="I11" s="31">
+        <v>1</v>
+      </c>
+      <c r="J11" s="31"/>
+      <c r="K11" s="31"/>
+      <c r="L11" s="31"/>
+      <c r="M11" s="31"/>
+      <c r="N11" s="31"/>
+    </row>
+    <row r="12" spans="1:14" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="25" t="str">
+        <f>GithubIssues!A12</f>
+        <v>https://github.com/i-adopt/users_stories/issues/12</v>
+      </c>
+      <c r="B12" s="25" t="str">
+        <f>GithubIssues!B12</f>
+        <v xml:space="preserve">data manager or scientist - nitrogen in biomass and fertilization - model /AnaEE02 </v>
+      </c>
+      <c r="C12" s="16" t="s">
+        <v>122</v>
+      </c>
+      <c r="D12" s="17" t="s">
+        <v>164</v>
+      </c>
+      <c r="E12" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="F12" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="G12" s="30"/>
+      <c r="H12" s="30">
+        <v>1</v>
+      </c>
+      <c r="I12" s="31">
+        <v>1</v>
+      </c>
+      <c r="J12" s="31"/>
+      <c r="K12" s="31"/>
+      <c r="L12" s="31"/>
+      <c r="M12" s="31"/>
+      <c r="N12" s="31"/>
+    </row>
+    <row r="13" spans="1:14" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="25" t="str">
+        <f>GithubIssues!A13</f>
+        <v>https://github.com/i-adopt/users_stories/issues/13</v>
+      </c>
+      <c r="B13" s="25" t="str">
+        <f>GithubIssues!B13</f>
+        <v>Scientist - Create standardized descriptions of new particle formation events - Interoperable and reusable data</v>
+      </c>
+      <c r="C13" s="16" t="s">
+        <v>122</v>
+      </c>
+      <c r="D13" s="17" t="s">
+        <v>148</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>154</v>
+      </c>
+      <c r="F13" s="7" t="s">
         <v>167</v>
       </c>
-      <c r="G2" s="31">
-        <v>1</v>
-      </c>
-      <c r="H2" s="31"/>
-      <c r="I2" s="32"/>
-      <c r="J2" s="32"/>
-      <c r="K2" s="32"/>
-      <c r="L2" s="32">
-        <v>1</v>
-      </c>
-      <c r="M2" s="32"/>
-      <c r="N2" s="32"/>
-    </row>
-    <row r="3" spans="1:14" ht="68.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="26" t="str">
-        <f>GithubIssues!A3</f>
-        <v>https://github.com/i-adopt/users_stories/issues/4</v>
-      </c>
-      <c r="B3" s="26" t="str">
-        <f>GithubIssues!B3</f>
-        <v>eLTER nitrogen cycle research</v>
-      </c>
-      <c r="C3" s="17" t="s">
-        <v>123</v>
-      </c>
-      <c r="D3" s="19" t="s">
-        <v>116</v>
-      </c>
-      <c r="E3" s="8" t="s">
-        <v>112</v>
-      </c>
-      <c r="F3" s="8" t="s">
-        <v>129</v>
-      </c>
-      <c r="G3" s="31"/>
-      <c r="H3" s="31">
-        <v>1</v>
-      </c>
-      <c r="I3" s="32">
-        <v>1</v>
-      </c>
-      <c r="J3" s="32"/>
-      <c r="K3" s="32"/>
-      <c r="L3" s="32"/>
-      <c r="M3" s="32"/>
-      <c r="N3" s="32"/>
-    </row>
-    <row r="4" spans="1:14" ht="55.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="26" t="str">
-        <f>GithubIssues!A4</f>
-        <v>https://github.com/i-adopt/users_stories/issues/5</v>
-      </c>
-      <c r="B4" s="26" t="str">
-        <f>GithubIssues!B4</f>
-        <v>Observer- Annotate observation in situ - interoperable descriptions from start</v>
-      </c>
-      <c r="C4" s="17" t="s">
-        <v>117</v>
-      </c>
-      <c r="D4" s="21" t="s">
-        <v>73</v>
-      </c>
-      <c r="E4" s="8" t="s">
-        <v>121</v>
-      </c>
-      <c r="F4" s="8" t="s">
-        <v>136</v>
-      </c>
-      <c r="G4" s="31"/>
-      <c r="H4" s="31"/>
-      <c r="I4" s="32"/>
-      <c r="J4" s="32">
-        <v>1</v>
-      </c>
-      <c r="K4" s="32"/>
-      <c r="L4" s="32"/>
-      <c r="M4" s="32"/>
-      <c r="N4" s="32">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="26" t="str">
-        <f>GithubIssues!A5</f>
-        <v>https://github.com/i-adopt/users_stories/issues/6</v>
-      </c>
-      <c r="B5" s="26" t="str">
-        <f>GithubIssues!B5</f>
-        <v>Vocabulary manager - Select the right URI for "nitrogen" - Better data integration and interoperability</v>
-      </c>
-      <c r="C5" s="17" t="s">
-        <v>109</v>
-      </c>
-      <c r="D5" s="18" t="s">
-        <v>89</v>
-      </c>
-      <c r="E5" s="8" t="s">
+      <c r="G13" s="30"/>
+      <c r="H13" s="30"/>
+      <c r="I13" s="31"/>
+      <c r="J13" s="31"/>
+      <c r="K13" s="31"/>
+      <c r="L13" s="31">
+        <v>1</v>
+      </c>
+      <c r="M13" s="31"/>
+      <c r="N13" s="31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="25" t="str">
+        <f>GithubIssues!A14</f>
+        <v>https://github.com/i-adopt/users_stories/issues/14</v>
+      </c>
+      <c r="B14" s="25" t="str">
+        <f>GithubIssues!B14</f>
+        <v>Data Manager - ObservableProperty with parameters - create identifiers for property+parameters</v>
+      </c>
+      <c r="C14" s="16" t="s">
+        <v>157</v>
+      </c>
+      <c r="D14" s="17" t="s">
+        <v>155</v>
+      </c>
+      <c r="E14" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="F14" s="7" t="s">
+        <v>152</v>
+      </c>
+      <c r="G14" s="30"/>
+      <c r="H14" s="30"/>
+      <c r="I14" s="31"/>
+      <c r="J14" s="31"/>
+      <c r="K14" s="31"/>
+      <c r="L14" s="31">
+        <v>1</v>
+      </c>
+      <c r="M14" s="31"/>
+      <c r="N14" s="31"/>
+    </row>
+    <row r="15" spans="1:14" ht="79.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="25" t="str">
+        <f>GithubIssues!A15</f>
+        <v>https://github.com/i-adopt/users_stories/issues/15</v>
+      </c>
+      <c r="B15" s="25" t="str">
+        <f>GithubIssues!B15</f>
+        <v xml:space="preserve">Terminology provider - access agreed mappings - gain efficiency in data exchange </v>
+      </c>
+      <c r="C15" s="16" t="s">
+        <v>108</v>
+      </c>
+      <c r="D15" s="20" t="s">
+        <v>171</v>
+      </c>
+      <c r="E15" s="35" t="s">
+        <v>170</v>
+      </c>
+      <c r="F15" s="7" t="s">
+        <v>172</v>
+      </c>
+      <c r="G15" s="30">
+        <v>1</v>
+      </c>
+      <c r="H15" s="36">
+        <v>1</v>
+      </c>
+      <c r="I15" s="37">
+        <v>1</v>
+      </c>
+      <c r="J15" s="37">
+        <v>1</v>
+      </c>
+      <c r="K15" s="31"/>
+      <c r="L15" s="31"/>
+      <c r="M15" s="31">
+        <v>1</v>
+      </c>
+      <c r="N15" s="31"/>
+    </row>
+    <row r="16" spans="1:14" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="25" t="str">
+        <f>GithubIssues!A16</f>
+        <v>https://github.com/i-adopt/users_stories/issues/16</v>
+      </c>
+      <c r="B16" s="25" t="str">
+        <f>GithubIssues!B16</f>
+        <v>Scientist - assess data - to generalize trait-environment-relationships in phytoplankton communities</v>
+      </c>
+      <c r="C16" s="16" t="s">
         <v>122</v>
       </c>
-      <c r="F5" s="8" t="s">
-        <v>168</v>
-      </c>
-      <c r="G5" s="31"/>
-      <c r="H5" s="31"/>
-      <c r="I5" s="32"/>
-      <c r="J5" s="32">
-        <v>1</v>
-      </c>
-      <c r="K5" s="32"/>
-      <c r="L5" s="32">
-        <v>1</v>
-      </c>
-      <c r="M5" s="32"/>
-      <c r="N5" s="32"/>
-    </row>
-    <row r="6" spans="1:14" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="26" t="str">
-        <f>GithubIssues!A6</f>
-        <v>https://github.com/i-adopt/users_stories/issues/7</v>
-      </c>
-      <c r="B6" s="26" t="str">
-        <f>GithubIssues!B6</f>
-        <v>Scientist - Integrate data - Efficient analysis</v>
-      </c>
-      <c r="C6" s="17" t="s">
-        <v>123</v>
-      </c>
-      <c r="D6" s="21" t="s">
-        <v>165</v>
-      </c>
-      <c r="E6" s="8" t="s">
-        <v>74</v>
-      </c>
-      <c r="F6" s="8" t="s">
-        <v>131</v>
-      </c>
-      <c r="G6" s="31"/>
-      <c r="H6" s="31">
-        <v>1</v>
-      </c>
-      <c r="I6" s="32">
-        <v>1</v>
-      </c>
-      <c r="J6" s="32"/>
-      <c r="K6" s="32"/>
-      <c r="L6" s="32"/>
-      <c r="M6" s="32"/>
-      <c r="N6" s="32"/>
-    </row>
-    <row r="7" spans="1:14" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="26" t="str">
-        <f>GithubIssues!A7</f>
-        <v>https://github.com/i-adopt/users_stories/issues/8</v>
-      </c>
-      <c r="B7" s="26" t="str">
-        <f>GithubIssues!B7</f>
-        <v>Scientist - find data - to calculate a Nitrogen budget for an algal population</v>
-      </c>
-      <c r="C7" s="17" t="s">
-        <v>123</v>
-      </c>
-      <c r="D7" s="20" t="s">
-        <v>133</v>
-      </c>
-      <c r="E7" s="8" t="s">
-        <v>132</v>
-      </c>
-      <c r="F7" s="8" t="s">
-        <v>131</v>
-      </c>
-      <c r="G7" s="31"/>
-      <c r="H7" s="31">
-        <v>1</v>
-      </c>
-      <c r="I7" s="32">
-        <v>1</v>
-      </c>
-      <c r="J7" s="32"/>
-      <c r="K7" s="32"/>
-      <c r="L7" s="32"/>
-      <c r="M7" s="32"/>
-      <c r="N7" s="32"/>
-    </row>
-    <row r="8" spans="1:14" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="26" t="str">
-        <f>GithubIssues!A8</f>
-        <v>https://github.com/i-adopt/users_stories/issues/9</v>
-      </c>
-      <c r="B8" s="26" t="str">
-        <f>GithubIssues!B8</f>
-        <v>Scientist - clean data - (reproduce) elemental analysis of sample</v>
-      </c>
-      <c r="C8" s="17" t="s">
-        <v>123</v>
-      </c>
-      <c r="D8" s="18" t="s">
-        <v>138</v>
-      </c>
-      <c r="E8" s="8" t="s">
-        <v>93</v>
-      </c>
-      <c r="F8" s="8" t="s">
-        <v>140</v>
-      </c>
-      <c r="G8" s="31"/>
-      <c r="H8" s="31"/>
-      <c r="I8" s="32">
-        <v>1</v>
-      </c>
-      <c r="J8" s="32"/>
-      <c r="K8" s="32">
-        <v>1</v>
-      </c>
-      <c r="L8" s="32"/>
-      <c r="M8" s="32"/>
-      <c r="N8" s="32"/>
-    </row>
-    <row r="9" spans="1:14" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="26" t="str">
-        <f>GithubIssues!A9</f>
-        <v>https://github.com/i-adopt/users_stories/issues/10</v>
-      </c>
-      <c r="B9" s="26" t="str">
-        <f>GithubIssues!B9</f>
-        <v>Bio-loggingData - NormalizeDataMeasurements - Interoperability</v>
-      </c>
-      <c r="C9" s="17" t="s">
-        <v>96</v>
-      </c>
-      <c r="D9" s="18" t="s">
-        <v>75</v>
-      </c>
-      <c r="E9" s="8" t="s">
-        <v>142</v>
-      </c>
-      <c r="F9" s="8" t="s">
-        <v>129</v>
-      </c>
-      <c r="G9" s="31"/>
-      <c r="H9" s="31">
-        <v>1</v>
-      </c>
-      <c r="I9" s="32">
-        <v>1</v>
-      </c>
-      <c r="J9" s="32"/>
-      <c r="K9" s="32"/>
-      <c r="L9" s="32"/>
-      <c r="M9" s="32"/>
-      <c r="N9" s="32"/>
-    </row>
-    <row r="10" spans="1:14" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="26" t="str">
-        <f>GithubIssues!A10</f>
-        <v>https://github.com/i-adopt/users_stories/issues/11</v>
-      </c>
-      <c r="B10" s="26" t="str">
-        <f>GithubIssues!B10</f>
-        <v>scientist - N forms in water - N&lt;-&gt;phytoplankton / AnaEE_01</v>
-      </c>
-      <c r="C10" s="17" t="s">
-        <v>123</v>
-      </c>
-      <c r="D10" s="18" t="s">
-        <v>75</v>
-      </c>
-      <c r="E10" s="8" t="s">
-        <v>144</v>
-      </c>
-      <c r="F10" s="8" t="s">
-        <v>129</v>
-      </c>
-      <c r="G10" s="31"/>
-      <c r="H10" s="31">
-        <v>1</v>
-      </c>
-      <c r="I10" s="32">
-        <v>1</v>
-      </c>
-      <c r="J10" s="32"/>
-      <c r="K10" s="32"/>
-      <c r="L10" s="32"/>
-      <c r="M10" s="32"/>
-      <c r="N10" s="32"/>
-    </row>
-    <row r="11" spans="1:14" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="26" t="str">
-        <f>GithubIssues!A11</f>
-        <v>https://github.com/i-adopt/users_stories/issues/12</v>
-      </c>
-      <c r="B11" s="26" t="str">
-        <f>GithubIssues!B11</f>
-        <v xml:space="preserve">data manager or scientist - nitrogen in biomass and fertilization - model /AnaEE02 </v>
-      </c>
-      <c r="C11" s="17" t="s">
-        <v>123</v>
-      </c>
-      <c r="D11" s="18" t="s">
-        <v>165</v>
-      </c>
-      <c r="E11" s="8" t="s">
-        <v>146</v>
-      </c>
-      <c r="F11" s="8" t="s">
-        <v>147</v>
-      </c>
-      <c r="G11" s="31"/>
-      <c r="H11" s="31">
-        <v>1</v>
-      </c>
-      <c r="I11" s="32">
-        <v>1</v>
-      </c>
-      <c r="J11" s="32"/>
-      <c r="K11" s="32"/>
-      <c r="L11" s="32"/>
-      <c r="M11" s="32"/>
-      <c r="N11" s="32"/>
-    </row>
-    <row r="12" spans="1:14" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="26" t="str">
-        <f>GithubIssues!A12</f>
-        <v>https://github.com/i-adopt/users_stories/issues/13</v>
-      </c>
-      <c r="B12" s="26" t="str">
-        <f>GithubIssues!B12</f>
-        <v>Scientist - Create standardized descriptions of new particle formation events - Interoperable and reusable data</v>
-      </c>
-      <c r="C12" s="17" t="s">
-        <v>123</v>
-      </c>
-      <c r="D12" s="18" t="s">
-        <v>149</v>
-      </c>
-      <c r="E12" s="8" t="s">
-        <v>155</v>
-      </c>
-      <c r="F12" s="8" t="s">
-        <v>169</v>
-      </c>
-      <c r="G12" s="31"/>
-      <c r="H12" s="31"/>
-      <c r="I12" s="32"/>
-      <c r="J12" s="32"/>
-      <c r="K12" s="32"/>
-      <c r="L12" s="32">
-        <v>1</v>
-      </c>
-      <c r="M12" s="32"/>
-      <c r="N12" s="32">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="26" t="str">
-        <f>GithubIssues!A13</f>
-        <v>https://github.com/i-adopt/users_stories/issues/14</v>
-      </c>
-      <c r="B13" s="26" t="str">
-        <f>GithubIssues!B13</f>
-        <v>Data Manager - ObservableProperty with parameters - create identifiers for property+parameters</v>
-      </c>
-      <c r="C13" s="17" t="s">
-        <v>158</v>
-      </c>
-      <c r="D13" s="18" t="s">
-        <v>156</v>
-      </c>
-      <c r="E13" s="8" t="s">
-        <v>102</v>
-      </c>
-      <c r="F13" s="8" t="s">
-        <v>153</v>
-      </c>
-      <c r="G13" s="31"/>
-      <c r="H13" s="31"/>
-      <c r="I13" s="32"/>
-      <c r="J13" s="32"/>
-      <c r="K13" s="32"/>
-      <c r="L13" s="32">
-        <v>1</v>
-      </c>
-      <c r="M13" s="32"/>
-      <c r="N13" s="32"/>
-    </row>
-    <row r="14" spans="1:14" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="26" t="str">
-        <f>GithubIssues!A14</f>
-        <v>https://github.com/i-adopt/users_stories/issues/15</v>
-      </c>
-      <c r="B14" s="26" t="str">
-        <f>GithubIssues!B14</f>
-        <v xml:space="preserve">Terminology provider - access agreed mappings - gain efficiency in data exchange </v>
-      </c>
-      <c r="C14" s="17" t="s">
-        <v>109</v>
-      </c>
-      <c r="D14" s="18" t="s">
-        <v>76</v>
-      </c>
-      <c r="E14" s="8" t="s">
-        <v>166</v>
-      </c>
-      <c r="F14" s="8" t="s">
+      <c r="D16" s="17" t="s">
         <v>88</v>
       </c>
-      <c r="G14" s="31"/>
-      <c r="H14" s="31"/>
-      <c r="I14" s="32"/>
-      <c r="J14" s="32"/>
-      <c r="K14" s="32"/>
-      <c r="L14" s="32"/>
-      <c r="M14" s="32">
-        <v>1</v>
-      </c>
-      <c r="N14" s="32"/>
-    </row>
-    <row r="15" spans="1:14" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="26" t="str">
-        <f>GithubIssues!A15</f>
-        <v>https://github.com/i-adopt/users_stories/issues/16</v>
-      </c>
-      <c r="B15" s="26" t="str">
-        <f>GithubIssues!B15</f>
-        <v>Scientist - assess data - to generalize trait-environment-relationships in phytoplankton communities</v>
-      </c>
-      <c r="C15" s="17" t="s">
-        <v>123</v>
-      </c>
-      <c r="D15" s="18" t="s">
-        <v>89</v>
-      </c>
-      <c r="E15" s="8" t="s">
-        <v>164</v>
-      </c>
-      <c r="F15" s="8" t="s">
-        <v>129</v>
-      </c>
-      <c r="G15" s="31"/>
-      <c r="H15" s="31">
-        <v>1</v>
-      </c>
-      <c r="I15" s="32">
-        <v>1</v>
-      </c>
-      <c r="J15" s="32"/>
-      <c r="K15" s="32"/>
-      <c r="L15" s="32"/>
-      <c r="M15" s="32"/>
-      <c r="N15" s="32"/>
+      <c r="E16" s="7" t="s">
+        <v>163</v>
+      </c>
+      <c r="F16" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="G16" s="30"/>
+      <c r="H16" s="30">
+        <v>1</v>
+      </c>
+      <c r="I16" s="31">
+        <v>1</v>
+      </c>
+      <c r="J16" s="31"/>
+      <c r="K16" s="31"/>
+      <c r="L16" s="31"/>
+      <c r="M16" s="31"/>
+      <c r="N16" s="31"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="8IxWvZLmM0ZchzaY/xcmIqj62K1Ob/cAtZudLrfZJUbNIPp58z05uQtBk6IjTn5JzDLlr0OVfDRy7dkEHFFTYw==" saltValue="tsB0czQw66adNwD+Zw9tWg==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -4503,615 +4748,615 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A1" s="25" t="str">
+      <c r="A1" s="24" t="str">
         <f>GithubIssues!A1</f>
         <v>github_url</v>
       </c>
-      <c r="B1" s="33" t="str">
+      <c r="B1" s="32" t="str">
         <f>Analysis_Coding!G1</f>
         <v>terminology management</v>
       </c>
-      <c r="C1" s="33" t="str">
+      <c r="C1" s="32" t="str">
         <f>Analysis_Coding!H1</f>
         <v>data integration and analysis</v>
       </c>
-      <c r="D1" s="33" t="str">
+      <c r="D1" s="32" t="str">
         <f>Analysis_Coding!I1</f>
         <v>semantic data search</v>
       </c>
-      <c r="E1" s="33" t="str">
+      <c r="E1" s="32" t="str">
         <f>Analysis_Coding!J1</f>
         <v>terminology search</v>
       </c>
-      <c r="F1" s="33" t="str">
+      <c r="F1" s="32" t="str">
         <f>Analysis_Coding!K1</f>
         <v>data cleaning</v>
       </c>
-      <c r="G1" s="33" t="str">
+      <c r="G1" s="32" t="str">
         <f>Analysis_Coding!L1</f>
         <v>semantic modelling</v>
       </c>
-      <c r="H1" s="33" t="str">
+      <c r="H1" s="32" t="str">
         <f>Analysis_Coding!M1</f>
         <v>terminology alignment</v>
       </c>
-      <c r="I1" s="33" t="str">
+      <c r="I1" s="32" t="str">
         <f>Analysis_Coding!N1</f>
         <v>semantic annotation</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="26" t="str">
+      <c r="A2" s="25" t="str">
         <f>GithubIssues!A2</f>
         <v>https://github.com/i-adopt/users_stories/issues/1</v>
       </c>
-      <c r="B2" s="29">
+      <c r="B2" s="28">
         <f>Analysis_Coding!G2</f>
         <v>1</v>
       </c>
-      <c r="C2" s="29">
+      <c r="C2" s="28">
         <f>Analysis_Coding!H2</f>
         <v>0</v>
       </c>
-      <c r="D2" s="29">
+      <c r="D2" s="28">
         <f>Analysis_Coding!I2</f>
         <v>0</v>
       </c>
-      <c r="E2" s="29">
+      <c r="E2" s="28">
         <f>Analysis_Coding!J2</f>
         <v>0</v>
       </c>
-      <c r="F2" s="29">
+      <c r="F2" s="28">
         <f>Analysis_Coding!K2</f>
         <v>0</v>
       </c>
-      <c r="G2" s="29">
+      <c r="G2" s="28">
         <f>Analysis_Coding!L2</f>
         <v>1</v>
       </c>
-      <c r="H2" s="29">
+      <c r="H2" s="28">
         <f>Analysis_Coding!M2</f>
         <v>0</v>
       </c>
-      <c r="I2" s="29">
+      <c r="I2" s="28">
         <f>Analysis_Coding!N2</f>
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="26" t="str">
-        <f>GithubIssues!A3</f>
+      <c r="A3" s="25" t="str">
+        <f>GithubIssues!A4</f>
         <v>https://github.com/i-adopt/users_stories/issues/4</v>
       </c>
-      <c r="B3" s="29">
-        <f>Analysis_Coding!G3</f>
-        <v>0</v>
-      </c>
-      <c r="C3" s="29">
-        <f>Analysis_Coding!H3</f>
-        <v>1</v>
-      </c>
-      <c r="D3" s="29">
-        <f>Analysis_Coding!I3</f>
-        <v>1</v>
-      </c>
-      <c r="E3" s="29">
-        <f>Analysis_Coding!J3</f>
-        <v>0</v>
-      </c>
-      <c r="F3" s="29">
-        <f>Analysis_Coding!K3</f>
-        <v>0</v>
-      </c>
-      <c r="G3" s="29">
-        <f>Analysis_Coding!L3</f>
-        <v>0</v>
-      </c>
-      <c r="H3" s="29">
-        <f>Analysis_Coding!M3</f>
-        <v>0</v>
-      </c>
-      <c r="I3" s="29">
-        <f>Analysis_Coding!N3</f>
+      <c r="B3" s="28">
+        <f>Analysis_Coding!G4</f>
+        <v>0</v>
+      </c>
+      <c r="C3" s="28">
+        <f>Analysis_Coding!H4</f>
+        <v>1</v>
+      </c>
+      <c r="D3" s="28">
+        <f>Analysis_Coding!I4</f>
+        <v>1</v>
+      </c>
+      <c r="E3" s="28">
+        <f>Analysis_Coding!J4</f>
+        <v>0</v>
+      </c>
+      <c r="F3" s="28">
+        <f>Analysis_Coding!K4</f>
+        <v>0</v>
+      </c>
+      <c r="G3" s="28">
+        <f>Analysis_Coding!L4</f>
+        <v>0</v>
+      </c>
+      <c r="H3" s="28">
+        <f>Analysis_Coding!M4</f>
+        <v>0</v>
+      </c>
+      <c r="I3" s="28">
+        <f>Analysis_Coding!N4</f>
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="26" t="str">
-        <f>GithubIssues!A4</f>
+      <c r="A4" s="25" t="str">
+        <f>GithubIssues!A5</f>
         <v>https://github.com/i-adopt/users_stories/issues/5</v>
       </c>
-      <c r="B4" s="29">
-        <f>Analysis_Coding!G4</f>
-        <v>0</v>
-      </c>
-      <c r="C4" s="29">
-        <f>Analysis_Coding!H4</f>
-        <v>0</v>
-      </c>
-      <c r="D4" s="29">
-        <f>Analysis_Coding!I4</f>
-        <v>0</v>
-      </c>
-      <c r="E4" s="29">
-        <f>Analysis_Coding!J4</f>
-        <v>1</v>
-      </c>
-      <c r="F4" s="29">
-        <f>Analysis_Coding!K4</f>
-        <v>0</v>
-      </c>
-      <c r="G4" s="29">
-        <f>Analysis_Coding!L4</f>
-        <v>0</v>
-      </c>
-      <c r="H4" s="29">
-        <f>Analysis_Coding!M4</f>
-        <v>0</v>
-      </c>
-      <c r="I4" s="29">
-        <f>Analysis_Coding!N4</f>
+      <c r="B4" s="28">
+        <f>Analysis_Coding!G5</f>
+        <v>0</v>
+      </c>
+      <c r="C4" s="28">
+        <f>Analysis_Coding!H5</f>
+        <v>0</v>
+      </c>
+      <c r="D4" s="28">
+        <f>Analysis_Coding!I5</f>
+        <v>0</v>
+      </c>
+      <c r="E4" s="28">
+        <f>Analysis_Coding!J5</f>
+        <v>1</v>
+      </c>
+      <c r="F4" s="28">
+        <f>Analysis_Coding!K5</f>
+        <v>0</v>
+      </c>
+      <c r="G4" s="28">
+        <f>Analysis_Coding!L5</f>
+        <v>0</v>
+      </c>
+      <c r="H4" s="28">
+        <f>Analysis_Coding!M5</f>
+        <v>0</v>
+      </c>
+      <c r="I4" s="28">
+        <f>Analysis_Coding!N5</f>
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="26" t="str">
-        <f>GithubIssues!A5</f>
+      <c r="A5" s="25" t="str">
+        <f>GithubIssues!A6</f>
         <v>https://github.com/i-adopt/users_stories/issues/6</v>
       </c>
-      <c r="B5" s="29">
-        <f>Analysis_Coding!G5</f>
-        <v>0</v>
-      </c>
-      <c r="C5" s="29">
-        <f>Analysis_Coding!H5</f>
-        <v>0</v>
-      </c>
-      <c r="D5" s="29">
-        <f>Analysis_Coding!I5</f>
-        <v>0</v>
-      </c>
-      <c r="E5" s="29">
-        <f>Analysis_Coding!J5</f>
-        <v>1</v>
-      </c>
-      <c r="F5" s="29">
-        <f>Analysis_Coding!K5</f>
-        <v>0</v>
-      </c>
-      <c r="G5" s="29">
-        <f>Analysis_Coding!L5</f>
-        <v>1</v>
-      </c>
-      <c r="H5" s="29">
-        <f>Analysis_Coding!M5</f>
-        <v>0</v>
-      </c>
-      <c r="I5" s="29">
-        <f>Analysis_Coding!N5</f>
+      <c r="B5" s="28">
+        <f>Analysis_Coding!G6</f>
+        <v>0</v>
+      </c>
+      <c r="C5" s="28">
+        <f>Analysis_Coding!H6</f>
+        <v>0</v>
+      </c>
+      <c r="D5" s="28">
+        <f>Analysis_Coding!I6</f>
+        <v>0</v>
+      </c>
+      <c r="E5" s="28">
+        <f>Analysis_Coding!J6</f>
+        <v>1</v>
+      </c>
+      <c r="F5" s="28">
+        <f>Analysis_Coding!K6</f>
+        <v>0</v>
+      </c>
+      <c r="G5" s="28">
+        <f>Analysis_Coding!L6</f>
+        <v>1</v>
+      </c>
+      <c r="H5" s="28">
+        <f>Analysis_Coding!M6</f>
+        <v>0</v>
+      </c>
+      <c r="I5" s="28">
+        <f>Analysis_Coding!N6</f>
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="26" t="str">
-        <f>GithubIssues!A6</f>
+      <c r="A6" s="25" t="str">
+        <f>GithubIssues!A7</f>
         <v>https://github.com/i-adopt/users_stories/issues/7</v>
       </c>
-      <c r="B6" s="29">
-        <f>Analysis_Coding!G6</f>
-        <v>0</v>
-      </c>
-      <c r="C6" s="29">
-        <f>Analysis_Coding!H6</f>
-        <v>1</v>
-      </c>
-      <c r="D6" s="29">
-        <f>Analysis_Coding!I6</f>
-        <v>1</v>
-      </c>
-      <c r="E6" s="29">
-        <f>Analysis_Coding!J6</f>
-        <v>0</v>
-      </c>
-      <c r="F6" s="29">
-        <f>Analysis_Coding!K6</f>
-        <v>0</v>
-      </c>
-      <c r="G6" s="29">
-        <f>Analysis_Coding!L6</f>
-        <v>0</v>
-      </c>
-      <c r="H6" s="29">
-        <f>Analysis_Coding!M6</f>
-        <v>0</v>
-      </c>
-      <c r="I6" s="29">
-        <f>Analysis_Coding!N6</f>
+      <c r="B6" s="28">
+        <f>Analysis_Coding!G7</f>
+        <v>0</v>
+      </c>
+      <c r="C6" s="28">
+        <f>Analysis_Coding!H7</f>
+        <v>1</v>
+      </c>
+      <c r="D6" s="28">
+        <f>Analysis_Coding!I7</f>
+        <v>1</v>
+      </c>
+      <c r="E6" s="28">
+        <f>Analysis_Coding!J7</f>
+        <v>0</v>
+      </c>
+      <c r="F6" s="28">
+        <f>Analysis_Coding!K7</f>
+        <v>0</v>
+      </c>
+      <c r="G6" s="28">
+        <f>Analysis_Coding!L7</f>
+        <v>0</v>
+      </c>
+      <c r="H6" s="28">
+        <f>Analysis_Coding!M7</f>
+        <v>0</v>
+      </c>
+      <c r="I6" s="28">
+        <f>Analysis_Coding!N7</f>
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="26" t="str">
-        <f>GithubIssues!A7</f>
+      <c r="A7" s="25" t="str">
+        <f>GithubIssues!A8</f>
         <v>https://github.com/i-adopt/users_stories/issues/8</v>
       </c>
-      <c r="B7" s="29">
-        <f>Analysis_Coding!G7</f>
-        <v>0</v>
-      </c>
-      <c r="C7" s="29">
-        <f>Analysis_Coding!H7</f>
-        <v>1</v>
-      </c>
-      <c r="D7" s="29">
-        <f>Analysis_Coding!I7</f>
-        <v>1</v>
-      </c>
-      <c r="E7" s="29">
-        <f>Analysis_Coding!J7</f>
-        <v>0</v>
-      </c>
-      <c r="F7" s="29">
-        <f>Analysis_Coding!K7</f>
-        <v>0</v>
-      </c>
-      <c r="G7" s="29">
-        <f>Analysis_Coding!L7</f>
-        <v>0</v>
-      </c>
-      <c r="H7" s="29">
-        <f>Analysis_Coding!M7</f>
-        <v>0</v>
-      </c>
-      <c r="I7" s="29">
-        <f>Analysis_Coding!N7</f>
+      <c r="B7" s="28">
+        <f>Analysis_Coding!G8</f>
+        <v>0</v>
+      </c>
+      <c r="C7" s="28">
+        <f>Analysis_Coding!H8</f>
+        <v>1</v>
+      </c>
+      <c r="D7" s="28">
+        <f>Analysis_Coding!I8</f>
+        <v>1</v>
+      </c>
+      <c r="E7" s="28">
+        <f>Analysis_Coding!J8</f>
+        <v>0</v>
+      </c>
+      <c r="F7" s="28">
+        <f>Analysis_Coding!K8</f>
+        <v>0</v>
+      </c>
+      <c r="G7" s="28">
+        <f>Analysis_Coding!L8</f>
+        <v>0</v>
+      </c>
+      <c r="H7" s="28">
+        <f>Analysis_Coding!M8</f>
+        <v>0</v>
+      </c>
+      <c r="I7" s="28">
+        <f>Analysis_Coding!N8</f>
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="26" t="str">
-        <f>GithubIssues!A8</f>
+      <c r="A8" s="25" t="str">
+        <f>GithubIssues!A9</f>
         <v>https://github.com/i-adopt/users_stories/issues/9</v>
       </c>
-      <c r="B8" s="29">
-        <f>Analysis_Coding!G8</f>
-        <v>0</v>
-      </c>
-      <c r="C8" s="29">
-        <f>Analysis_Coding!H8</f>
-        <v>0</v>
-      </c>
-      <c r="D8" s="29">
-        <f>Analysis_Coding!I8</f>
-        <v>1</v>
-      </c>
-      <c r="E8" s="29">
-        <f>Analysis_Coding!J8</f>
-        <v>0</v>
-      </c>
-      <c r="F8" s="29">
-        <f>Analysis_Coding!K8</f>
-        <v>1</v>
-      </c>
-      <c r="G8" s="29">
-        <f>Analysis_Coding!L8</f>
-        <v>0</v>
-      </c>
-      <c r="H8" s="29">
-        <f>Analysis_Coding!M8</f>
-        <v>0</v>
-      </c>
-      <c r="I8" s="29">
-        <f>Analysis_Coding!N8</f>
+      <c r="B8" s="28">
+        <f>Analysis_Coding!G9</f>
+        <v>0</v>
+      </c>
+      <c r="C8" s="28">
+        <f>Analysis_Coding!H9</f>
+        <v>0</v>
+      </c>
+      <c r="D8" s="28">
+        <f>Analysis_Coding!I9</f>
+        <v>1</v>
+      </c>
+      <c r="E8" s="28">
+        <f>Analysis_Coding!J9</f>
+        <v>0</v>
+      </c>
+      <c r="F8" s="28">
+        <f>Analysis_Coding!K9</f>
+        <v>1</v>
+      </c>
+      <c r="G8" s="28">
+        <f>Analysis_Coding!L9</f>
+        <v>0</v>
+      </c>
+      <c r="H8" s="28">
+        <f>Analysis_Coding!M9</f>
+        <v>0</v>
+      </c>
+      <c r="I8" s="28">
+        <f>Analysis_Coding!N9</f>
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="26" t="str">
-        <f>GithubIssues!A9</f>
+      <c r="A9" s="25" t="str">
+        <f>GithubIssues!A10</f>
         <v>https://github.com/i-adopt/users_stories/issues/10</v>
       </c>
-      <c r="B9" s="29">
-        <f>Analysis_Coding!G9</f>
-        <v>0</v>
-      </c>
-      <c r="C9" s="29">
-        <f>Analysis_Coding!H9</f>
-        <v>1</v>
-      </c>
-      <c r="D9" s="29">
-        <f>Analysis_Coding!I9</f>
-        <v>1</v>
-      </c>
-      <c r="E9" s="29">
-        <f>Analysis_Coding!J9</f>
-        <v>0</v>
-      </c>
-      <c r="F9" s="29">
-        <f>Analysis_Coding!K9</f>
-        <v>0</v>
-      </c>
-      <c r="G9" s="29">
-        <f>Analysis_Coding!L9</f>
-        <v>0</v>
-      </c>
-      <c r="H9" s="29">
-        <f>Analysis_Coding!M9</f>
-        <v>0</v>
-      </c>
-      <c r="I9" s="29">
-        <f>Analysis_Coding!N9</f>
+      <c r="B9" s="28">
+        <f>Analysis_Coding!G10</f>
+        <v>0</v>
+      </c>
+      <c r="C9" s="28">
+        <f>Analysis_Coding!H10</f>
+        <v>1</v>
+      </c>
+      <c r="D9" s="28">
+        <f>Analysis_Coding!I10</f>
+        <v>1</v>
+      </c>
+      <c r="E9" s="28">
+        <f>Analysis_Coding!J10</f>
+        <v>0</v>
+      </c>
+      <c r="F9" s="28">
+        <f>Analysis_Coding!K10</f>
+        <v>0</v>
+      </c>
+      <c r="G9" s="28">
+        <f>Analysis_Coding!L10</f>
+        <v>0</v>
+      </c>
+      <c r="H9" s="28">
+        <f>Analysis_Coding!M10</f>
+        <v>0</v>
+      </c>
+      <c r="I9" s="28">
+        <f>Analysis_Coding!N10</f>
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="26" t="str">
-        <f>GithubIssues!A10</f>
+      <c r="A10" s="25" t="str">
+        <f>GithubIssues!A11</f>
         <v>https://github.com/i-adopt/users_stories/issues/11</v>
       </c>
-      <c r="B10" s="29">
-        <f>Analysis_Coding!G10</f>
-        <v>0</v>
-      </c>
-      <c r="C10" s="29">
-        <f>Analysis_Coding!H10</f>
-        <v>1</v>
-      </c>
-      <c r="D10" s="29">
-        <f>Analysis_Coding!I10</f>
-        <v>1</v>
-      </c>
-      <c r="E10" s="29">
-        <f>Analysis_Coding!J10</f>
-        <v>0</v>
-      </c>
-      <c r="F10" s="29">
-        <f>Analysis_Coding!K10</f>
-        <v>0</v>
-      </c>
-      <c r="G10" s="29">
-        <f>Analysis_Coding!L10</f>
-        <v>0</v>
-      </c>
-      <c r="H10" s="29">
-        <f>Analysis_Coding!M10</f>
-        <v>0</v>
-      </c>
-      <c r="I10" s="29">
-        <f>Analysis_Coding!N10</f>
+      <c r="B10" s="28">
+        <f>Analysis_Coding!G11</f>
+        <v>0</v>
+      </c>
+      <c r="C10" s="28">
+        <f>Analysis_Coding!H11</f>
+        <v>1</v>
+      </c>
+      <c r="D10" s="28">
+        <f>Analysis_Coding!I11</f>
+        <v>1</v>
+      </c>
+      <c r="E10" s="28">
+        <f>Analysis_Coding!J11</f>
+        <v>0</v>
+      </c>
+      <c r="F10" s="28">
+        <f>Analysis_Coding!K11</f>
+        <v>0</v>
+      </c>
+      <c r="G10" s="28">
+        <f>Analysis_Coding!L11</f>
+        <v>0</v>
+      </c>
+      <c r="H10" s="28">
+        <f>Analysis_Coding!M11</f>
+        <v>0</v>
+      </c>
+      <c r="I10" s="28">
+        <f>Analysis_Coding!N11</f>
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="26" t="str">
-        <f>GithubIssues!A11</f>
+      <c r="A11" s="25" t="str">
+        <f>GithubIssues!A12</f>
         <v>https://github.com/i-adopt/users_stories/issues/12</v>
       </c>
-      <c r="B11" s="29">
-        <f>Analysis_Coding!G11</f>
-        <v>0</v>
-      </c>
-      <c r="C11" s="29">
-        <f>Analysis_Coding!H11</f>
-        <v>1</v>
-      </c>
-      <c r="D11" s="29">
-        <f>Analysis_Coding!I11</f>
-        <v>1</v>
-      </c>
-      <c r="E11" s="29">
-        <f>Analysis_Coding!J11</f>
-        <v>0</v>
-      </c>
-      <c r="F11" s="29">
-        <f>Analysis_Coding!K11</f>
-        <v>0</v>
-      </c>
-      <c r="G11" s="29">
-        <f>Analysis_Coding!L11</f>
-        <v>0</v>
-      </c>
-      <c r="H11" s="29">
-        <f>Analysis_Coding!M11</f>
-        <v>0</v>
-      </c>
-      <c r="I11" s="29">
-        <f>Analysis_Coding!N11</f>
+      <c r="B11" s="28">
+        <f>Analysis_Coding!G12</f>
+        <v>0</v>
+      </c>
+      <c r="C11" s="28">
+        <f>Analysis_Coding!H12</f>
+        <v>1</v>
+      </c>
+      <c r="D11" s="28">
+        <f>Analysis_Coding!I12</f>
+        <v>1</v>
+      </c>
+      <c r="E11" s="28">
+        <f>Analysis_Coding!J12</f>
+        <v>0</v>
+      </c>
+      <c r="F11" s="28">
+        <f>Analysis_Coding!K12</f>
+        <v>0</v>
+      </c>
+      <c r="G11" s="28">
+        <f>Analysis_Coding!L12</f>
+        <v>0</v>
+      </c>
+      <c r="H11" s="28">
+        <f>Analysis_Coding!M12</f>
+        <v>0</v>
+      </c>
+      <c r="I11" s="28">
+        <f>Analysis_Coding!N12</f>
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="26" t="str">
-        <f>GithubIssues!A12</f>
+      <c r="A12" s="25" t="str">
+        <f>GithubIssues!A13</f>
         <v>https://github.com/i-adopt/users_stories/issues/13</v>
       </c>
-      <c r="B12" s="29">
-        <f>Analysis_Coding!G12</f>
-        <v>0</v>
-      </c>
-      <c r="C12" s="29">
-        <f>Analysis_Coding!H12</f>
-        <v>0</v>
-      </c>
-      <c r="D12" s="29">
-        <f>Analysis_Coding!I12</f>
-        <v>0</v>
-      </c>
-      <c r="E12" s="29">
-        <f>Analysis_Coding!J12</f>
-        <v>0</v>
-      </c>
-      <c r="F12" s="29">
-        <f>Analysis_Coding!K12</f>
-        <v>0</v>
-      </c>
-      <c r="G12" s="29">
-        <f>Analysis_Coding!L12</f>
-        <v>1</v>
-      </c>
-      <c r="H12" s="29">
-        <f>Analysis_Coding!M12</f>
-        <v>0</v>
-      </c>
-      <c r="I12" s="29">
-        <f>Analysis_Coding!N12</f>
+      <c r="B12" s="28">
+        <f>Analysis_Coding!G13</f>
+        <v>0</v>
+      </c>
+      <c r="C12" s="28">
+        <f>Analysis_Coding!H13</f>
+        <v>0</v>
+      </c>
+      <c r="D12" s="28">
+        <f>Analysis_Coding!I13</f>
+        <v>0</v>
+      </c>
+      <c r="E12" s="28">
+        <f>Analysis_Coding!J13</f>
+        <v>0</v>
+      </c>
+      <c r="F12" s="28">
+        <f>Analysis_Coding!K13</f>
+        <v>0</v>
+      </c>
+      <c r="G12" s="28">
+        <f>Analysis_Coding!L13</f>
+        <v>1</v>
+      </c>
+      <c r="H12" s="28">
+        <f>Analysis_Coding!M13</f>
+        <v>0</v>
+      </c>
+      <c r="I12" s="28">
+        <f>Analysis_Coding!N13</f>
         <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="26" t="str">
-        <f>GithubIssues!A13</f>
+      <c r="A13" s="25" t="str">
+        <f>GithubIssues!A14</f>
         <v>https://github.com/i-adopt/users_stories/issues/14</v>
       </c>
-      <c r="B13" s="29">
-        <f>Analysis_Coding!G13</f>
-        <v>0</v>
-      </c>
-      <c r="C13" s="29">
-        <f>Analysis_Coding!H13</f>
-        <v>0</v>
-      </c>
-      <c r="D13" s="29">
-        <f>Analysis_Coding!I13</f>
-        <v>0</v>
-      </c>
-      <c r="E13" s="29">
-        <f>Analysis_Coding!J13</f>
-        <v>0</v>
-      </c>
-      <c r="F13" s="29">
-        <f>Analysis_Coding!K13</f>
-        <v>0</v>
-      </c>
-      <c r="G13" s="29">
-        <f>Analysis_Coding!L13</f>
-        <v>1</v>
-      </c>
-      <c r="H13" s="29">
-        <f>Analysis_Coding!M13</f>
-        <v>0</v>
-      </c>
-      <c r="I13" s="29">
-        <f>Analysis_Coding!N13</f>
+      <c r="B13" s="28">
+        <f>Analysis_Coding!G14</f>
+        <v>0</v>
+      </c>
+      <c r="C13" s="28">
+        <f>Analysis_Coding!H14</f>
+        <v>0</v>
+      </c>
+      <c r="D13" s="28">
+        <f>Analysis_Coding!I14</f>
+        <v>0</v>
+      </c>
+      <c r="E13" s="28">
+        <f>Analysis_Coding!J14</f>
+        <v>0</v>
+      </c>
+      <c r="F13" s="28">
+        <f>Analysis_Coding!K14</f>
+        <v>0</v>
+      </c>
+      <c r="G13" s="28">
+        <f>Analysis_Coding!L14</f>
+        <v>1</v>
+      </c>
+      <c r="H13" s="28">
+        <f>Analysis_Coding!M14</f>
+        <v>0</v>
+      </c>
+      <c r="I13" s="28">
+        <f>Analysis_Coding!N14</f>
         <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="26" t="str">
-        <f>GithubIssues!A14</f>
+      <c r="A14" s="25" t="str">
+        <f>GithubIssues!A15</f>
         <v>https://github.com/i-adopt/users_stories/issues/15</v>
       </c>
-      <c r="B14" s="29">
-        <f>Analysis_Coding!G14</f>
-        <v>0</v>
-      </c>
-      <c r="C14" s="29">
-        <f>Analysis_Coding!H14</f>
-        <v>0</v>
-      </c>
-      <c r="D14" s="29">
-        <f>Analysis_Coding!I14</f>
-        <v>0</v>
-      </c>
-      <c r="E14" s="29">
-        <f>Analysis_Coding!J14</f>
-        <v>0</v>
-      </c>
-      <c r="F14" s="29">
-        <f>Analysis_Coding!K14</f>
-        <v>0</v>
-      </c>
-      <c r="G14" s="29">
-        <f>Analysis_Coding!L14</f>
-        <v>0</v>
-      </c>
-      <c r="H14" s="29">
-        <f>Analysis_Coding!M14</f>
-        <v>1</v>
-      </c>
-      <c r="I14" s="29">
-        <f>Analysis_Coding!N14</f>
+      <c r="B14" s="28">
+        <f>Analysis_Coding!G15</f>
+        <v>1</v>
+      </c>
+      <c r="C14" s="28">
+        <f>Analysis_Coding!H15</f>
+        <v>1</v>
+      </c>
+      <c r="D14" s="28">
+        <f>Analysis_Coding!I15</f>
+        <v>1</v>
+      </c>
+      <c r="E14" s="28">
+        <f>Analysis_Coding!J15</f>
+        <v>1</v>
+      </c>
+      <c r="F14" s="28">
+        <f>Analysis_Coding!K15</f>
+        <v>0</v>
+      </c>
+      <c r="G14" s="28">
+        <f>Analysis_Coding!L15</f>
+        <v>0</v>
+      </c>
+      <c r="H14" s="28">
+        <f>Analysis_Coding!M15</f>
+        <v>1</v>
+      </c>
+      <c r="I14" s="28">
+        <f>Analysis_Coding!N15</f>
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="26" t="str">
-        <f>GithubIssues!A15</f>
+      <c r="A15" s="25" t="str">
+        <f>GithubIssues!A16</f>
         <v>https://github.com/i-adopt/users_stories/issues/16</v>
       </c>
-      <c r="B15" s="29">
-        <f>Analysis_Coding!G15</f>
-        <v>0</v>
-      </c>
-      <c r="C15" s="29">
-        <f>Analysis_Coding!H15</f>
-        <v>1</v>
-      </c>
-      <c r="D15" s="29">
-        <f>Analysis_Coding!I15</f>
-        <v>1</v>
-      </c>
-      <c r="E15" s="29">
-        <f>Analysis_Coding!J15</f>
-        <v>0</v>
-      </c>
-      <c r="F15" s="29">
-        <f>Analysis_Coding!K15</f>
-        <v>0</v>
-      </c>
-      <c r="G15" s="29">
-        <f>Analysis_Coding!L15</f>
-        <v>0</v>
-      </c>
-      <c r="H15" s="29">
-        <f>Analysis_Coding!M15</f>
-        <v>0</v>
-      </c>
-      <c r="I15" s="29">
-        <f>Analysis_Coding!N15</f>
+      <c r="B15" s="28">
+        <f>Analysis_Coding!G16</f>
+        <v>0</v>
+      </c>
+      <c r="C15" s="28">
+        <f>Analysis_Coding!H16</f>
+        <v>1</v>
+      </c>
+      <c r="D15" s="28">
+        <f>Analysis_Coding!I16</f>
+        <v>1</v>
+      </c>
+      <c r="E15" s="28">
+        <f>Analysis_Coding!J16</f>
+        <v>0</v>
+      </c>
+      <c r="F15" s="28">
+        <f>Analysis_Coding!K16</f>
+        <v>0</v>
+      </c>
+      <c r="G15" s="28">
+        <f>Analysis_Coding!L16</f>
+        <v>0</v>
+      </c>
+      <c r="H15" s="28">
+        <f>Analysis_Coding!M16</f>
+        <v>0</v>
+      </c>
+      <c r="I15" s="28">
+        <f>Analysis_Coding!N16</f>
         <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="34" t="s">
-        <v>170</v>
-      </c>
-      <c r="B16" s="35">
+      <c r="A16" s="33" t="s">
+        <v>168</v>
+      </c>
+      <c r="B16" s="34">
         <f>SUM(B2:B15)</f>
-        <v>1</v>
-      </c>
-      <c r="C16" s="35">
+        <v>2</v>
+      </c>
+      <c r="C16" s="34">
         <f t="shared" ref="C16:I16" si="0">SUM(C2:C15)</f>
-        <v>7</v>
-      </c>
-      <c r="D16" s="35">
+        <v>8</v>
+      </c>
+      <c r="D16" s="34">
         <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="E16" s="35">
+        <v>9</v>
+      </c>
+      <c r="E16" s="34">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="F16" s="34">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="G16" s="34">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="H16" s="34">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="I16" s="34">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="F16" s="35">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="G16" s="35">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="H16" s="35">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="I16" s="35">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B17">
         <v>14</v>

</xml_diff>

<commit_message>
added user story from https://github.com/i-adopt/users_stories/issues/17
</commit_message>
<xml_diff>
--- a/I-AdoptUserStoriesanalysis_25022020.xlsx
+++ b/I-AdoptUserStoriesanalysis_25022020.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12030" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12030" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Config" sheetId="2" r:id="rId1"/>
@@ -19,8 +19,8 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Analysis_Coding!$D$2:$D$16</definedName>
-    <definedName name="_xlchart.0" hidden="1">Results_UseCases!$B$16:$I$16</definedName>
-    <definedName name="_xlchart.1" hidden="1">Results_UseCases!$B$1:$I$1</definedName>
+    <definedName name="_xlchart.0" hidden="1">Results_UseCases!$B$1:$I$1</definedName>
+    <definedName name="_xlchart.1" hidden="1">Results_UseCases!$B$20:$I$20</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="192">
   <si>
     <t>https://github.com/i-adopt/users_stories/issues/1</t>
   </si>
@@ -2290,6 +2290,137 @@
   </si>
   <si>
     <t>transform the representation of observable properties (&amp;related concepts) from inspire model to O&amp;M standard to enable their explicit descriptions</t>
+  </si>
+  <si>
+    <t>https://github.com/i-adopt/users_stories/issues/17</t>
+  </si>
+  <si>
+    <t>Data manager - interchange between BODC PUV P01 and CF standard names - deliver SeaDataNet CF-NetCDF</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> louatbodc</t>
+  </si>
+  <si>
+    <t>Data manager</t>
+  </si>
+  <si>
+    <t>Marine and atmospheric</t>
+  </si>
+  <si>
+    <t>SeaDataNet transport formats - http://doi.org/10.13155/56547</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">to use both </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>BODC PUV P01 and CF</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> standard </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">name terms </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>interchangeably</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">So that our Data Assembly Centre can deliver fully CF </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>compliant formats</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> such as SeaDataNet CF-NetCDF files (which require both P01 and CF names) and easily deliver and </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>transform</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> between</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> multiple formats </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>such as EGO and Ocean Data View.</t>
+    </r>
+  </si>
+  <si>
+    <t>support translation of term names between two terminologies (BODC PUV P01 and CF) to deliver data files compliant with the models.</t>
   </si>
 </sst>
 </file>
@@ -2461,13 +2592,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -2569,6 +2697,22 @@
     <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2592,10 +2736,10 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:strDim type="cat">
-        <cx:f dir="row">_xlchart.1</cx:f>
+        <cx:f dir="row">_xlchart.0</cx:f>
       </cx:strDim>
       <cx:numDim type="size">
-        <cx:f dir="row">_xlchart.0</cx:f>
+        <cx:f dir="row">_xlchart.1</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -2647,7 +2791,7 @@
         <cx:series layoutId="sunburst" uniqueId="{24BC00EE-2991-439A-B546-DC55FFC9F96F}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.1</cx:f>
+              <cx:f>_xlchart.0</cx:f>
               <cx:v>terminology management data integration and analysis semantic data search terminology search data cleaning semantic modelling terminology alignment semantic annotation</cx:v>
             </cx:txData>
           </cx:tx>
@@ -3231,7 +3375,7 @@
     <xdr:to>
       <xdr:col>17</xdr:col>
       <xdr:colOff>485775</xdr:colOff>
-      <xdr:row>20</xdr:row>
+      <xdr:row>24</xdr:row>
       <xdr:rowOff>104774</xdr:rowOff>
     </xdr:to>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -3558,7 +3702,7 @@
   <dimension ref="A1:B20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3567,54 +3711,54 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="7" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="8" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="9" t="s">
+      <c r="A3" s="8" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="9" t="s">
+      <c r="A4" s="8" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="9" t="s">
+      <c r="A5" s="8" t="s">
         <v>157</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="9" t="s">
+      <c r="A6" s="8" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="9"/>
+      <c r="A7" s="8"/>
     </row>
     <row r="8" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="9"/>
+      <c r="A8" s="8"/>
     </row>
     <row r="9" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="12" t="s">
+      <c r="A9" s="11" t="s">
         <v>103</v>
       </c>
-      <c r="B9" s="10" t="s">
+      <c r="B9" s="9" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="12" t="s">
+      <c r="A10" s="11" t="s">
         <v>112</v>
       </c>
-      <c r="B10" s="10" t="s">
+      <c r="B10" s="9" t="s">
         <v>113</v>
       </c>
     </row>
@@ -3624,7 +3768,7 @@
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="21" t="s">
+      <c r="A12" s="20" t="s">
         <v>124</v>
       </c>
     </row>
@@ -3634,37 +3778,37 @@
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="22" t="s">
+      <c r="A14" s="21" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="22" t="s">
+      <c r="A15" s="21" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" s="22" t="s">
+      <c r="A16" s="21" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" s="22" t="s">
+      <c r="A17" s="21" t="s">
         <v>138</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" s="22" t="s">
+      <c r="A18" s="21" t="s">
         <v>152</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" s="22" t="s">
+      <c r="A19" s="21" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" s="22" t="s">
+      <c r="A20" s="21" t="s">
         <v>82</v>
       </c>
     </row>
@@ -3681,8 +3825,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H17"/>
   <sheetViews>
-    <sheetView zoomScale="64" zoomScaleNormal="64" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView zoomScale="15" zoomScaleNormal="15" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3698,424 +3842,441 @@
     <col min="12" max="12" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="13" t="s">
+    <row r="1" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="12" t="s">
         <v>65</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="C1" s="12" t="s">
         <v>67</v>
       </c>
-      <c r="D1" s="13" t="s">
+      <c r="D1" s="12" t="s">
         <v>68</v>
       </c>
-      <c r="E1" s="13" t="s">
+      <c r="E1" s="12" t="s">
         <v>69</v>
       </c>
-      <c r="F1" s="13" t="s">
+      <c r="F1" s="12" t="s">
         <v>70</v>
       </c>
-      <c r="G1" s="13" t="s">
+      <c r="G1" s="12" t="s">
         <v>71</v>
       </c>
-      <c r="H1" s="14" t="s">
+      <c r="H1" s="13" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="333.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="38" t="s">
+      <c r="A2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="37" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="E2" s="6" t="s">
+      <c r="D2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="F2" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="G2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="H2" s="3" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="333.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="B3" s="38" t="s">
+      <c r="B3" s="37" t="s">
         <v>174</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="3" t="s">
         <v>176</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="3" t="s">
         <v>175</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="E3" s="5" t="s">
         <v>181</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="F3" s="5" t="s">
         <v>177</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="G3" s="3" t="s">
         <v>178</v>
       </c>
-      <c r="H3" s="4" t="s">
+      <c r="H3" s="3" t="s">
         <v>179</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="210" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="E4" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="F4" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="G4" s="5" t="s">
+      <c r="G4" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="H4" s="4" t="s">
+      <c r="H4" s="3" t="s">
         <v>129</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="75" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D5" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="E5" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="F5" s="4" t="s">
+      <c r="F5" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="G5" s="4" t="s">
+      <c r="G5" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="H5" s="4" t="s">
+      <c r="H5" s="3" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="150" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="D6" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="E6" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="F6" s="4" t="s">
+      <c r="F6" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="G6" s="4" t="s">
+      <c r="G6" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="H6" s="4" t="s">
+      <c r="H6" s="3" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="105" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="D7" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="E7" s="4" t="s">
+      <c r="E7" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="F7" s="4" t="s">
+      <c r="F7" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="G7" s="4" t="s">
+      <c r="G7" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="H7" s="4" t="s">
+      <c r="H7" s="3" t="s">
         <v>123</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="300" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
+      <c r="A8" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C8" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="D8" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="E8" s="4" t="s">
+      <c r="E8" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="F8" s="4" t="s">
+      <c r="F8" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="G8" s="4" t="s">
+      <c r="G8" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="H8" s="4" t="s">
+      <c r="H8" s="3" t="s">
         <v>133</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="150" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
+      <c r="A9" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C9" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="D9" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="E9" s="4" t="s">
+      <c r="E9" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="F9" s="4" t="s">
+      <c r="F9" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="G9" s="4" t="s">
+      <c r="G9" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="H9" s="4" t="s">
+      <c r="H9" s="3" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="243.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
+      <c r="A10" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B10" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="C10" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="D10" s="4" t="s">
+      <c r="D10" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="E10" s="4" t="s">
+      <c r="E10" s="3" t="s">
         <v>140</v>
       </c>
-      <c r="F10" s="4" t="s">
+      <c r="F10" s="3" t="s">
         <v>142</v>
       </c>
-      <c r="G10" s="4" t="s">
+      <c r="G10" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="H10" s="4" t="s">
+      <c r="H10" s="3" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="165" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
+      <c r="A11" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="B11" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="C11" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="D11" s="4" t="s">
+      <c r="D11" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E11" s="4" t="s">
+      <c r="E11" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="F11" s="4" t="s">
+      <c r="F11" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="G11" s="4" t="s">
+      <c r="G11" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="H11" s="4"/>
+      <c r="H11" s="3"/>
     </row>
     <row r="12" spans="1:8" ht="90" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
+      <c r="A12" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="B12" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="C12" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="D12" s="4" t="s">
+      <c r="D12" s="3" t="s">
         <v>147</v>
       </c>
-      <c r="E12" s="4" t="s">
+      <c r="E12" s="3" t="s">
         <v>153</v>
       </c>
-      <c r="F12" s="4" t="s">
+      <c r="F12" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="G12" s="4" t="s">
+      <c r="G12" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="H12" s="4"/>
+      <c r="H12" s="3"/>
     </row>
     <row r="13" spans="1:8" ht="225" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
+      <c r="A13" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="B13" s="4" t="s">
+      <c r="B13" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="C13" s="4" t="s">
+      <c r="C13" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="D13" s="4" t="s">
+      <c r="D13" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="E13" s="4" t="s">
+      <c r="E13" s="3" t="s">
         <v>150</v>
       </c>
-      <c r="F13" s="4" t="s">
+      <c r="F13" s="3" t="s">
         <v>151</v>
       </c>
-      <c r="G13" s="4" t="s">
+      <c r="G13" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="H13" s="4" t="s">
+      <c r="H13" s="3" t="s">
         <v>149</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="406.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
+      <c r="A14" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="B14" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="C14" s="4" t="s">
+      <c r="C14" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="D14" s="4" t="s">
+      <c r="D14" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="E14" s="4" t="s">
+      <c r="E14" s="3" t="s">
         <v>156</v>
       </c>
-      <c r="F14" s="23" t="s">
+      <c r="F14" s="22" t="s">
         <v>159</v>
       </c>
-      <c r="G14" s="4" t="s">
+      <c r="G14" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="H14" s="4" t="s">
+      <c r="H14" s="3" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="300" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
+      <c r="A15" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="B15" s="4" t="s">
+      <c r="B15" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="C15" s="4" t="s">
+      <c r="C15" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="D15" s="4" t="s">
+      <c r="D15" s="3" t="s">
         <v>160</v>
       </c>
-      <c r="E15" s="4" t="s">
+      <c r="E15" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="F15" s="4" t="s">
+      <c r="F15" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="G15" s="4" t="s">
+      <c r="G15" s="3" t="s">
         <v>161</v>
       </c>
-      <c r="H15" s="4" t="s">
+      <c r="H15" s="3" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="90" x14ac:dyDescent="0.25">
-      <c r="A16" s="3" t="s">
+      <c r="A16" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="B16" s="4" t="s">
+      <c r="B16" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="C16" s="4" t="s">
+      <c r="C16" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="D16" s="4" t="s">
+      <c r="D16" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="E16" s="4" t="s">
+      <c r="E16" s="3" t="s">
         <v>162</v>
       </c>
-      <c r="F16" s="4" t="s">
+      <c r="F16" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="G16" s="4" t="s">
+      <c r="G16" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="H16" s="4"/>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="2"/>
-      <c r="B17" s="2"/>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
-      <c r="F17" s="2"/>
-      <c r="G17" s="2"/>
+      <c r="H16" s="3"/>
+    </row>
+    <row r="17" spans="1:8" ht="195" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="G17" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="H17" s="3" t="s">
+        <v>188</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
@@ -4134,18 +4295,19 @@
     <hyperlink ref="A16" r:id="rId13"/>
     <hyperlink ref="A4" r:id="rId14"/>
     <hyperlink ref="A3" r:id="rId15"/>
+    <hyperlink ref="A17" r:id="rId16"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId16"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId17"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N16"/>
+  <dimension ref="A1:N17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView zoomScale="30" zoomScaleNormal="30" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2:N17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4165,575 +4327,593 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="63" x14ac:dyDescent="0.25">
-      <c r="A1" s="24" t="str">
+      <c r="A1" s="23" t="str">
         <f>GithubIssues!A1</f>
         <v>github_url</v>
       </c>
-      <c r="B1" s="24" t="str">
+      <c r="B1" s="23" t="str">
         <f>GithubIssues!B1</f>
         <v>issue_title</v>
       </c>
-      <c r="C1" s="26" t="s">
+      <c r="C1" s="25" t="s">
         <v>105</v>
       </c>
-      <c r="D1" s="26" t="s">
+      <c r="D1" s="25" t="s">
         <v>114</v>
       </c>
-      <c r="E1" s="26" t="s">
+      <c r="E1" s="25" t="s">
         <v>106</v>
       </c>
-      <c r="F1" s="27" t="s">
+      <c r="F1" s="26" t="s">
         <v>107</v>
       </c>
-      <c r="G1" s="29" t="s">
+      <c r="G1" s="28" t="s">
         <v>125</v>
       </c>
-      <c r="H1" s="29" t="s">
+      <c r="H1" s="28" t="s">
         <v>134</v>
       </c>
-      <c r="I1" s="29" t="s">
+      <c r="I1" s="28" t="s">
         <v>126</v>
       </c>
-      <c r="J1" s="29" t="s">
+      <c r="J1" s="28" t="s">
         <v>127</v>
       </c>
-      <c r="K1" s="29" t="s">
+      <c r="K1" s="28" t="s">
         <v>138</v>
       </c>
-      <c r="L1" s="29" t="s">
+      <c r="L1" s="28" t="s">
         <v>152</v>
       </c>
-      <c r="M1" s="29" t="s">
+      <c r="M1" s="28" t="s">
         <v>87</v>
       </c>
-      <c r="N1" s="29" t="s">
+      <c r="N1" s="28" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="2" spans="1:14" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="25" t="str">
-        <f>GithubIssues!A2</f>
-        <v>https://github.com/i-adopt/users_stories/issues/1</v>
-      </c>
-      <c r="B2" s="25" t="str">
-        <f>GithubIssues!B2</f>
-        <v>Asset manager tracks nitrogen model changes to assess impact on related apps</v>
-      </c>
-      <c r="C2" s="16" t="s">
+      <c r="A2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="37" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="15" t="s">
         <v>108</v>
       </c>
-      <c r="D2" s="17" t="s">
+      <c r="D2" s="16" t="s">
         <v>88</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="E2" s="6" t="s">
         <v>110</v>
       </c>
-      <c r="F2" s="11" t="s">
+      <c r="F2" s="10" t="s">
         <v>165</v>
       </c>
-      <c r="G2" s="30">
-        <v>1</v>
-      </c>
-      <c r="H2" s="30"/>
-      <c r="I2" s="31"/>
-      <c r="J2" s="31"/>
-      <c r="K2" s="31"/>
-      <c r="L2" s="31">
-        <v>1</v>
-      </c>
-      <c r="M2" s="31"/>
-      <c r="N2" s="31"/>
+      <c r="G2" s="29">
+        <v>1</v>
+      </c>
+      <c r="H2" s="29"/>
+      <c r="I2" s="30"/>
+      <c r="J2" s="30"/>
+      <c r="K2" s="30"/>
+      <c r="L2" s="30">
+        <v>1</v>
+      </c>
+      <c r="M2" s="30"/>
+      <c r="N2" s="30"/>
     </row>
     <row r="3" spans="1:14" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="25" t="str">
-        <f>GithubIssues!A3</f>
-        <v>https://github.com/i-adopt/users_stories/issues/3</v>
-      </c>
-      <c r="B3" s="25" t="str">
-        <f>GithubIssues!B3</f>
-        <v>Soil Data manager - Normalize data - Achievement of a standard</v>
-      </c>
-      <c r="C3" s="39" t="s">
+      <c r="A3" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="B3" s="37" t="s">
+        <v>174</v>
+      </c>
+      <c r="C3" s="38" t="s">
         <v>95</v>
       </c>
-      <c r="D3" s="20" t="s">
+      <c r="D3" s="19" t="s">
         <v>180</v>
       </c>
-      <c r="E3" s="7" t="s">
+      <c r="E3" s="6" t="s">
         <v>182</v>
       </c>
-      <c r="F3" s="40" t="s">
+      <c r="F3" s="39" t="s">
         <v>152</v>
       </c>
-      <c r="G3" s="30"/>
-      <c r="H3" s="30"/>
-      <c r="I3" s="31"/>
-      <c r="J3" s="31"/>
-      <c r="K3" s="31"/>
-      <c r="L3" s="31">
-        <v>1</v>
-      </c>
-      <c r="M3" s="31"/>
-      <c r="N3" s="31"/>
+      <c r="G3" s="29"/>
+      <c r="H3" s="29"/>
+      <c r="I3" s="30"/>
+      <c r="J3" s="30"/>
+      <c r="K3" s="30"/>
+      <c r="L3" s="30">
+        <v>1</v>
+      </c>
+      <c r="M3" s="30"/>
+      <c r="N3" s="30"/>
     </row>
     <row r="4" spans="1:14" ht="68.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="25" t="str">
-        <f>GithubIssues!A4</f>
-        <v>https://github.com/i-adopt/users_stories/issues/4</v>
-      </c>
-      <c r="B4" s="25" t="str">
-        <f>GithubIssues!B4</f>
-        <v>eLTER nitrogen cycle research</v>
-      </c>
-      <c r="C4" s="16" t="s">
+      <c r="A4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="15" t="s">
         <v>122</v>
       </c>
-      <c r="D4" s="18" t="s">
+      <c r="D4" s="17" t="s">
         <v>115</v>
       </c>
-      <c r="E4" s="7" t="s">
+      <c r="E4" s="6" t="s">
         <v>111</v>
       </c>
-      <c r="F4" s="7" t="s">
+      <c r="F4" s="6" t="s">
         <v>128</v>
       </c>
-      <c r="G4" s="30"/>
-      <c r="H4" s="30">
-        <v>1</v>
-      </c>
-      <c r="I4" s="31">
-        <v>1</v>
-      </c>
-      <c r="J4" s="31"/>
-      <c r="K4" s="31"/>
-      <c r="L4" s="31"/>
-      <c r="M4" s="31"/>
-      <c r="N4" s="31"/>
+      <c r="G4" s="29"/>
+      <c r="H4" s="29">
+        <v>1</v>
+      </c>
+      <c r="I4" s="30">
+        <v>1</v>
+      </c>
+      <c r="J4" s="30"/>
+      <c r="K4" s="30"/>
+      <c r="L4" s="30"/>
+      <c r="M4" s="30"/>
+      <c r="N4" s="30"/>
     </row>
     <row r="5" spans="1:14" ht="55.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="25" t="str">
-        <f>GithubIssues!A5</f>
-        <v>https://github.com/i-adopt/users_stories/issues/5</v>
-      </c>
-      <c r="B5" s="25" t="str">
-        <f>GithubIssues!B5</f>
-        <v>Observer- Annotate observation in situ - interoperable descriptions from start</v>
-      </c>
-      <c r="C5" s="16" t="s">
+      <c r="A5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="15" t="s">
         <v>116</v>
       </c>
-      <c r="D5" s="20" t="s">
+      <c r="D5" s="19" t="s">
         <v>73</v>
       </c>
-      <c r="E5" s="7" t="s">
+      <c r="E5" s="6" t="s">
         <v>120</v>
       </c>
-      <c r="F5" s="7" t="s">
+      <c r="F5" s="6" t="s">
         <v>135</v>
       </c>
-      <c r="G5" s="30"/>
-      <c r="H5" s="30"/>
-      <c r="I5" s="31"/>
-      <c r="J5" s="31">
-        <v>1</v>
-      </c>
-      <c r="K5" s="31"/>
-      <c r="L5" s="31"/>
-      <c r="M5" s="31"/>
-      <c r="N5" s="31">
+      <c r="G5" s="29"/>
+      <c r="H5" s="29"/>
+      <c r="I5" s="30"/>
+      <c r="J5" s="30">
+        <v>1</v>
+      </c>
+      <c r="K5" s="30"/>
+      <c r="L5" s="30"/>
+      <c r="M5" s="30"/>
+      <c r="N5" s="30">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:14" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="25" t="str">
-        <f>GithubIssues!A6</f>
-        <v>https://github.com/i-adopt/users_stories/issues/6</v>
-      </c>
-      <c r="B6" s="25" t="str">
-        <f>GithubIssues!B6</f>
-        <v>Vocabulary manager - Select the right URI for "nitrogen" - Better data integration and interoperability</v>
-      </c>
-      <c r="C6" s="16" t="s">
+      <c r="A6" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" s="15" t="s">
         <v>108</v>
       </c>
-      <c r="D6" s="17" t="s">
+      <c r="D6" s="16" t="s">
         <v>88</v>
       </c>
-      <c r="E6" s="7" t="s">
+      <c r="E6" s="6" t="s">
         <v>121</v>
       </c>
-      <c r="F6" s="7" t="s">
+      <c r="F6" s="6" t="s">
         <v>166</v>
       </c>
-      <c r="G6" s="30"/>
-      <c r="H6" s="30"/>
-      <c r="I6" s="31"/>
-      <c r="J6" s="31">
-        <v>1</v>
-      </c>
-      <c r="K6" s="31"/>
-      <c r="L6" s="31">
-        <v>1</v>
-      </c>
-      <c r="M6" s="31"/>
-      <c r="N6" s="31"/>
+      <c r="G6" s="29"/>
+      <c r="H6" s="29"/>
+      <c r="I6" s="30"/>
+      <c r="J6" s="30">
+        <v>1</v>
+      </c>
+      <c r="K6" s="30"/>
+      <c r="L6" s="30">
+        <v>1</v>
+      </c>
+      <c r="M6" s="30"/>
+      <c r="N6" s="30"/>
     </row>
     <row r="7" spans="1:14" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="25" t="str">
-        <f>GithubIssues!A7</f>
-        <v>https://github.com/i-adopt/users_stories/issues/7</v>
-      </c>
-      <c r="B7" s="25" t="str">
-        <f>GithubIssues!B7</f>
-        <v>Scientist - Integrate data - Efficient analysis</v>
-      </c>
-      <c r="C7" s="16" t="s">
+      <c r="A7" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" s="15" t="s">
         <v>122</v>
       </c>
-      <c r="D7" s="20" t="s">
+      <c r="D7" s="19" t="s">
         <v>164</v>
       </c>
-      <c r="E7" s="7" t="s">
+      <c r="E7" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="F7" s="7" t="s">
+      <c r="F7" s="6" t="s">
         <v>130</v>
       </c>
-      <c r="G7" s="30"/>
-      <c r="H7" s="30">
-        <v>1</v>
-      </c>
-      <c r="I7" s="31">
-        <v>1</v>
-      </c>
-      <c r="J7" s="31"/>
-      <c r="K7" s="31"/>
-      <c r="L7" s="31"/>
-      <c r="M7" s="31"/>
-      <c r="N7" s="31"/>
+      <c r="G7" s="29"/>
+      <c r="H7" s="29">
+        <v>1</v>
+      </c>
+      <c r="I7" s="30">
+        <v>1</v>
+      </c>
+      <c r="J7" s="30"/>
+      <c r="K7" s="30"/>
+      <c r="L7" s="30"/>
+      <c r="M7" s="30"/>
+      <c r="N7" s="30"/>
     </row>
     <row r="8" spans="1:14" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="25" t="str">
-        <f>GithubIssues!A8</f>
-        <v>https://github.com/i-adopt/users_stories/issues/8</v>
-      </c>
-      <c r="B8" s="25" t="str">
-        <f>GithubIssues!B8</f>
-        <v>Scientist - find data - to calculate a Nitrogen budget for an algal population</v>
-      </c>
-      <c r="C8" s="16" t="s">
+      <c r="A8" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C8" s="15" t="s">
         <v>122</v>
       </c>
-      <c r="D8" s="19" t="s">
+      <c r="D8" s="18" t="s">
         <v>132</v>
       </c>
-      <c r="E8" s="7" t="s">
+      <c r="E8" s="6" t="s">
         <v>131</v>
       </c>
-      <c r="F8" s="7" t="s">
+      <c r="F8" s="6" t="s">
         <v>130</v>
       </c>
-      <c r="G8" s="30"/>
-      <c r="H8" s="30">
-        <v>1</v>
-      </c>
-      <c r="I8" s="31">
-        <v>1</v>
-      </c>
-      <c r="J8" s="31"/>
-      <c r="K8" s="31"/>
-      <c r="L8" s="31"/>
-      <c r="M8" s="31"/>
-      <c r="N8" s="31"/>
+      <c r="G8" s="29"/>
+      <c r="H8" s="29">
+        <v>1</v>
+      </c>
+      <c r="I8" s="30">
+        <v>1</v>
+      </c>
+      <c r="J8" s="30"/>
+      <c r="K8" s="30"/>
+      <c r="L8" s="30"/>
+      <c r="M8" s="30"/>
+      <c r="N8" s="30"/>
     </row>
     <row r="9" spans="1:14" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="25" t="str">
-        <f>GithubIssues!A9</f>
-        <v>https://github.com/i-adopt/users_stories/issues/9</v>
-      </c>
-      <c r="B9" s="25" t="str">
-        <f>GithubIssues!B9</f>
-        <v>Scientist - clean data - (reproduce) elemental analysis of sample</v>
-      </c>
-      <c r="C9" s="16" t="s">
+      <c r="A9" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C9" s="15" t="s">
         <v>122</v>
       </c>
-      <c r="D9" s="17" t="s">
+      <c r="D9" s="16" t="s">
         <v>137</v>
       </c>
-      <c r="E9" s="7" t="s">
+      <c r="E9" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="F9" s="7" t="s">
+      <c r="F9" s="6" t="s">
         <v>139</v>
       </c>
-      <c r="G9" s="30"/>
-      <c r="H9" s="30"/>
-      <c r="I9" s="31">
-        <v>1</v>
-      </c>
-      <c r="J9" s="31"/>
-      <c r="K9" s="31">
-        <v>1</v>
-      </c>
-      <c r="L9" s="31"/>
-      <c r="M9" s="31"/>
-      <c r="N9" s="31"/>
+      <c r="G9" s="29"/>
+      <c r="H9" s="29"/>
+      <c r="I9" s="30">
+        <v>1</v>
+      </c>
+      <c r="J9" s="30"/>
+      <c r="K9" s="30">
+        <v>1</v>
+      </c>
+      <c r="L9" s="30"/>
+      <c r="M9" s="30"/>
+      <c r="N9" s="30"/>
     </row>
     <row r="10" spans="1:14" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="25" t="str">
-        <f>GithubIssues!A10</f>
-        <v>https://github.com/i-adopt/users_stories/issues/10</v>
-      </c>
-      <c r="B10" s="25" t="str">
-        <f>GithubIssues!B10</f>
-        <v>Bio-loggingData - NormalizeDataMeasurements - Interoperability</v>
-      </c>
-      <c r="C10" s="16" t="s">
+      <c r="A10" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C10" s="15" t="s">
         <v>95</v>
       </c>
-      <c r="D10" s="17" t="s">
+      <c r="D10" s="16" t="s">
         <v>75</v>
       </c>
-      <c r="E10" s="7" t="s">
+      <c r="E10" s="6" t="s">
         <v>141</v>
       </c>
-      <c r="F10" s="7" t="s">
+      <c r="F10" s="6" t="s">
         <v>128</v>
       </c>
-      <c r="G10" s="30"/>
-      <c r="H10" s="30">
-        <v>1</v>
-      </c>
-      <c r="I10" s="31">
-        <v>1</v>
-      </c>
-      <c r="J10" s="31"/>
-      <c r="K10" s="31"/>
-      <c r="L10" s="31"/>
-      <c r="M10" s="31"/>
-      <c r="N10" s="31"/>
+      <c r="G10" s="29"/>
+      <c r="H10" s="29">
+        <v>1</v>
+      </c>
+      <c r="I10" s="30">
+        <v>1</v>
+      </c>
+      <c r="J10" s="30"/>
+      <c r="K10" s="30"/>
+      <c r="L10" s="30"/>
+      <c r="M10" s="30"/>
+      <c r="N10" s="30"/>
     </row>
     <row r="11" spans="1:14" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="25" t="str">
-        <f>GithubIssues!A11</f>
-        <v>https://github.com/i-adopt/users_stories/issues/11</v>
-      </c>
-      <c r="B11" s="25" t="str">
-        <f>GithubIssues!B11</f>
-        <v>scientist - N forms in water - N&lt;-&gt;phytoplankton / AnaEE_01</v>
-      </c>
-      <c r="C11" s="16" t="s">
+      <c r="A11" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C11" s="15" t="s">
         <v>122</v>
       </c>
-      <c r="D11" s="17" t="s">
+      <c r="D11" s="16" t="s">
         <v>75</v>
       </c>
-      <c r="E11" s="7" t="s">
+      <c r="E11" s="6" t="s">
         <v>143</v>
       </c>
-      <c r="F11" s="7" t="s">
+      <c r="F11" s="6" t="s">
         <v>128</v>
       </c>
-      <c r="G11" s="30"/>
-      <c r="H11" s="30">
-        <v>1</v>
-      </c>
-      <c r="I11" s="31">
-        <v>1</v>
-      </c>
-      <c r="J11" s="31"/>
-      <c r="K11" s="31"/>
-      <c r="L11" s="31"/>
-      <c r="M11" s="31"/>
-      <c r="N11" s="31"/>
+      <c r="G11" s="29"/>
+      <c r="H11" s="29">
+        <v>1</v>
+      </c>
+      <c r="I11" s="30">
+        <v>1</v>
+      </c>
+      <c r="J11" s="30"/>
+      <c r="K11" s="30"/>
+      <c r="L11" s="30"/>
+      <c r="M11" s="30"/>
+      <c r="N11" s="30"/>
     </row>
     <row r="12" spans="1:14" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="25" t="str">
-        <f>GithubIssues!A12</f>
-        <v>https://github.com/i-adopt/users_stories/issues/12</v>
-      </c>
-      <c r="B12" s="25" t="str">
-        <f>GithubIssues!B12</f>
-        <v xml:space="preserve">data manager or scientist - nitrogen in biomass and fertilization - model /AnaEE02 </v>
-      </c>
-      <c r="C12" s="16" t="s">
+      <c r="A12" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C12" s="15" t="s">
         <v>122</v>
       </c>
-      <c r="D12" s="17" t="s">
+      <c r="D12" s="16" t="s">
         <v>164</v>
       </c>
-      <c r="E12" s="7" t="s">
+      <c r="E12" s="6" t="s">
         <v>145</v>
       </c>
-      <c r="F12" s="7" t="s">
+      <c r="F12" s="6" t="s">
         <v>146</v>
       </c>
-      <c r="G12" s="30"/>
-      <c r="H12" s="30">
-        <v>1</v>
-      </c>
-      <c r="I12" s="31">
-        <v>1</v>
-      </c>
-      <c r="J12" s="31"/>
-      <c r="K12" s="31"/>
-      <c r="L12" s="31"/>
-      <c r="M12" s="31"/>
-      <c r="N12" s="31"/>
+      <c r="G12" s="29"/>
+      <c r="H12" s="29">
+        <v>1</v>
+      </c>
+      <c r="I12" s="30">
+        <v>1</v>
+      </c>
+      <c r="J12" s="30"/>
+      <c r="K12" s="30"/>
+      <c r="L12" s="30"/>
+      <c r="M12" s="30"/>
+      <c r="N12" s="30"/>
     </row>
     <row r="13" spans="1:14" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="25" t="str">
-        <f>GithubIssues!A13</f>
-        <v>https://github.com/i-adopt/users_stories/issues/13</v>
-      </c>
-      <c r="B13" s="25" t="str">
-        <f>GithubIssues!B13</f>
-        <v>Scientist - Create standardized descriptions of new particle formation events - Interoperable and reusable data</v>
-      </c>
-      <c r="C13" s="16" t="s">
+      <c r="A13" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C13" s="15" t="s">
         <v>122</v>
       </c>
-      <c r="D13" s="17" t="s">
+      <c r="D13" s="16" t="s">
         <v>148</v>
       </c>
-      <c r="E13" s="7" t="s">
+      <c r="E13" s="6" t="s">
         <v>154</v>
       </c>
-      <c r="F13" s="7" t="s">
+      <c r="F13" s="6" t="s">
         <v>167</v>
       </c>
-      <c r="G13" s="30"/>
-      <c r="H13" s="30"/>
-      <c r="I13" s="31"/>
-      <c r="J13" s="31"/>
-      <c r="K13" s="31"/>
-      <c r="L13" s="31">
-        <v>1</v>
-      </c>
-      <c r="M13" s="31"/>
-      <c r="N13" s="31">
+      <c r="G13" s="29"/>
+      <c r="H13" s="29"/>
+      <c r="I13" s="30"/>
+      <c r="J13" s="30"/>
+      <c r="K13" s="30"/>
+      <c r="L13" s="30">
+        <v>1</v>
+      </c>
+      <c r="M13" s="30"/>
+      <c r="N13" s="30">
         <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:14" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="25" t="str">
-        <f>GithubIssues!A14</f>
-        <v>https://github.com/i-adopt/users_stories/issues/14</v>
-      </c>
-      <c r="B14" s="25" t="str">
-        <f>GithubIssues!B14</f>
-        <v>Data Manager - ObservableProperty with parameters - create identifiers for property+parameters</v>
-      </c>
-      <c r="C14" s="16" t="s">
+      <c r="A14" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="C14" s="15" t="s">
         <v>157</v>
       </c>
-      <c r="D14" s="17" t="s">
+      <c r="D14" s="16" t="s">
         <v>155</v>
       </c>
-      <c r="E14" s="7" t="s">
+      <c r="E14" s="6" t="s">
         <v>101</v>
       </c>
-      <c r="F14" s="7" t="s">
+      <c r="F14" s="6" t="s">
         <v>152</v>
       </c>
-      <c r="G14" s="30"/>
-      <c r="H14" s="30"/>
-      <c r="I14" s="31"/>
-      <c r="J14" s="31"/>
-      <c r="K14" s="31"/>
-      <c r="L14" s="31">
-        <v>1</v>
-      </c>
-      <c r="M14" s="31"/>
-      <c r="N14" s="31"/>
+      <c r="G14" s="29"/>
+      <c r="H14" s="29"/>
+      <c r="I14" s="30"/>
+      <c r="J14" s="30"/>
+      <c r="K14" s="30"/>
+      <c r="L14" s="30">
+        <v>1</v>
+      </c>
+      <c r="M14" s="30"/>
+      <c r="N14" s="30"/>
     </row>
     <row r="15" spans="1:14" ht="79.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="25" t="str">
-        <f>GithubIssues!A15</f>
-        <v>https://github.com/i-adopt/users_stories/issues/15</v>
-      </c>
-      <c r="B15" s="25" t="str">
-        <f>GithubIssues!B15</f>
-        <v xml:space="preserve">Terminology provider - access agreed mappings - gain efficiency in data exchange </v>
-      </c>
-      <c r="C15" s="16" t="s">
+      <c r="A15" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C15" s="15" t="s">
         <v>108</v>
       </c>
-      <c r="D15" s="20" t="s">
+      <c r="D15" s="19" t="s">
         <v>171</v>
       </c>
-      <c r="E15" s="35" t="s">
+      <c r="E15" s="34" t="s">
         <v>170</v>
       </c>
-      <c r="F15" s="7" t="s">
+      <c r="F15" s="6" t="s">
         <v>172</v>
       </c>
-      <c r="G15" s="30">
-        <v>1</v>
-      </c>
-      <c r="H15" s="36">
-        <v>1</v>
-      </c>
-      <c r="I15" s="37">
-        <v>1</v>
-      </c>
-      <c r="J15" s="37">
-        <v>1</v>
-      </c>
-      <c r="K15" s="31"/>
-      <c r="L15" s="31"/>
-      <c r="M15" s="31">
-        <v>1</v>
-      </c>
-      <c r="N15" s="31"/>
+      <c r="G15" s="29">
+        <v>1</v>
+      </c>
+      <c r="H15" s="35">
+        <v>1</v>
+      </c>
+      <c r="I15" s="36">
+        <v>1</v>
+      </c>
+      <c r="J15" s="36">
+        <v>1</v>
+      </c>
+      <c r="K15" s="30"/>
+      <c r="L15" s="30"/>
+      <c r="M15" s="30">
+        <v>1</v>
+      </c>
+      <c r="N15" s="30"/>
     </row>
     <row r="16" spans="1:14" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="25" t="str">
-        <f>GithubIssues!A16</f>
-        <v>https://github.com/i-adopt/users_stories/issues/16</v>
-      </c>
-      <c r="B16" s="25" t="str">
-        <f>GithubIssues!B16</f>
-        <v>Scientist - assess data - to generalize trait-environment-relationships in phytoplankton communities</v>
-      </c>
-      <c r="C16" s="16" t="s">
+      <c r="A16" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C16" s="15" t="s">
         <v>122</v>
       </c>
-      <c r="D16" s="17" t="s">
+      <c r="D16" s="16" t="s">
         <v>88</v>
       </c>
-      <c r="E16" s="7" t="s">
+      <c r="E16" s="6" t="s">
         <v>163</v>
       </c>
-      <c r="F16" s="7" t="s">
+      <c r="F16" s="6" t="s">
         <v>128</v>
       </c>
-      <c r="G16" s="30"/>
-      <c r="H16" s="30">
-        <v>1</v>
-      </c>
-      <c r="I16" s="31">
-        <v>1</v>
-      </c>
-      <c r="J16" s="31"/>
-      <c r="K16" s="31"/>
-      <c r="L16" s="31"/>
-      <c r="M16" s="31"/>
-      <c r="N16" s="31"/>
+      <c r="G16" s="29"/>
+      <c r="H16" s="29">
+        <v>1</v>
+      </c>
+      <c r="I16" s="30">
+        <v>1</v>
+      </c>
+      <c r="J16" s="30"/>
+      <c r="K16" s="30"/>
+      <c r="L16" s="30"/>
+      <c r="M16" s="30"/>
+      <c r="N16" s="30"/>
+    </row>
+    <row r="17" spans="1:14" ht="60" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="C17" s="41" t="s">
+        <v>157</v>
+      </c>
+      <c r="D17" s="38" t="s">
+        <v>132</v>
+      </c>
+      <c r="E17" s="40" t="s">
+        <v>191</v>
+      </c>
+      <c r="F17" s="42" t="s">
+        <v>87</v>
+      </c>
+      <c r="G17" s="24"/>
+      <c r="H17" s="24"/>
+      <c r="I17" s="27"/>
+      <c r="J17" s="27"/>
+      <c r="K17" s="27"/>
+      <c r="L17" s="27"/>
+      <c r="M17" s="43">
+        <v>1</v>
+      </c>
+      <c r="N17" s="27"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1"/>
+    <hyperlink ref="A5" r:id="rId2"/>
+    <hyperlink ref="A6" r:id="rId3"/>
+    <hyperlink ref="A7" r:id="rId4"/>
+    <hyperlink ref="A8" r:id="rId5"/>
+    <hyperlink ref="A9" r:id="rId6"/>
+    <hyperlink ref="A10" r:id="rId7"/>
+    <hyperlink ref="A11" r:id="rId8"/>
+    <hyperlink ref="A12" r:id="rId9"/>
+    <hyperlink ref="A13" r:id="rId10"/>
+    <hyperlink ref="A14" r:id="rId11"/>
+    <hyperlink ref="A15" r:id="rId12"/>
+    <hyperlink ref="A16" r:id="rId13"/>
+    <hyperlink ref="A4" r:id="rId14"/>
+    <hyperlink ref="A3" r:id="rId15"/>
+    <hyperlink ref="A17" r:id="rId16"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId17"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I17"/>
+  <dimension ref="A1:I21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I28" sqref="I28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20:I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4748,618 +4928,716 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A1" s="24" t="str">
+      <c r="A1" s="23" t="str">
         <f>GithubIssues!A1</f>
         <v>github_url</v>
       </c>
-      <c r="B1" s="32" t="str">
+      <c r="B1" s="31" t="str">
         <f>Analysis_Coding!G1</f>
         <v>terminology management</v>
       </c>
-      <c r="C1" s="32" t="str">
+      <c r="C1" s="31" t="str">
         <f>Analysis_Coding!H1</f>
         <v>data integration and analysis</v>
       </c>
-      <c r="D1" s="32" t="str">
+      <c r="D1" s="31" t="str">
         <f>Analysis_Coding!I1</f>
         <v>semantic data search</v>
       </c>
-      <c r="E1" s="32" t="str">
+      <c r="E1" s="31" t="str">
         <f>Analysis_Coding!J1</f>
         <v>terminology search</v>
       </c>
-      <c r="F1" s="32" t="str">
+      <c r="F1" s="31" t="str">
         <f>Analysis_Coding!K1</f>
         <v>data cleaning</v>
       </c>
-      <c r="G1" s="32" t="str">
+      <c r="G1" s="31" t="str">
         <f>Analysis_Coding!L1</f>
         <v>semantic modelling</v>
       </c>
-      <c r="H1" s="32" t="str">
+      <c r="H1" s="31" t="str">
         <f>Analysis_Coding!M1</f>
         <v>terminology alignment</v>
       </c>
-      <c r="I1" s="32" t="str">
+      <c r="I1" s="31" t="str">
         <f>Analysis_Coding!N1</f>
         <v>semantic annotation</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="25" t="str">
+      <c r="A2" s="24" t="str">
         <f>GithubIssues!A2</f>
         <v>https://github.com/i-adopt/users_stories/issues/1</v>
       </c>
-      <c r="B2" s="28">
+      <c r="B2" s="27">
         <f>Analysis_Coding!G2</f>
         <v>1</v>
       </c>
-      <c r="C2" s="28">
+      <c r="C2" s="27">
         <f>Analysis_Coding!H2</f>
         <v>0</v>
       </c>
-      <c r="D2" s="28">
+      <c r="D2" s="27">
         <f>Analysis_Coding!I2</f>
         <v>0</v>
       </c>
-      <c r="E2" s="28">
+      <c r="E2" s="27">
         <f>Analysis_Coding!J2</f>
         <v>0</v>
       </c>
-      <c r="F2" s="28">
+      <c r="F2" s="27">
         <f>Analysis_Coding!K2</f>
         <v>0</v>
       </c>
-      <c r="G2" s="28">
+      <c r="G2" s="27">
         <f>Analysis_Coding!L2</f>
         <v>1</v>
       </c>
-      <c r="H2" s="28">
+      <c r="H2" s="27">
         <f>Analysis_Coding!M2</f>
         <v>0</v>
       </c>
-      <c r="I2" s="28">
+      <c r="I2" s="27">
         <f>Analysis_Coding!N2</f>
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="25" t="str">
+      <c r="A3" s="24" t="str">
+        <f>GithubIssues!A3</f>
+        <v>https://github.com/i-adopt/users_stories/issues/3</v>
+      </c>
+      <c r="B3" s="27">
+        <f>Analysis_Coding!G3</f>
+        <v>0</v>
+      </c>
+      <c r="C3" s="27">
+        <f>Analysis_Coding!H3</f>
+        <v>0</v>
+      </c>
+      <c r="D3" s="27">
+        <f>Analysis_Coding!I3</f>
+        <v>0</v>
+      </c>
+      <c r="E3" s="27">
+        <f>Analysis_Coding!J3</f>
+        <v>0</v>
+      </c>
+      <c r="F3" s="27">
+        <f>Analysis_Coding!K3</f>
+        <v>0</v>
+      </c>
+      <c r="G3" s="27">
+        <f>Analysis_Coding!L3</f>
+        <v>1</v>
+      </c>
+      <c r="H3" s="27">
+        <f>Analysis_Coding!M3</f>
+        <v>0</v>
+      </c>
+      <c r="I3" s="27">
+        <f>Analysis_Coding!N3</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="24" t="str">
         <f>GithubIssues!A4</f>
         <v>https://github.com/i-adopt/users_stories/issues/4</v>
       </c>
-      <c r="B3" s="28">
+      <c r="B4" s="27">
         <f>Analysis_Coding!G4</f>
         <v>0</v>
       </c>
-      <c r="C3" s="28">
+      <c r="C4" s="27">
         <f>Analysis_Coding!H4</f>
         <v>1</v>
       </c>
-      <c r="D3" s="28">
+      <c r="D4" s="27">
         <f>Analysis_Coding!I4</f>
         <v>1</v>
       </c>
-      <c r="E3" s="28">
+      <c r="E4" s="27">
         <f>Analysis_Coding!J4</f>
         <v>0</v>
       </c>
-      <c r="F3" s="28">
+      <c r="F4" s="27">
         <f>Analysis_Coding!K4</f>
         <v>0</v>
       </c>
-      <c r="G3" s="28">
+      <c r="G4" s="27">
         <f>Analysis_Coding!L4</f>
         <v>0</v>
       </c>
-      <c r="H3" s="28">
+      <c r="H4" s="27">
         <f>Analysis_Coding!M4</f>
         <v>0</v>
       </c>
-      <c r="I3" s="28">
+      <c r="I4" s="27">
         <f>Analysis_Coding!N4</f>
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="25" t="str">
+    <row r="5" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="24" t="str">
         <f>GithubIssues!A5</f>
         <v>https://github.com/i-adopt/users_stories/issues/5</v>
       </c>
-      <c r="B4" s="28">
+      <c r="B5" s="27">
         <f>Analysis_Coding!G5</f>
         <v>0</v>
       </c>
-      <c r="C4" s="28">
+      <c r="C5" s="27">
         <f>Analysis_Coding!H5</f>
         <v>0</v>
       </c>
-      <c r="D4" s="28">
+      <c r="D5" s="27">
         <f>Analysis_Coding!I5</f>
         <v>0</v>
       </c>
-      <c r="E4" s="28">
+      <c r="E5" s="27">
         <f>Analysis_Coding!J5</f>
         <v>1</v>
       </c>
-      <c r="F4" s="28">
+      <c r="F5" s="27">
         <f>Analysis_Coding!K5</f>
         <v>0</v>
       </c>
-      <c r="G4" s="28">
+      <c r="G5" s="27">
         <f>Analysis_Coding!L5</f>
         <v>0</v>
       </c>
-      <c r="H4" s="28">
+      <c r="H5" s="27">
         <f>Analysis_Coding!M5</f>
         <v>0</v>
       </c>
-      <c r="I4" s="28">
+      <c r="I5" s="27">
         <f>Analysis_Coding!N5</f>
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="25" t="str">
+    <row r="6" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="24" t="str">
         <f>GithubIssues!A6</f>
         <v>https://github.com/i-adopt/users_stories/issues/6</v>
       </c>
-      <c r="B5" s="28">
+      <c r="B6" s="27">
         <f>Analysis_Coding!G6</f>
         <v>0</v>
       </c>
-      <c r="C5" s="28">
+      <c r="C6" s="27">
         <f>Analysis_Coding!H6</f>
         <v>0</v>
       </c>
-      <c r="D5" s="28">
+      <c r="D6" s="27">
         <f>Analysis_Coding!I6</f>
         <v>0</v>
       </c>
-      <c r="E5" s="28">
+      <c r="E6" s="27">
         <f>Analysis_Coding!J6</f>
         <v>1</v>
       </c>
-      <c r="F5" s="28">
+      <c r="F6" s="27">
         <f>Analysis_Coding!K6</f>
         <v>0</v>
       </c>
-      <c r="G5" s="28">
+      <c r="G6" s="27">
         <f>Analysis_Coding!L6</f>
         <v>1</v>
       </c>
-      <c r="H5" s="28">
+      <c r="H6" s="27">
         <f>Analysis_Coding!M6</f>
         <v>0</v>
       </c>
-      <c r="I5" s="28">
+      <c r="I6" s="27">
         <f>Analysis_Coding!N6</f>
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="25" t="str">
+    <row r="7" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="24" t="str">
         <f>GithubIssues!A7</f>
         <v>https://github.com/i-adopt/users_stories/issues/7</v>
       </c>
-      <c r="B6" s="28">
+      <c r="B7" s="27">
         <f>Analysis_Coding!G7</f>
         <v>0</v>
       </c>
-      <c r="C6" s="28">
+      <c r="C7" s="27">
         <f>Analysis_Coding!H7</f>
         <v>1</v>
       </c>
-      <c r="D6" s="28">
+      <c r="D7" s="27">
         <f>Analysis_Coding!I7</f>
         <v>1</v>
       </c>
-      <c r="E6" s="28">
+      <c r="E7" s="27">
         <f>Analysis_Coding!J7</f>
         <v>0</v>
       </c>
-      <c r="F6" s="28">
+      <c r="F7" s="27">
         <f>Analysis_Coding!K7</f>
         <v>0</v>
       </c>
-      <c r="G6" s="28">
+      <c r="G7" s="27">
         <f>Analysis_Coding!L7</f>
         <v>0</v>
       </c>
-      <c r="H6" s="28">
+      <c r="H7" s="27">
         <f>Analysis_Coding!M7</f>
         <v>0</v>
       </c>
-      <c r="I6" s="28">
+      <c r="I7" s="27">
         <f>Analysis_Coding!N7</f>
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="25" t="str">
+    <row r="8" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="24" t="str">
         <f>GithubIssues!A8</f>
         <v>https://github.com/i-adopt/users_stories/issues/8</v>
       </c>
-      <c r="B7" s="28">
+      <c r="B8" s="27">
         <f>Analysis_Coding!G8</f>
         <v>0</v>
       </c>
-      <c r="C7" s="28">
+      <c r="C8" s="27">
         <f>Analysis_Coding!H8</f>
         <v>1</v>
       </c>
-      <c r="D7" s="28">
+      <c r="D8" s="27">
         <f>Analysis_Coding!I8</f>
         <v>1</v>
       </c>
-      <c r="E7" s="28">
+      <c r="E8" s="27">
         <f>Analysis_Coding!J8</f>
         <v>0</v>
       </c>
-      <c r="F7" s="28">
+      <c r="F8" s="27">
         <f>Analysis_Coding!K8</f>
         <v>0</v>
       </c>
-      <c r="G7" s="28">
+      <c r="G8" s="27">
         <f>Analysis_Coding!L8</f>
         <v>0</v>
       </c>
-      <c r="H7" s="28">
+      <c r="H8" s="27">
         <f>Analysis_Coding!M8</f>
         <v>0</v>
       </c>
-      <c r="I7" s="28">
+      <c r="I8" s="27">
         <f>Analysis_Coding!N8</f>
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="25" t="str">
+    <row r="9" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="24" t="str">
         <f>GithubIssues!A9</f>
         <v>https://github.com/i-adopt/users_stories/issues/9</v>
       </c>
-      <c r="B8" s="28">
+      <c r="B9" s="27">
         <f>Analysis_Coding!G9</f>
         <v>0</v>
       </c>
-      <c r="C8" s="28">
+      <c r="C9" s="27">
         <f>Analysis_Coding!H9</f>
         <v>0</v>
       </c>
-      <c r="D8" s="28">
+      <c r="D9" s="27">
         <f>Analysis_Coding!I9</f>
         <v>1</v>
       </c>
-      <c r="E8" s="28">
+      <c r="E9" s="27">
         <f>Analysis_Coding!J9</f>
         <v>0</v>
       </c>
-      <c r="F8" s="28">
+      <c r="F9" s="27">
         <f>Analysis_Coding!K9</f>
         <v>1</v>
       </c>
-      <c r="G8" s="28">
+      <c r="G9" s="27">
         <f>Analysis_Coding!L9</f>
         <v>0</v>
       </c>
-      <c r="H8" s="28">
+      <c r="H9" s="27">
         <f>Analysis_Coding!M9</f>
         <v>0</v>
       </c>
-      <c r="I8" s="28">
+      <c r="I9" s="27">
         <f>Analysis_Coding!N9</f>
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="25" t="str">
+    <row r="10" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="24" t="str">
         <f>GithubIssues!A10</f>
         <v>https://github.com/i-adopt/users_stories/issues/10</v>
       </c>
-      <c r="B9" s="28">
+      <c r="B10" s="27">
         <f>Analysis_Coding!G10</f>
         <v>0</v>
       </c>
-      <c r="C9" s="28">
+      <c r="C10" s="27">
         <f>Analysis_Coding!H10</f>
         <v>1</v>
       </c>
-      <c r="D9" s="28">
+      <c r="D10" s="27">
         <f>Analysis_Coding!I10</f>
         <v>1</v>
       </c>
-      <c r="E9" s="28">
+      <c r="E10" s="27">
         <f>Analysis_Coding!J10</f>
         <v>0</v>
       </c>
-      <c r="F9" s="28">
+      <c r="F10" s="27">
         <f>Analysis_Coding!K10</f>
         <v>0</v>
       </c>
-      <c r="G9" s="28">
+      <c r="G10" s="27">
         <f>Analysis_Coding!L10</f>
         <v>0</v>
       </c>
-      <c r="H9" s="28">
+      <c r="H10" s="27">
         <f>Analysis_Coding!M10</f>
         <v>0</v>
       </c>
-      <c r="I9" s="28">
+      <c r="I10" s="27">
         <f>Analysis_Coding!N10</f>
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="25" t="str">
+    <row r="11" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="24" t="str">
         <f>GithubIssues!A11</f>
         <v>https://github.com/i-adopt/users_stories/issues/11</v>
       </c>
-      <c r="B10" s="28">
+      <c r="B11" s="27">
         <f>Analysis_Coding!G11</f>
         <v>0</v>
       </c>
-      <c r="C10" s="28">
+      <c r="C11" s="27">
         <f>Analysis_Coding!H11</f>
         <v>1</v>
       </c>
-      <c r="D10" s="28">
+      <c r="D11" s="27">
         <f>Analysis_Coding!I11</f>
         <v>1</v>
       </c>
-      <c r="E10" s="28">
+      <c r="E11" s="27">
         <f>Analysis_Coding!J11</f>
         <v>0</v>
       </c>
-      <c r="F10" s="28">
+      <c r="F11" s="27">
         <f>Analysis_Coding!K11</f>
         <v>0</v>
       </c>
-      <c r="G10" s="28">
+      <c r="G11" s="27">
         <f>Analysis_Coding!L11</f>
         <v>0</v>
       </c>
-      <c r="H10" s="28">
+      <c r="H11" s="27">
         <f>Analysis_Coding!M11</f>
         <v>0</v>
       </c>
-      <c r="I10" s="28">
+      <c r="I11" s="27">
         <f>Analysis_Coding!N11</f>
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="25" t="str">
+    <row r="12" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="24" t="str">
         <f>GithubIssues!A12</f>
         <v>https://github.com/i-adopt/users_stories/issues/12</v>
       </c>
-      <c r="B11" s="28">
+      <c r="B12" s="27">
         <f>Analysis_Coding!G12</f>
         <v>0</v>
       </c>
-      <c r="C11" s="28">
+      <c r="C12" s="27">
         <f>Analysis_Coding!H12</f>
         <v>1</v>
       </c>
-      <c r="D11" s="28">
+      <c r="D12" s="27">
         <f>Analysis_Coding!I12</f>
         <v>1</v>
       </c>
-      <c r="E11" s="28">
+      <c r="E12" s="27">
         <f>Analysis_Coding!J12</f>
         <v>0</v>
       </c>
-      <c r="F11" s="28">
+      <c r="F12" s="27">
         <f>Analysis_Coding!K12</f>
         <v>0</v>
       </c>
-      <c r="G11" s="28">
+      <c r="G12" s="27">
         <f>Analysis_Coding!L12</f>
         <v>0</v>
       </c>
-      <c r="H11" s="28">
+      <c r="H12" s="27">
         <f>Analysis_Coding!M12</f>
         <v>0</v>
       </c>
-      <c r="I11" s="28">
+      <c r="I12" s="27">
         <f>Analysis_Coding!N12</f>
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="25" t="str">
+    <row r="13" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="24" t="str">
         <f>GithubIssues!A13</f>
         <v>https://github.com/i-adopt/users_stories/issues/13</v>
       </c>
-      <c r="B12" s="28">
+      <c r="B13" s="27">
         <f>Analysis_Coding!G13</f>
         <v>0</v>
       </c>
-      <c r="C12" s="28">
+      <c r="C13" s="27">
         <f>Analysis_Coding!H13</f>
         <v>0</v>
       </c>
-      <c r="D12" s="28">
+      <c r="D13" s="27">
         <f>Analysis_Coding!I13</f>
         <v>0</v>
       </c>
-      <c r="E12" s="28">
+      <c r="E13" s="27">
         <f>Analysis_Coding!J13</f>
         <v>0</v>
       </c>
-      <c r="F12" s="28">
+      <c r="F13" s="27">
         <f>Analysis_Coding!K13</f>
         <v>0</v>
       </c>
-      <c r="G12" s="28">
+      <c r="G13" s="27">
         <f>Analysis_Coding!L13</f>
         <v>1</v>
       </c>
-      <c r="H12" s="28">
+      <c r="H13" s="27">
         <f>Analysis_Coding!M13</f>
         <v>0</v>
       </c>
-      <c r="I12" s="28">
+      <c r="I13" s="27">
         <f>Analysis_Coding!N13</f>
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="25" t="str">
+    <row r="14" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="24" t="str">
         <f>GithubIssues!A14</f>
         <v>https://github.com/i-adopt/users_stories/issues/14</v>
       </c>
-      <c r="B13" s="28">
+      <c r="B14" s="27">
         <f>Analysis_Coding!G14</f>
         <v>0</v>
       </c>
-      <c r="C13" s="28">
+      <c r="C14" s="27">
         <f>Analysis_Coding!H14</f>
         <v>0</v>
       </c>
-      <c r="D13" s="28">
+      <c r="D14" s="27">
         <f>Analysis_Coding!I14</f>
         <v>0</v>
       </c>
-      <c r="E13" s="28">
+      <c r="E14" s="27">
         <f>Analysis_Coding!J14</f>
         <v>0</v>
       </c>
-      <c r="F13" s="28">
+      <c r="F14" s="27">
         <f>Analysis_Coding!K14</f>
         <v>0</v>
       </c>
-      <c r="G13" s="28">
+      <c r="G14" s="27">
         <f>Analysis_Coding!L14</f>
         <v>1</v>
       </c>
-      <c r="H13" s="28">
+      <c r="H14" s="27">
         <f>Analysis_Coding!M14</f>
         <v>0</v>
       </c>
-      <c r="I13" s="28">
+      <c r="I14" s="27">
         <f>Analysis_Coding!N14</f>
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="25" t="str">
+    <row r="15" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="24" t="str">
         <f>GithubIssues!A15</f>
         <v>https://github.com/i-adopt/users_stories/issues/15</v>
       </c>
-      <c r="B14" s="28">
+      <c r="B15" s="27">
         <f>Analysis_Coding!G15</f>
         <v>1</v>
       </c>
-      <c r="C14" s="28">
+      <c r="C15" s="27">
         <f>Analysis_Coding!H15</f>
         <v>1</v>
       </c>
-      <c r="D14" s="28">
+      <c r="D15" s="27">
         <f>Analysis_Coding!I15</f>
         <v>1</v>
       </c>
-      <c r="E14" s="28">
+      <c r="E15" s="27">
         <f>Analysis_Coding!J15</f>
         <v>1</v>
       </c>
-      <c r="F14" s="28">
+      <c r="F15" s="27">
         <f>Analysis_Coding!K15</f>
         <v>0</v>
       </c>
-      <c r="G14" s="28">
+      <c r="G15" s="27">
         <f>Analysis_Coding!L15</f>
         <v>0</v>
       </c>
-      <c r="H14" s="28">
+      <c r="H15" s="27">
         <f>Analysis_Coding!M15</f>
         <v>1</v>
       </c>
-      <c r="I14" s="28">
+      <c r="I15" s="27">
         <f>Analysis_Coding!N15</f>
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="25" t="str">
+    <row r="16" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="24" t="str">
         <f>GithubIssues!A16</f>
         <v>https://github.com/i-adopt/users_stories/issues/16</v>
       </c>
-      <c r="B15" s="28">
+      <c r="B16" s="27">
         <f>Analysis_Coding!G16</f>
         <v>0</v>
       </c>
-      <c r="C15" s="28">
+      <c r="C16" s="27">
         <f>Analysis_Coding!H16</f>
         <v>1</v>
       </c>
-      <c r="D15" s="28">
+      <c r="D16" s="27">
         <f>Analysis_Coding!I16</f>
         <v>1</v>
       </c>
-      <c r="E15" s="28">
+      <c r="E16" s="27">
         <f>Analysis_Coding!J16</f>
         <v>0</v>
       </c>
-      <c r="F15" s="28">
+      <c r="F16" s="27">
         <f>Analysis_Coding!K16</f>
         <v>0</v>
       </c>
-      <c r="G15" s="28">
+      <c r="G16" s="27">
         <f>Analysis_Coding!L16</f>
         <v>0</v>
       </c>
-      <c r="H15" s="28">
+      <c r="H16" s="27">
         <f>Analysis_Coding!M16</f>
         <v>0</v>
       </c>
-      <c r="I15" s="28">
+      <c r="I16" s="27">
         <f>Analysis_Coding!N16</f>
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="33" t="s">
+    <row r="17" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="24" t="str">
+        <f>GithubIssues!A17</f>
+        <v>https://github.com/i-adopt/users_stories/issues/17</v>
+      </c>
+      <c r="B17" s="27">
+        <f>Analysis_Coding!G17</f>
+        <v>0</v>
+      </c>
+      <c r="C17" s="27">
+        <f>Analysis_Coding!H17</f>
+        <v>0</v>
+      </c>
+      <c r="D17" s="27">
+        <f>Analysis_Coding!I17</f>
+        <v>0</v>
+      </c>
+      <c r="E17" s="27">
+        <f>Analysis_Coding!J17</f>
+        <v>0</v>
+      </c>
+      <c r="F17" s="27">
+        <f>Analysis_Coding!K17</f>
+        <v>0</v>
+      </c>
+      <c r="G17" s="27">
+        <f>Analysis_Coding!L17</f>
+        <v>0</v>
+      </c>
+      <c r="H17" s="27">
+        <f>Analysis_Coding!M17</f>
+        <v>1</v>
+      </c>
+      <c r="I17" s="27">
+        <f>Analysis_Coding!N17</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="44"/>
+      <c r="B18" s="45"/>
+      <c r="C18" s="45"/>
+      <c r="D18" s="45"/>
+      <c r="E18" s="45"/>
+      <c r="F18" s="45"/>
+      <c r="G18" s="45"/>
+      <c r="H18" s="45"/>
+      <c r="I18" s="45"/>
+    </row>
+    <row r="19" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="44"/>
+      <c r="B19" s="45"/>
+      <c r="C19" s="45"/>
+      <c r="D19" s="45"/>
+      <c r="E19" s="45"/>
+      <c r="F19" s="45"/>
+      <c r="G19" s="45"/>
+      <c r="H19" s="45"/>
+      <c r="I19" s="45"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" s="32" t="s">
         <v>168</v>
       </c>
-      <c r="B16" s="34">
-        <f>SUM(B2:B15)</f>
+      <c r="B20" s="33">
+        <f>SUM(B2:B17)</f>
         <v>2</v>
       </c>
-      <c r="C16" s="34">
-        <f t="shared" ref="C16:I16" si="0">SUM(C2:C15)</f>
+      <c r="C20" s="33">
+        <f t="shared" ref="C20:I20" si="0">SUM(C2:C17)</f>
         <v>8</v>
       </c>
-      <c r="D16" s="34">
+      <c r="D20" s="33">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="E16" s="34">
+      <c r="E20" s="33">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="F16" s="34">
+      <c r="F20" s="33">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="G16" s="34">
+      <c r="G20" s="33">
         <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="H16" s="34">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="I16" s="34">
+        <v>5</v>
+      </c>
+      <c r="H20" s="33">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+      <c r="I20" s="33">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
         <v>169</v>
       </c>
-      <c r="B17">
-        <v>14</v>
+      <c r="B21">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added use cases of 18-21
</commit_message>
<xml_diff>
--- a/I-AdoptUserStoriesanalysis_25022020.xlsx
+++ b/I-AdoptUserStoriesanalysis_25022020.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr hidePivotFieldList="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11010"/>
+  <workbookPr hidePivotFieldList="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anusu\python-workspace\usecase_analysis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/uqadevar/Documents/usecase_analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B84C865E-11DF-1046-B7F0-9945A2D975C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12030" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="19820" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Config" sheetId="2" r:id="rId1"/>
@@ -19,20 +20,53 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Analysis_Coding!$D$2:$D$16</definedName>
-    <definedName name="_xlchart.0" hidden="1">Results_UseCases!$B$1:$I$1</definedName>
-    <definedName name="_xlchart.1" hidden="1">Results_UseCases!$B$20:$I$20</definedName>
+    <definedName name="_xlchart.v1.0" hidden="1">Results_UseCases!$B$1:$I$1</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">Results_UseCases!$B$23:$I$23</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">Results_UseCases!$B$1:$I$1</definedName>
+    <definedName name="_xlchart.v1.22" hidden="1">Results_UseCases!$B$1:$I$1</definedName>
+    <definedName name="_xlchart.v1.23" hidden="1">Results_UseCases!$B$23:$I$23</definedName>
+    <definedName name="_xlchart.v1.24" hidden="1">Results_UseCases!$B$1:$I$1</definedName>
+    <definedName name="_xlchart.v1.25" hidden="1">Results_UseCases!$B$23:$I$23</definedName>
+    <definedName name="_xlchart.v1.3" hidden="1">Results_UseCases!$B$23:$I$23</definedName>
+    <definedName name="_xlchart.v1.4" hidden="1">Results_UseCases!$B$1:$I$1</definedName>
+    <definedName name="_xlchart.v1.5" hidden="1">Results_UseCases!$B$23:$I$23</definedName>
+    <definedName name="_xlchart.v2.10" hidden="1">Results_UseCases!$D$1</definedName>
+    <definedName name="_xlchart.v2.11" hidden="1">Results_UseCases!$D$2:$D$21</definedName>
+    <definedName name="_xlchart.v2.12" hidden="1">Results_UseCases!$E$1</definedName>
+    <definedName name="_xlchart.v2.13" hidden="1">Results_UseCases!$E$2:$E$21</definedName>
+    <definedName name="_xlchart.v2.14" hidden="1">Results_UseCases!$F$1</definedName>
+    <definedName name="_xlchart.v2.15" hidden="1">Results_UseCases!$F$2:$F$21</definedName>
+    <definedName name="_xlchart.v2.16" hidden="1">Results_UseCases!$G$1</definedName>
+    <definedName name="_xlchart.v2.17" hidden="1">Results_UseCases!$G$2:$G$21</definedName>
+    <definedName name="_xlchart.v2.18" hidden="1">Results_UseCases!$H$1</definedName>
+    <definedName name="_xlchart.v2.19" hidden="1">Results_UseCases!$H$2:$H$21</definedName>
+    <definedName name="_xlchart.v2.20" hidden="1">Results_UseCases!$I$1</definedName>
+    <definedName name="_xlchart.v2.21" hidden="1">Results_UseCases!$I$2:$I$21</definedName>
+    <definedName name="_xlchart.v2.6" hidden="1">Results_UseCases!$B$1</definedName>
+    <definedName name="_xlchart.v2.7" hidden="1">Results_UseCases!$B$2:$B$21</definedName>
+    <definedName name="_xlchart.v2.8" hidden="1">Results_UseCases!$C$1</definedName>
+    <definedName name="_xlchart.v2.9" hidden="1">Results_UseCases!$C$2:$C$21</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="231">
   <si>
     <t>https://github.com/i-adopt/users_stories/issues/1</t>
   </si>
@@ -2118,9 +2152,6 @@
     <t>SUM</t>
   </si>
   <si>
-    <t>N (number of user stories)</t>
-  </si>
-  <si>
     <t>use agreed mappings or alignments between terminologies to improve data exchange and integration</t>
   </si>
   <si>
@@ -2421,13 +2452,406 @@
   </si>
   <si>
     <t>support translation of term names between two terminologies (BODC PUV P01 and CF) to deliver data files compliant with the models.</t>
+  </si>
+  <si>
+    <t>https://github.com/i-adopt/users_stories/issues/21</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://github.com/i-adopt/users_stories/issues/21 </t>
+  </si>
+  <si>
+    <t>International Organization/Network Operator/Researcher - Improve the WIGOS Metadata Standard - Enable adequate use of observations/Support search engines</t>
+  </si>
+  <si>
+    <t>joergklausen</t>
+  </si>
+  <si>
+    <t>The value of observations is enhanced, now and in the distant future</t>
+  </si>
+  <si>
+    <t>Atmosphere, Terrestrial, Marine, Space, Hydrological, Cryosphere, Solid Earth</t>
+  </si>
+  <si>
+    <t>International Organization (WMO), Network Operator, Data Archive, Researcher</t>
+  </si>
+  <si>
+    <t>WIGOS Metadata Standard: Semantic standard and code tables. https://github.com/wmo-im/wmds/
+Please consider getting in touch with TT-WIGOSMD, so that efforts can be aligned.</t>
+  </si>
+  <si>
+    <t>standard representation of observed properties to support data discovery and interoperabilit with other data providers.</t>
+  </si>
+  <si>
+    <t>semantic modelling, data integration and analysis, semantic data search</t>
+  </si>
+  <si>
+    <t xml:space="preserve">N </t>
+  </si>
+  <si>
+    <t>https://github.com/i-adopt/users_stories/issues/18</t>
+  </si>
+  <si>
+    <t>Data engineer - create variable list - harmonize vocabular</t>
+  </si>
+  <si>
+    <t>smguru</t>
+  </si>
+  <si>
+    <t>Data Engineer</t>
+  </si>
+  <si>
+    <t>Environment, Ecology ecosystem</t>
+  </si>
+  <si>
+    <t>The aim is to harmonise observed properties without changing the definition of the original properties from the data sources.</t>
+  </si>
+  <si>
+    <t>https://github.com/i-adopt/users_stories/issues/19</t>
+  </si>
+  <si>
+    <t>metadata administrator</t>
+  </si>
+  <si>
+    <t>Data manager - improve semantic richness of coastal research metadata - better data interoperability and reusability</t>
+  </si>
+  <si>
+    <t>LM-HZG</t>
+  </si>
+  <si>
+    <t>bio-)geochemistry, environmental chemistry, oceanography and various earth system science modelling efforts with focus on interactions of ocean, land, atmosphere and us humans</t>
+  </si>
+  <si>
+    <t>everything that improves mutual understanding of (field) data producers and modellers, even from the same research domain, would help a lot</t>
+  </si>
+  <si>
+    <t>https://github.com/i-adopt/users_stories/issues/20</t>
+  </si>
+  <si>
+    <t>Researcher- find long time series data - efficient semantic search across multiple vocabularies</t>
+  </si>
+  <si>
+    <t>researcher</t>
+  </si>
+  <si>
+    <t>mabablue</t>
+  </si>
+  <si>
+    <t>aerosol science, atmospheric physics</t>
+  </si>
+  <si>
+    <t>see https://github.com/xiaofengleo/actris for a more detailed description
+This is a user story from ENVRI-FAIR WP8 Semantic Search WG (Lara Ferrighi) and the ACTRIS RI (Richard Rud, Paul Eckhardt)</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>create a global variables</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> list</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">I can </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>harmonise</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> different terms of similar conceptual meaning coming</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t xml:space="preserve"> from different data sources</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> into a common terminology to enable</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> data i</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>ntegration and discovery</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> of data from different data sources.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>…</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>harmonize</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> the inventory of coastal research </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>metadata</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> in our institutes data repository in order to reach a highest-possible degree of FAIRness</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">every interested party or stakeholder benefits from </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>(meta-)data interoperability and re-usability</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>find</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> long time series of aerosol optical properties in remote areas via </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>semantic search</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>across</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>multiple vocabularies</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">I can </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>find the same (NetCDF) data across the use of different vocabularies</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> WIGOS, CF Standard Names and the ACTRIS In Situ (internal vocabulary) for variable names.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Provide an international </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>standard</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> to document observations</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> comprehensively
+Use the standard operationally to adequately </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>describe observations</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Adequately describe my data holdings and enable DAR
+Adequately describe observations and </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>find/use other peoples'/organizations' observations</t>
+    </r>
+  </si>
+  <si>
+    <t>semantic representation of observed properties for data harmonization across different sources</t>
+  </si>
+  <si>
+    <t>semantic representation of observed properties for data interoperability</t>
+  </si>
+  <si>
+    <t>semantic search across multiple sources</t>
+  </si>
+  <si>
+    <t>semantic modelling, terminology management, terminology alignment, semantic data search</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="10" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2496,6 +2920,18 @@
     <font>
       <b/>
       <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF0070C0"/>
+      <name val="Calibri (Body)"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -2592,7 +3028,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -2674,11 +3110,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -2712,7 +3144,54 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2731,67 +3210,69 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chartEx1.xml><?xml version="1.0" encoding="utf-8"?>
 <cx:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex">
   <cx:chartData>
     <cx:data id="0">
       <cx:strDim type="cat">
-        <cx:f dir="row">_xlchart.0</cx:f>
+        <cx:f dir="row">_xlchart.v1.0</cx:f>
       </cx:strDim>
       <cx:numDim type="size">
-        <cx:f dir="row">_xlchart.1</cx:f>
+        <cx:f dir="row">_xlchart.v1.1</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
   <cx:chart>
     <cx:title pos="t" align="ctr" overlay="0">
       <cx:tx>
-        <cx:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1" compatLnSpc="0"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr algn="ctr" rtl="0">
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:sysClr val="windowText" lastClr="000000">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:sysClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr kumimoji="0" lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
-                <a:ln>
-                  <a:noFill/>
-                </a:ln>
-                <a:solidFill>
-                  <a:sysClr val="windowText" lastClr="000000">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:sysClr>
-                </a:solidFill>
-                <a:effectLst/>
-                <a:uLnTx/>
-                <a:uFillTx/>
-                <a:latin typeface="Calibri" panose="020F0502020204030204"/>
-              </a:rPr>
-              <a:t>Use Cases Coverage (N=14)</a:t>
-            </a:r>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </cx:rich>
+        <cx:txData>
+          <cx:v>Use Cases Coverage (N=43)</cx:v>
+        </cx:txData>
       </cx:tx>
+      <cx:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1" compatLnSpc="0"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr" rtl="0">
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:sysClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:r>
+            <a:rPr kumimoji="0" lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:sysClr>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:uLnTx/>
+              <a:uFillTx/>
+              <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+            </a:rPr>
+            <a:t>Use Cases Coverage (N=43)</a:t>
+          </a:r>
+        </a:p>
+      </cx:txPr>
     </cx:title>
     <cx:plotArea>
       <cx:plotAreaRegion>
         <cx:series layoutId="sunburst" uniqueId="{24BC00EE-2991-439A-B546-DC55FFC9F96F}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.0</cx:f>
+              <cx:f>_xlchart.v1.0</cx:f>
               <cx:v>terminology management data integration and analysis semantic data search terminology search data cleaning semantic modelling terminology alignment semantic annotation</cx:v>
             </cx:txData>
           </cx:tx>
@@ -3375,14 +3856,20 @@
     <xdr:to>
       <xdr:col>17</xdr:col>
       <xdr:colOff>485775</xdr:colOff>
-      <xdr:row>24</xdr:row>
+      <xdr:row>27</xdr:row>
       <xdr:rowOff>104774</xdr:rowOff>
     </xdr:to>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" Requires="cx">
+      <mc:Choice xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" Requires="cx1">
         <xdr:graphicFrame macro="">
           <xdr:nvGraphicFramePr>
-            <xdr:cNvPr id="2" name="Chart 1"/>
+            <xdr:cNvPr id="2" name="Chart 1">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000002000000}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
             <xdr:cNvGraphicFramePr/>
           </xdr:nvGraphicFramePr>
           <xdr:xfrm>
@@ -3391,7 +3878,7 @@
           </xdr:xfrm>
           <a:graphic>
             <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2014/chartex">
-              <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+              <cx:chart xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
             </a:graphicData>
           </a:graphic>
         </xdr:graphicFrame>
@@ -3405,6 +3892,10 @@
             </xdr:cNvSpPr>
           </xdr:nvSpPr>
           <xdr:spPr>
+            <a:xfrm>
+              <a:off x="13490575" y="571499"/>
+              <a:ext cx="5270500" cy="4384675"/>
+            </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
@@ -3422,7 +3913,7 @@
             <a:lstStyle/>
             <a:p>
               <a:r>
-                <a:rPr lang="en-US" sz="1100"/>
+                <a:rPr lang="en-GB" sz="1100"/>
                 <a:t>This chart isn't available in your version of Excel.
 Editing this shape or saving this workbook into a different file format will permanently break the chart.</a:t>
               </a:r>
@@ -3698,55 +4189,55 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="42.28515625" customWidth="1"/>
+    <col min="1" max="1" width="42.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="8" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="8" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="8" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="8" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="8"/>
     </row>
-    <row r="8" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="8"/>
     </row>
-    <row r="9" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="11" t="s">
         <v>103</v>
       </c>
@@ -3754,7 +4245,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="11" t="s">
         <v>112</v>
       </c>
@@ -3762,87 +4253,87 @@
         <v>113</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" s="20" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" s="21" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" s="21" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" s="21" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A17" s="21" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A18" s="21" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A19" s="21" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A20" s="21" t="s">
         <v>82</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B9" r:id="rId1"/>
-    <hyperlink ref="B10" r:id="rId2"/>
+    <hyperlink ref="B9" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="B10" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H17"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:H21"/>
   <sheetViews>
-    <sheetView zoomScale="15" zoomScaleNormal="15" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A17"/>
+    <sheetView topLeftCell="A19" zoomScale="128" zoomScaleNormal="128" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18:B20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16.5703125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="24.140625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="13.7109375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="16.7109375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="21.28515625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="20.5703125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="16.5" style="1" customWidth="1"/>
+    <col min="2" max="2" width="24.1640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="13.6640625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="16.6640625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="21.33203125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="20.5" style="1" customWidth="1"/>
     <col min="7" max="7" width="14" style="1" customWidth="1"/>
-    <col min="8" max="8" width="66.140625" style="1" customWidth="1"/>
-    <col min="12" max="12" width="9.140625" customWidth="1"/>
+    <col min="8" max="8" width="66.1640625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="9.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" s="14" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="12" t="s">
         <v>65</v>
       </c>
@@ -3868,11 +4359,11 @@
         <v>72</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="333.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="333.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="37" t="s">
+      <c r="B2" s="35" t="s">
         <v>3</v>
       </c>
       <c r="C2" s="3" t="s">
@@ -3894,33 +4385,33 @@
         <v>109</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="333.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="333.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="B3" s="35" t="s">
         <v>173</v>
       </c>
-      <c r="B3" s="37" t="s">
+      <c r="C3" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>174</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="E3" s="5" t="s">
+        <v>180</v>
+      </c>
+      <c r="F3" s="5" t="s">
         <v>176</v>
       </c>
-      <c r="D3" s="3" t="s">
-        <v>175</v>
-      </c>
-      <c r="E3" s="5" t="s">
-        <v>181</v>
-      </c>
-      <c r="F3" s="5" t="s">
+      <c r="G3" s="3" t="s">
         <v>177</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="H3" s="3" t="s">
         <v>178</v>
       </c>
-      <c r="H3" s="3" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="210" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:8" ht="192" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>7</v>
       </c>
@@ -3946,7 +4437,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="80" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>9</v>
       </c>
@@ -3972,7 +4463,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="150" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="160" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>15</v>
       </c>
@@ -3998,7 +4489,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="105" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="96" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>21</v>
       </c>
@@ -4024,7 +4515,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="300" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="256" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>26</v>
       </c>
@@ -4050,7 +4541,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="150" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" ht="128" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>31</v>
       </c>
@@ -4076,7 +4567,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="243.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" ht="243.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>36</v>
       </c>
@@ -4102,7 +4593,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="165" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" ht="144" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>43</v>
       </c>
@@ -4126,7 +4617,7 @@
       </c>
       <c r="H11" s="3"/>
     </row>
-    <row r="12" spans="1:8" ht="90" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" ht="80" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>47</v>
       </c>
@@ -4150,7 +4641,7 @@
       </c>
       <c r="H12" s="3"/>
     </row>
-    <row r="13" spans="1:8" ht="225" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" ht="176" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>49</v>
       </c>
@@ -4176,7 +4667,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="406.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" ht="406.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>55</v>
       </c>
@@ -4202,7 +4693,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="300" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" ht="272" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>57</v>
       </c>
@@ -4228,7 +4719,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="90" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" ht="96" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>60</v>
       </c>
@@ -4252,81 +4743,189 @@
       </c>
       <c r="H16" s="3"/>
     </row>
-    <row r="17" spans="1:8" ht="195" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" ht="192" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="B17" s="3" t="s">
         <v>183</v>
       </c>
-      <c r="B17" s="3" t="s">
+      <c r="C17" s="3" t="s">
         <v>184</v>
       </c>
-      <c r="C17" s="3" t="s">
+      <c r="D17" s="3" t="s">
         <v>185</v>
       </c>
-      <c r="D17" s="3" t="s">
+      <c r="E17" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="G17" s="3" t="s">
         <v>186</v>
       </c>
-      <c r="E17" s="3" t="s">
-        <v>189</v>
-      </c>
-      <c r="F17" s="3" t="s">
-        <v>190</v>
-      </c>
-      <c r="G17" s="3" t="s">
+      <c r="H17" s="3" t="s">
         <v>187</v>
       </c>
-      <c r="H17" s="3" t="s">
-        <v>188</v>
+    </row>
+    <row r="18" spans="1:8" ht="160" x14ac:dyDescent="0.2">
+      <c r="A18" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>204</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="G18" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="H18" s="3" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="224" x14ac:dyDescent="0.2">
+      <c r="A19" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="B19" s="47" t="s">
+        <v>210</v>
+      </c>
+      <c r="C19" s="44" t="s">
+        <v>211</v>
+      </c>
+      <c r="D19" s="44" t="s">
+        <v>209</v>
+      </c>
+      <c r="E19" s="44" t="s">
+        <v>222</v>
+      </c>
+      <c r="F19" s="44" t="s">
+        <v>223</v>
+      </c>
+      <c r="G19" s="44" t="s">
+        <v>212</v>
+      </c>
+      <c r="H19" s="44" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="128" x14ac:dyDescent="0.2">
+      <c r="A20" s="45" t="s">
+        <v>214</v>
+      </c>
+      <c r="B20" s="44" t="s">
+        <v>215</v>
+      </c>
+      <c r="C20" s="44" t="s">
+        <v>217</v>
+      </c>
+      <c r="D20" s="44" t="s">
+        <v>216</v>
+      </c>
+      <c r="E20" s="44" t="s">
+        <v>224</v>
+      </c>
+      <c r="F20" s="44" t="s">
+        <v>225</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="H20" s="44" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="261" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="45" t="s">
+        <v>192</v>
+      </c>
+      <c r="B21" s="44" t="s">
+        <v>193</v>
+      </c>
+      <c r="C21" s="44" t="s">
+        <v>194</v>
+      </c>
+      <c r="D21" s="44" t="s">
+        <v>197</v>
+      </c>
+      <c r="E21" s="44" t="s">
+        <v>226</v>
+      </c>
+      <c r="F21" s="44" t="s">
+        <v>195</v>
+      </c>
+      <c r="G21" s="44" t="s">
+        <v>196</v>
+      </c>
+      <c r="H21" s="3" t="s">
+        <v>198</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1"/>
-    <hyperlink ref="A5" r:id="rId2"/>
-    <hyperlink ref="A6" r:id="rId3"/>
-    <hyperlink ref="A7" r:id="rId4"/>
-    <hyperlink ref="A8" r:id="rId5"/>
-    <hyperlink ref="A9" r:id="rId6"/>
-    <hyperlink ref="A10" r:id="rId7"/>
-    <hyperlink ref="A11" r:id="rId8"/>
-    <hyperlink ref="A12" r:id="rId9"/>
-    <hyperlink ref="A13" r:id="rId10"/>
-    <hyperlink ref="A14" r:id="rId11"/>
-    <hyperlink ref="A15" r:id="rId12"/>
-    <hyperlink ref="A16" r:id="rId13"/>
-    <hyperlink ref="A4" r:id="rId14"/>
-    <hyperlink ref="A3" r:id="rId15"/>
-    <hyperlink ref="A17" r:id="rId16"/>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="A5" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
+    <hyperlink ref="A6" r:id="rId3" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
+    <hyperlink ref="A7" r:id="rId4" xr:uid="{00000000-0004-0000-0100-000003000000}"/>
+    <hyperlink ref="A8" r:id="rId5" xr:uid="{00000000-0004-0000-0100-000004000000}"/>
+    <hyperlink ref="A9" r:id="rId6" xr:uid="{00000000-0004-0000-0100-000005000000}"/>
+    <hyperlink ref="A10" r:id="rId7" xr:uid="{00000000-0004-0000-0100-000006000000}"/>
+    <hyperlink ref="A11" r:id="rId8" xr:uid="{00000000-0004-0000-0100-000007000000}"/>
+    <hyperlink ref="A12" r:id="rId9" xr:uid="{00000000-0004-0000-0100-000008000000}"/>
+    <hyperlink ref="A13" r:id="rId10" xr:uid="{00000000-0004-0000-0100-000009000000}"/>
+    <hyperlink ref="A14" r:id="rId11" xr:uid="{00000000-0004-0000-0100-00000A000000}"/>
+    <hyperlink ref="A15" r:id="rId12" xr:uid="{00000000-0004-0000-0100-00000B000000}"/>
+    <hyperlink ref="A16" r:id="rId13" xr:uid="{00000000-0004-0000-0100-00000C000000}"/>
+    <hyperlink ref="A4" r:id="rId14" xr:uid="{00000000-0004-0000-0100-00000D000000}"/>
+    <hyperlink ref="A3" r:id="rId15" xr:uid="{00000000-0004-0000-0100-00000E000000}"/>
+    <hyperlink ref="A17" r:id="rId16" xr:uid="{00000000-0004-0000-0100-00000F000000}"/>
+    <hyperlink ref="A21" r:id="rId17" xr:uid="{941C89A0-C9B1-344E-8E6F-3187DC9327CC}"/>
+    <hyperlink ref="A18" r:id="rId18" xr:uid="{F1D3E0C5-9358-1B49-95E2-F3645EC1B4C9}"/>
+    <hyperlink ref="A19" r:id="rId19" xr:uid="{59B79177-84D9-E34C-9306-E4C5911ECA32}"/>
+    <hyperlink ref="A20" r:id="rId20" xr:uid="{6EF1EEFE-C3BE-9042-AA3A-7117816A86F9}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId17"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId21"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N17"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:N21"/>
   <sheetViews>
-    <sheetView zoomScale="30" zoomScaleNormal="30" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2:N17"/>
+    <sheetView topLeftCell="A8" zoomScale="87" zoomScaleNormal="87" workbookViewId="0">
+      <selection activeCell="G18" sqref="G18:N20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="50.42578125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="44.140625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="22.28515625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="23.7109375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="38.140625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="25.140625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="50.5" style="1" customWidth="1"/>
+    <col min="2" max="2" width="44.1640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="22.33203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="23.6640625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="38.1640625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="25.1640625" style="1" customWidth="1"/>
     <col min="7" max="7" width="13" style="1" customWidth="1"/>
-    <col min="8" max="8" width="12.28515625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="11.5703125" customWidth="1"/>
+    <col min="8" max="8" width="12.33203125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="11.5" customWidth="1"/>
     <col min="10" max="10" width="14" customWidth="1"/>
-    <col min="12" max="12" width="13.28515625" customWidth="1"/>
-    <col min="13" max="14" width="15.42578125" customWidth="1"/>
+    <col min="12" max="12" width="13.33203125" customWidth="1"/>
+    <col min="13" max="14" width="15.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="63" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" ht="51" x14ac:dyDescent="0.2">
       <c r="A1" s="23" t="str">
         <f>GithubIssues!A1</f>
         <v>github_url</v>
@@ -4372,11 +4971,11 @@
         <v>82</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="37" t="s">
+      <c r="B2" s="35" t="s">
         <v>3</v>
       </c>
       <c r="C2" s="15" t="s">
@@ -4404,23 +5003,23 @@
       <c r="M2" s="30"/>
       <c r="N2" s="30"/>
     </row>
-    <row r="3" spans="1:14" ht="75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" ht="75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="B3" s="35" t="s">
         <v>173</v>
       </c>
-      <c r="B3" s="37" t="s">
-        <v>174</v>
-      </c>
-      <c r="C3" s="38" t="s">
+      <c r="C3" s="36" t="s">
         <v>95</v>
       </c>
       <c r="D3" s="19" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>182</v>
-      </c>
-      <c r="F3" s="39" t="s">
+        <v>181</v>
+      </c>
+      <c r="F3" s="37" t="s">
         <v>152</v>
       </c>
       <c r="G3" s="29"/>
@@ -4434,7 +5033,7 @@
       <c r="M3" s="30"/>
       <c r="N3" s="30"/>
     </row>
-    <row r="4" spans="1:14" ht="68.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" ht="68.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>7</v>
       </c>
@@ -4466,7 +5065,7 @@
       <c r="M4" s="30"/>
       <c r="N4" s="30"/>
     </row>
-    <row r="5" spans="1:14" ht="55.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" ht="55.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>9</v>
       </c>
@@ -4498,7 +5097,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:14" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" ht="53.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>15</v>
       </c>
@@ -4530,7 +5129,7 @@
       <c r="M6" s="30"/>
       <c r="N6" s="30"/>
     </row>
-    <row r="7" spans="1:14" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>21</v>
       </c>
@@ -4562,7 +5161,7 @@
       <c r="M7" s="30"/>
       <c r="N7" s="30"/>
     </row>
-    <row r="8" spans="1:14" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" ht="52.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>26</v>
       </c>
@@ -4594,7 +5193,7 @@
       <c r="M8" s="30"/>
       <c r="N8" s="30"/>
     </row>
-    <row r="9" spans="1:14" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>31</v>
       </c>
@@ -4626,7 +5225,7 @@
       <c r="M9" s="30"/>
       <c r="N9" s="30"/>
     </row>
-    <row r="10" spans="1:14" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" ht="51.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>36</v>
       </c>
@@ -4658,7 +5257,7 @@
       <c r="M10" s="30"/>
       <c r="N10" s="30"/>
     </row>
-    <row r="11" spans="1:14" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" ht="45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>43</v>
       </c>
@@ -4690,7 +5289,7 @@
       <c r="M11" s="30"/>
       <c r="N11" s="30"/>
     </row>
-    <row r="12" spans="1:14" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>47</v>
       </c>
@@ -4722,7 +5321,7 @@
       <c r="M12" s="30"/>
       <c r="N12" s="30"/>
     </row>
-    <row r="13" spans="1:14" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" ht="52.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>49</v>
       </c>
@@ -4754,7 +5353,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:14" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" ht="51.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>55</v>
       </c>
@@ -4784,7 +5383,7 @@
       <c r="M14" s="30"/>
       <c r="N14" s="30"/>
     </row>
-    <row r="15" spans="1:14" ht="79.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" ht="79.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>57</v>
       </c>
@@ -4795,24 +5394,24 @@
         <v>108</v>
       </c>
       <c r="D15" s="19" t="s">
+        <v>170</v>
+      </c>
+      <c r="E15" s="32" t="s">
+        <v>169</v>
+      </c>
+      <c r="F15" s="6" t="s">
         <v>171</v>
       </c>
-      <c r="E15" s="34" t="s">
-        <v>170</v>
-      </c>
-      <c r="F15" s="6" t="s">
-        <v>172</v>
-      </c>
       <c r="G15" s="29">
         <v>1</v>
       </c>
-      <c r="H15" s="35">
-        <v>1</v>
-      </c>
-      <c r="I15" s="36">
-        <v>1</v>
-      </c>
-      <c r="J15" s="36">
+      <c r="H15" s="33">
+        <v>1</v>
+      </c>
+      <c r="I15" s="34">
+        <v>1</v>
+      </c>
+      <c r="J15" s="34">
         <v>1</v>
       </c>
       <c r="K15" s="30"/>
@@ -4822,7 +5421,7 @@
       </c>
       <c r="N15" s="30"/>
     </row>
-    <row r="16" spans="1:14" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" ht="53.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>60</v>
       </c>
@@ -4854,23 +5453,23 @@
       <c r="M16" s="30"/>
       <c r="N16" s="30"/>
     </row>
-    <row r="17" spans="1:14" ht="60" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14" ht="48" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="B17" s="3" t="s">
         <v>183</v>
       </c>
-      <c r="B17" s="3" t="s">
-        <v>184</v>
-      </c>
-      <c r="C17" s="41" t="s">
+      <c r="C17" s="39" t="s">
         <v>157</v>
       </c>
-      <c r="D17" s="38" t="s">
+      <c r="D17" s="36" t="s">
         <v>132</v>
       </c>
-      <c r="E17" s="40" t="s">
-        <v>191</v>
-      </c>
-      <c r="F17" s="42" t="s">
+      <c r="E17" s="38" t="s">
+        <v>190</v>
+      </c>
+      <c r="F17" s="40" t="s">
         <v>87</v>
       </c>
       <c r="G17" s="24"/>
@@ -4879,765 +5478,989 @@
       <c r="J17" s="27"/>
       <c r="K17" s="27"/>
       <c r="L17" s="27"/>
-      <c r="M17" s="43">
+      <c r="M17" s="41">
         <v>1</v>
       </c>
       <c r="N17" s="27"/>
+    </row>
+    <row r="18" spans="1:14" ht="68" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>157</v>
+      </c>
+      <c r="D18" s="48" t="s">
+        <v>75</v>
+      </c>
+      <c r="E18" s="6" t="s">
+        <v>227</v>
+      </c>
+      <c r="F18" s="50" t="s">
+        <v>230</v>
+      </c>
+      <c r="G18" s="52">
+        <v>1</v>
+      </c>
+      <c r="H18" s="52"/>
+      <c r="I18" s="51">
+        <v>1</v>
+      </c>
+      <c r="J18" s="51"/>
+      <c r="K18" s="51"/>
+      <c r="L18" s="51">
+        <v>1</v>
+      </c>
+      <c r="M18" s="51">
+        <v>1</v>
+      </c>
+      <c r="N18" s="51"/>
+    </row>
+    <row r="19" spans="1:14" ht="48" x14ac:dyDescent="0.2">
+      <c r="A19" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="B19" s="47" t="s">
+        <v>210</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>157</v>
+      </c>
+      <c r="D19" s="48" t="s">
+        <v>155</v>
+      </c>
+      <c r="E19" s="6" t="s">
+        <v>228</v>
+      </c>
+      <c r="F19" s="50" t="s">
+        <v>146</v>
+      </c>
+      <c r="G19" s="52"/>
+      <c r="H19" s="52">
+        <v>1</v>
+      </c>
+      <c r="I19" s="51"/>
+      <c r="J19" s="51"/>
+      <c r="K19" s="51"/>
+      <c r="L19" s="51">
+        <v>1</v>
+      </c>
+      <c r="M19" s="51"/>
+      <c r="N19" s="51"/>
+    </row>
+    <row r="20" spans="1:14" ht="48" x14ac:dyDescent="0.2">
+      <c r="A20" s="45" t="s">
+        <v>214</v>
+      </c>
+      <c r="B20" s="44" t="s">
+        <v>215</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="D20" s="48" t="s">
+        <v>155</v>
+      </c>
+      <c r="E20" s="6" t="s">
+        <v>229</v>
+      </c>
+      <c r="F20" s="50" t="s">
+        <v>146</v>
+      </c>
+      <c r="G20" s="52"/>
+      <c r="H20" s="52">
+        <v>1</v>
+      </c>
+      <c r="I20" s="51">
+        <v>1</v>
+      </c>
+      <c r="J20" s="51"/>
+      <c r="K20" s="51"/>
+      <c r="L20" s="51"/>
+      <c r="M20" s="51"/>
+      <c r="N20" s="51"/>
+    </row>
+    <row r="21" spans="1:14" ht="64" x14ac:dyDescent="0.2">
+      <c r="A21" s="43" t="s">
+        <v>191</v>
+      </c>
+      <c r="B21" s="46" t="s">
+        <v>193</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="D21" s="49" t="s">
+        <v>132</v>
+      </c>
+      <c r="E21" s="44" t="s">
+        <v>199</v>
+      </c>
+      <c r="F21" s="6" t="s">
+        <v>200</v>
+      </c>
+      <c r="G21" s="52"/>
+      <c r="H21" s="52">
+        <v>1</v>
+      </c>
+      <c r="I21" s="51">
+        <v>1</v>
+      </c>
+      <c r="J21" s="51"/>
+      <c r="K21" s="51"/>
+      <c r="L21" s="51">
+        <v>1</v>
+      </c>
+      <c r="M21" s="51"/>
+      <c r="N21" s="51"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1"/>
-    <hyperlink ref="A5" r:id="rId2"/>
-    <hyperlink ref="A6" r:id="rId3"/>
-    <hyperlink ref="A7" r:id="rId4"/>
-    <hyperlink ref="A8" r:id="rId5"/>
-    <hyperlink ref="A9" r:id="rId6"/>
-    <hyperlink ref="A10" r:id="rId7"/>
-    <hyperlink ref="A11" r:id="rId8"/>
-    <hyperlink ref="A12" r:id="rId9"/>
-    <hyperlink ref="A13" r:id="rId10"/>
-    <hyperlink ref="A14" r:id="rId11"/>
-    <hyperlink ref="A15" r:id="rId12"/>
-    <hyperlink ref="A16" r:id="rId13"/>
-    <hyperlink ref="A4" r:id="rId14"/>
-    <hyperlink ref="A3" r:id="rId15"/>
-    <hyperlink ref="A17" r:id="rId16"/>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
+    <hyperlink ref="A5" r:id="rId2" xr:uid="{00000000-0004-0000-0200-000001000000}"/>
+    <hyperlink ref="A6" r:id="rId3" xr:uid="{00000000-0004-0000-0200-000002000000}"/>
+    <hyperlink ref="A7" r:id="rId4" xr:uid="{00000000-0004-0000-0200-000003000000}"/>
+    <hyperlink ref="A8" r:id="rId5" xr:uid="{00000000-0004-0000-0200-000004000000}"/>
+    <hyperlink ref="A9" r:id="rId6" xr:uid="{00000000-0004-0000-0200-000005000000}"/>
+    <hyperlink ref="A10" r:id="rId7" xr:uid="{00000000-0004-0000-0200-000006000000}"/>
+    <hyperlink ref="A11" r:id="rId8" xr:uid="{00000000-0004-0000-0200-000007000000}"/>
+    <hyperlink ref="A12" r:id="rId9" xr:uid="{00000000-0004-0000-0200-000008000000}"/>
+    <hyperlink ref="A13" r:id="rId10" xr:uid="{00000000-0004-0000-0200-000009000000}"/>
+    <hyperlink ref="A14" r:id="rId11" xr:uid="{00000000-0004-0000-0200-00000A000000}"/>
+    <hyperlink ref="A15" r:id="rId12" xr:uid="{00000000-0004-0000-0200-00000B000000}"/>
+    <hyperlink ref="A16" r:id="rId13" xr:uid="{00000000-0004-0000-0200-00000C000000}"/>
+    <hyperlink ref="A4" r:id="rId14" xr:uid="{00000000-0004-0000-0200-00000D000000}"/>
+    <hyperlink ref="A3" r:id="rId15" xr:uid="{00000000-0004-0000-0200-00000E000000}"/>
+    <hyperlink ref="A17" r:id="rId16" xr:uid="{00000000-0004-0000-0200-00000F000000}"/>
+    <hyperlink ref="A21" r:id="rId17" xr:uid="{37996934-38AC-9C41-9B56-605207D9413E}"/>
+    <hyperlink ref="A18" r:id="rId18" xr:uid="{B548DAA8-6177-2243-812C-4B78D6CDD036}"/>
+    <hyperlink ref="A19" r:id="rId19" xr:uid="{E04DAA6E-365E-C74D-B098-E4870C45C048}"/>
+    <hyperlink ref="A20" r:id="rId20" xr:uid="{10594345-84E7-5B49-8BF4-A3AA53EDD089}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId17"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId21"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I21"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A1:I24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20:I20"/>
+      <selection activeCell="I35" sqref="I35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="68.5703125" customWidth="1"/>
-    <col min="2" max="2" width="15.42578125" customWidth="1"/>
-    <col min="3" max="3" width="13.140625" customWidth="1"/>
-    <col min="5" max="5" width="11.7109375" customWidth="1"/>
-    <col min="7" max="7" width="11.140625" customWidth="1"/>
-    <col min="8" max="8" width="11.5703125" customWidth="1"/>
+    <col min="1" max="1" width="68.5" customWidth="1"/>
+    <col min="2" max="2" width="15.5" customWidth="1"/>
+    <col min="3" max="3" width="13.1640625" customWidth="1"/>
+    <col min="5" max="5" width="11.6640625" customWidth="1"/>
+    <col min="7" max="7" width="11.1640625" customWidth="1"/>
+    <col min="8" max="8" width="11.5" customWidth="1"/>
     <col min="9" max="9" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="48" x14ac:dyDescent="0.2">
       <c r="A1" s="23" t="str">
         <f>GithubIssues!A1</f>
         <v>github_url</v>
       </c>
-      <c r="B1" s="31" t="str">
+      <c r="B1" s="53" t="str">
         <f>Analysis_Coding!G1</f>
         <v>terminology management</v>
       </c>
-      <c r="C1" s="31" t="str">
+      <c r="C1" s="53" t="str">
         <f>Analysis_Coding!H1</f>
         <v>data integration and analysis</v>
       </c>
-      <c r="D1" s="31" t="str">
+      <c r="D1" s="53" t="str">
         <f>Analysis_Coding!I1</f>
         <v>semantic data search</v>
       </c>
-      <c r="E1" s="31" t="str">
+      <c r="E1" s="53" t="str">
         <f>Analysis_Coding!J1</f>
         <v>terminology search</v>
       </c>
-      <c r="F1" s="31" t="str">
+      <c r="F1" s="53" t="str">
         <f>Analysis_Coding!K1</f>
         <v>data cleaning</v>
       </c>
-      <c r="G1" s="31" t="str">
+      <c r="G1" s="53" t="str">
         <f>Analysis_Coding!L1</f>
         <v>semantic modelling</v>
       </c>
-      <c r="H1" s="31" t="str">
+      <c r="H1" s="53" t="str">
         <f>Analysis_Coding!M1</f>
         <v>terminology alignment</v>
       </c>
-      <c r="I1" s="31" t="str">
+      <c r="I1" s="53" t="str">
         <f>Analysis_Coding!N1</f>
         <v>semantic annotation</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="24" t="str">
         <f>GithubIssues!A2</f>
         <v>https://github.com/i-adopt/users_stories/issues/1</v>
       </c>
-      <c r="B2" s="27">
+      <c r="B2" s="54">
         <f>Analysis_Coding!G2</f>
         <v>1</v>
       </c>
-      <c r="C2" s="27">
+      <c r="C2" s="54">
         <f>Analysis_Coding!H2</f>
         <v>0</v>
       </c>
-      <c r="D2" s="27">
+      <c r="D2" s="54">
         <f>Analysis_Coding!I2</f>
         <v>0</v>
       </c>
-      <c r="E2" s="27">
+      <c r="E2" s="54">
         <f>Analysis_Coding!J2</f>
         <v>0</v>
       </c>
-      <c r="F2" s="27">
+      <c r="F2" s="54">
         <f>Analysis_Coding!K2</f>
         <v>0</v>
       </c>
-      <c r="G2" s="27">
+      <c r="G2" s="54">
         <f>Analysis_Coding!L2</f>
         <v>1</v>
       </c>
-      <c r="H2" s="27">
+      <c r="H2" s="54">
         <f>Analysis_Coding!M2</f>
         <v>0</v>
       </c>
-      <c r="I2" s="27">
+      <c r="I2" s="54">
         <f>Analysis_Coding!N2</f>
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="24" t="str">
         <f>GithubIssues!A3</f>
         <v>https://github.com/i-adopt/users_stories/issues/3</v>
       </c>
-      <c r="B3" s="27">
+      <c r="B3" s="54">
         <f>Analysis_Coding!G3</f>
         <v>0</v>
       </c>
-      <c r="C3" s="27">
+      <c r="C3" s="54">
         <f>Analysis_Coding!H3</f>
         <v>0</v>
       </c>
-      <c r="D3" s="27">
+      <c r="D3" s="54">
         <f>Analysis_Coding!I3</f>
         <v>0</v>
       </c>
-      <c r="E3" s="27">
+      <c r="E3" s="54">
         <f>Analysis_Coding!J3</f>
         <v>0</v>
       </c>
-      <c r="F3" s="27">
+      <c r="F3" s="54">
         <f>Analysis_Coding!K3</f>
         <v>0</v>
       </c>
-      <c r="G3" s="27">
+      <c r="G3" s="54">
         <f>Analysis_Coding!L3</f>
         <v>1</v>
       </c>
-      <c r="H3" s="27">
+      <c r="H3" s="54">
         <f>Analysis_Coding!M3</f>
         <v>0</v>
       </c>
-      <c r="I3" s="27">
+      <c r="I3" s="54">
         <f>Analysis_Coding!N3</f>
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="24" t="str">
         <f>GithubIssues!A4</f>
         <v>https://github.com/i-adopt/users_stories/issues/4</v>
       </c>
-      <c r="B4" s="27">
+      <c r="B4" s="54">
         <f>Analysis_Coding!G4</f>
         <v>0</v>
       </c>
-      <c r="C4" s="27">
+      <c r="C4" s="54">
         <f>Analysis_Coding!H4</f>
         <v>1</v>
       </c>
-      <c r="D4" s="27">
+      <c r="D4" s="54">
         <f>Analysis_Coding!I4</f>
         <v>1</v>
       </c>
-      <c r="E4" s="27">
+      <c r="E4" s="54">
         <f>Analysis_Coding!J4</f>
         <v>0</v>
       </c>
-      <c r="F4" s="27">
+      <c r="F4" s="54">
         <f>Analysis_Coding!K4</f>
         <v>0</v>
       </c>
-      <c r="G4" s="27">
+      <c r="G4" s="54">
         <f>Analysis_Coding!L4</f>
         <v>0</v>
       </c>
-      <c r="H4" s="27">
+      <c r="H4" s="54">
         <f>Analysis_Coding!M4</f>
         <v>0</v>
       </c>
-      <c r="I4" s="27">
+      <c r="I4" s="54">
         <f>Analysis_Coding!N4</f>
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="24" t="str">
         <f>GithubIssues!A5</f>
         <v>https://github.com/i-adopt/users_stories/issues/5</v>
       </c>
-      <c r="B5" s="27">
+      <c r="B5" s="54">
         <f>Analysis_Coding!G5</f>
         <v>0</v>
       </c>
-      <c r="C5" s="27">
+      <c r="C5" s="54">
         <f>Analysis_Coding!H5</f>
         <v>0</v>
       </c>
-      <c r="D5" s="27">
+      <c r="D5" s="54">
         <f>Analysis_Coding!I5</f>
         <v>0</v>
       </c>
-      <c r="E5" s="27">
+      <c r="E5" s="54">
         <f>Analysis_Coding!J5</f>
         <v>1</v>
       </c>
-      <c r="F5" s="27">
+      <c r="F5" s="54">
         <f>Analysis_Coding!K5</f>
         <v>0</v>
       </c>
-      <c r="G5" s="27">
+      <c r="G5" s="54">
         <f>Analysis_Coding!L5</f>
         <v>0</v>
       </c>
-      <c r="H5" s="27">
+      <c r="H5" s="54">
         <f>Analysis_Coding!M5</f>
         <v>0</v>
       </c>
-      <c r="I5" s="27">
+      <c r="I5" s="54">
         <f>Analysis_Coding!N5</f>
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="24" t="str">
         <f>GithubIssues!A6</f>
         <v>https://github.com/i-adopt/users_stories/issues/6</v>
       </c>
-      <c r="B6" s="27">
+      <c r="B6" s="54">
         <f>Analysis_Coding!G6</f>
         <v>0</v>
       </c>
-      <c r="C6" s="27">
+      <c r="C6" s="54">
         <f>Analysis_Coding!H6</f>
         <v>0</v>
       </c>
-      <c r="D6" s="27">
+      <c r="D6" s="54">
         <f>Analysis_Coding!I6</f>
         <v>0</v>
       </c>
-      <c r="E6" s="27">
+      <c r="E6" s="54">
         <f>Analysis_Coding!J6</f>
         <v>1</v>
       </c>
-      <c r="F6" s="27">
+      <c r="F6" s="54">
         <f>Analysis_Coding!K6</f>
         <v>0</v>
       </c>
-      <c r="G6" s="27">
+      <c r="G6" s="54">
         <f>Analysis_Coding!L6</f>
         <v>1</v>
       </c>
-      <c r="H6" s="27">
+      <c r="H6" s="54">
         <f>Analysis_Coding!M6</f>
         <v>0</v>
       </c>
-      <c r="I6" s="27">
+      <c r="I6" s="54">
         <f>Analysis_Coding!N6</f>
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="24" t="str">
         <f>GithubIssues!A7</f>
         <v>https://github.com/i-adopt/users_stories/issues/7</v>
       </c>
-      <c r="B7" s="27">
+      <c r="B7" s="54">
         <f>Analysis_Coding!G7</f>
         <v>0</v>
       </c>
-      <c r="C7" s="27">
+      <c r="C7" s="54">
         <f>Analysis_Coding!H7</f>
         <v>1</v>
       </c>
-      <c r="D7" s="27">
+      <c r="D7" s="54">
         <f>Analysis_Coding!I7</f>
         <v>1</v>
       </c>
-      <c r="E7" s="27">
+      <c r="E7" s="54">
         <f>Analysis_Coding!J7</f>
         <v>0</v>
       </c>
-      <c r="F7" s="27">
+      <c r="F7" s="54">
         <f>Analysis_Coding!K7</f>
         <v>0</v>
       </c>
-      <c r="G7" s="27">
+      <c r="G7" s="54">
         <f>Analysis_Coding!L7</f>
         <v>0</v>
       </c>
-      <c r="H7" s="27">
+      <c r="H7" s="54">
         <f>Analysis_Coding!M7</f>
         <v>0</v>
       </c>
-      <c r="I7" s="27">
+      <c r="I7" s="54">
         <f>Analysis_Coding!N7</f>
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="24" t="str">
         <f>GithubIssues!A8</f>
         <v>https://github.com/i-adopt/users_stories/issues/8</v>
       </c>
-      <c r="B8" s="27">
+      <c r="B8" s="54">
         <f>Analysis_Coding!G8</f>
         <v>0</v>
       </c>
-      <c r="C8" s="27">
+      <c r="C8" s="54">
         <f>Analysis_Coding!H8</f>
         <v>1</v>
       </c>
-      <c r="D8" s="27">
+      <c r="D8" s="54">
         <f>Analysis_Coding!I8</f>
         <v>1</v>
       </c>
-      <c r="E8" s="27">
+      <c r="E8" s="54">
         <f>Analysis_Coding!J8</f>
         <v>0</v>
       </c>
-      <c r="F8" s="27">
+      <c r="F8" s="54">
         <f>Analysis_Coding!K8</f>
         <v>0</v>
       </c>
-      <c r="G8" s="27">
+      <c r="G8" s="54">
         <f>Analysis_Coding!L8</f>
         <v>0</v>
       </c>
-      <c r="H8" s="27">
+      <c r="H8" s="54">
         <f>Analysis_Coding!M8</f>
         <v>0</v>
       </c>
-      <c r="I8" s="27">
+      <c r="I8" s="54">
         <f>Analysis_Coding!N8</f>
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="24" t="str">
         <f>GithubIssues!A9</f>
         <v>https://github.com/i-adopt/users_stories/issues/9</v>
       </c>
-      <c r="B9" s="27">
+      <c r="B9" s="54">
         <f>Analysis_Coding!G9</f>
         <v>0</v>
       </c>
-      <c r="C9" s="27">
+      <c r="C9" s="54">
         <f>Analysis_Coding!H9</f>
         <v>0</v>
       </c>
-      <c r="D9" s="27">
+      <c r="D9" s="54">
         <f>Analysis_Coding!I9</f>
         <v>1</v>
       </c>
-      <c r="E9" s="27">
+      <c r="E9" s="54">
         <f>Analysis_Coding!J9</f>
         <v>0</v>
       </c>
-      <c r="F9" s="27">
+      <c r="F9" s="54">
         <f>Analysis_Coding!K9</f>
         <v>1</v>
       </c>
-      <c r="G9" s="27">
+      <c r="G9" s="54">
         <f>Analysis_Coding!L9</f>
         <v>0</v>
       </c>
-      <c r="H9" s="27">
+      <c r="H9" s="54">
         <f>Analysis_Coding!M9</f>
         <v>0</v>
       </c>
-      <c r="I9" s="27">
+      <c r="I9" s="54">
         <f>Analysis_Coding!N9</f>
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="24" t="str">
         <f>GithubIssues!A10</f>
         <v>https://github.com/i-adopt/users_stories/issues/10</v>
       </c>
-      <c r="B10" s="27">
+      <c r="B10" s="54">
         <f>Analysis_Coding!G10</f>
         <v>0</v>
       </c>
-      <c r="C10" s="27">
+      <c r="C10" s="54">
         <f>Analysis_Coding!H10</f>
         <v>1</v>
       </c>
-      <c r="D10" s="27">
+      <c r="D10" s="54">
         <f>Analysis_Coding!I10</f>
         <v>1</v>
       </c>
-      <c r="E10" s="27">
+      <c r="E10" s="54">
         <f>Analysis_Coding!J10</f>
         <v>0</v>
       </c>
-      <c r="F10" s="27">
+      <c r="F10" s="54">
         <f>Analysis_Coding!K10</f>
         <v>0</v>
       </c>
-      <c r="G10" s="27">
+      <c r="G10" s="54">
         <f>Analysis_Coding!L10</f>
         <v>0</v>
       </c>
-      <c r="H10" s="27">
+      <c r="H10" s="54">
         <f>Analysis_Coding!M10</f>
         <v>0</v>
       </c>
-      <c r="I10" s="27">
+      <c r="I10" s="54">
         <f>Analysis_Coding!N10</f>
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="24" t="str">
         <f>GithubIssues!A11</f>
         <v>https://github.com/i-adopt/users_stories/issues/11</v>
       </c>
-      <c r="B11" s="27">
+      <c r="B11" s="54">
         <f>Analysis_Coding!G11</f>
         <v>0</v>
       </c>
-      <c r="C11" s="27">
+      <c r="C11" s="54">
         <f>Analysis_Coding!H11</f>
         <v>1</v>
       </c>
-      <c r="D11" s="27">
+      <c r="D11" s="54">
         <f>Analysis_Coding!I11</f>
         <v>1</v>
       </c>
-      <c r="E11" s="27">
+      <c r="E11" s="54">
         <f>Analysis_Coding!J11</f>
         <v>0</v>
       </c>
-      <c r="F11" s="27">
+      <c r="F11" s="54">
         <f>Analysis_Coding!K11</f>
         <v>0</v>
       </c>
-      <c r="G11" s="27">
+      <c r="G11" s="54">
         <f>Analysis_Coding!L11</f>
         <v>0</v>
       </c>
-      <c r="H11" s="27">
+      <c r="H11" s="54">
         <f>Analysis_Coding!M11</f>
         <v>0</v>
       </c>
-      <c r="I11" s="27">
+      <c r="I11" s="54">
         <f>Analysis_Coding!N11</f>
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="24" t="str">
         <f>GithubIssues!A12</f>
         <v>https://github.com/i-adopt/users_stories/issues/12</v>
       </c>
-      <c r="B12" s="27">
+      <c r="B12" s="54">
         <f>Analysis_Coding!G12</f>
         <v>0</v>
       </c>
-      <c r="C12" s="27">
+      <c r="C12" s="54">
         <f>Analysis_Coding!H12</f>
         <v>1</v>
       </c>
-      <c r="D12" s="27">
+      <c r="D12" s="54">
         <f>Analysis_Coding!I12</f>
         <v>1</v>
       </c>
-      <c r="E12" s="27">
+      <c r="E12" s="54">
         <f>Analysis_Coding!J12</f>
         <v>0</v>
       </c>
-      <c r="F12" s="27">
+      <c r="F12" s="54">
         <f>Analysis_Coding!K12</f>
         <v>0</v>
       </c>
-      <c r="G12" s="27">
+      <c r="G12" s="54">
         <f>Analysis_Coding!L12</f>
         <v>0</v>
       </c>
-      <c r="H12" s="27">
+      <c r="H12" s="54">
         <f>Analysis_Coding!M12</f>
         <v>0</v>
       </c>
-      <c r="I12" s="27">
+      <c r="I12" s="54">
         <f>Analysis_Coding!N12</f>
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="24" t="str">
         <f>GithubIssues!A13</f>
         <v>https://github.com/i-adopt/users_stories/issues/13</v>
       </c>
-      <c r="B13" s="27">
+      <c r="B13" s="54">
         <f>Analysis_Coding!G13</f>
         <v>0</v>
       </c>
-      <c r="C13" s="27">
+      <c r="C13" s="54">
         <f>Analysis_Coding!H13</f>
         <v>0</v>
       </c>
-      <c r="D13" s="27">
+      <c r="D13" s="54">
         <f>Analysis_Coding!I13</f>
         <v>0</v>
       </c>
-      <c r="E13" s="27">
+      <c r="E13" s="54">
         <f>Analysis_Coding!J13</f>
         <v>0</v>
       </c>
-      <c r="F13" s="27">
+      <c r="F13" s="54">
         <f>Analysis_Coding!K13</f>
         <v>0</v>
       </c>
-      <c r="G13" s="27">
+      <c r="G13" s="54">
         <f>Analysis_Coding!L13</f>
         <v>1</v>
       </c>
-      <c r="H13" s="27">
+      <c r="H13" s="54">
         <f>Analysis_Coding!M13</f>
         <v>0</v>
       </c>
-      <c r="I13" s="27">
+      <c r="I13" s="54">
         <f>Analysis_Coding!N13</f>
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="24" t="str">
         <f>GithubIssues!A14</f>
         <v>https://github.com/i-adopt/users_stories/issues/14</v>
       </c>
-      <c r="B14" s="27">
+      <c r="B14" s="54">
         <f>Analysis_Coding!G14</f>
         <v>0</v>
       </c>
-      <c r="C14" s="27">
+      <c r="C14" s="54">
         <f>Analysis_Coding!H14</f>
         <v>0</v>
       </c>
-      <c r="D14" s="27">
+      <c r="D14" s="54">
         <f>Analysis_Coding!I14</f>
         <v>0</v>
       </c>
-      <c r="E14" s="27">
+      <c r="E14" s="54">
         <f>Analysis_Coding!J14</f>
         <v>0</v>
       </c>
-      <c r="F14" s="27">
+      <c r="F14" s="54">
         <f>Analysis_Coding!K14</f>
         <v>0</v>
       </c>
-      <c r="G14" s="27">
+      <c r="G14" s="54">
         <f>Analysis_Coding!L14</f>
         <v>1</v>
       </c>
-      <c r="H14" s="27">
+      <c r="H14" s="54">
         <f>Analysis_Coding!M14</f>
         <v>0</v>
       </c>
-      <c r="I14" s="27">
+      <c r="I14" s="54">
         <f>Analysis_Coding!N14</f>
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="24" t="str">
         <f>GithubIssues!A15</f>
         <v>https://github.com/i-adopt/users_stories/issues/15</v>
       </c>
-      <c r="B15" s="27">
+      <c r="B15" s="54">
         <f>Analysis_Coding!G15</f>
         <v>1</v>
       </c>
-      <c r="C15" s="27">
+      <c r="C15" s="54">
         <f>Analysis_Coding!H15</f>
         <v>1</v>
       </c>
-      <c r="D15" s="27">
+      <c r="D15" s="54">
         <f>Analysis_Coding!I15</f>
         <v>1</v>
       </c>
-      <c r="E15" s="27">
+      <c r="E15" s="54">
         <f>Analysis_Coding!J15</f>
         <v>1</v>
       </c>
-      <c r="F15" s="27">
+      <c r="F15" s="54">
         <f>Analysis_Coding!K15</f>
         <v>0</v>
       </c>
-      <c r="G15" s="27">
+      <c r="G15" s="54">
         <f>Analysis_Coding!L15</f>
         <v>0</v>
       </c>
-      <c r="H15" s="27">
+      <c r="H15" s="54">
         <f>Analysis_Coding!M15</f>
         <v>1</v>
       </c>
-      <c r="I15" s="27">
+      <c r="I15" s="54">
         <f>Analysis_Coding!N15</f>
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="24" t="str">
         <f>GithubIssues!A16</f>
         <v>https://github.com/i-adopt/users_stories/issues/16</v>
       </c>
-      <c r="B16" s="27">
+      <c r="B16" s="54">
         <f>Analysis_Coding!G16</f>
         <v>0</v>
       </c>
-      <c r="C16" s="27">
+      <c r="C16" s="54">
         <f>Analysis_Coding!H16</f>
         <v>1</v>
       </c>
-      <c r="D16" s="27">
+      <c r="D16" s="54">
         <f>Analysis_Coding!I16</f>
         <v>1</v>
       </c>
-      <c r="E16" s="27">
+      <c r="E16" s="54">
         <f>Analysis_Coding!J16</f>
         <v>0</v>
       </c>
-      <c r="F16" s="27">
+      <c r="F16" s="54">
         <f>Analysis_Coding!K16</f>
         <v>0</v>
       </c>
-      <c r="G16" s="27">
+      <c r="G16" s="54">
         <f>Analysis_Coding!L16</f>
         <v>0</v>
       </c>
-      <c r="H16" s="27">
+      <c r="H16" s="54">
         <f>Analysis_Coding!M16</f>
         <v>0</v>
       </c>
-      <c r="I16" s="27">
+      <c r="I16" s="54">
         <f>Analysis_Coding!N16</f>
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="24" t="str">
         <f>GithubIssues!A17</f>
         <v>https://github.com/i-adopt/users_stories/issues/17</v>
       </c>
-      <c r="B17" s="27">
+      <c r="B17" s="54">
         <f>Analysis_Coding!G17</f>
         <v>0</v>
       </c>
-      <c r="C17" s="27">
+      <c r="C17" s="54">
         <f>Analysis_Coding!H17</f>
         <v>0</v>
       </c>
-      <c r="D17" s="27">
+      <c r="D17" s="54">
         <f>Analysis_Coding!I17</f>
         <v>0</v>
       </c>
-      <c r="E17" s="27">
+      <c r="E17" s="54">
         <f>Analysis_Coding!J17</f>
         <v>0</v>
       </c>
-      <c r="F17" s="27">
+      <c r="F17" s="54">
         <f>Analysis_Coding!K17</f>
         <v>0</v>
       </c>
-      <c r="G17" s="27">
+      <c r="G17" s="54">
         <f>Analysis_Coding!L17</f>
         <v>0</v>
       </c>
-      <c r="H17" s="27">
+      <c r="H17" s="54">
         <f>Analysis_Coding!M17</f>
         <v>1</v>
       </c>
-      <c r="I17" s="27">
+      <c r="I17" s="54">
         <f>Analysis_Coding!N17</f>
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="44"/>
-      <c r="B18" s="45"/>
-      <c r="C18" s="45"/>
-      <c r="D18" s="45"/>
-      <c r="E18" s="45"/>
-      <c r="F18" s="45"/>
-      <c r="G18" s="45"/>
-      <c r="H18" s="45"/>
-      <c r="I18" s="45"/>
-    </row>
-    <row r="19" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="44"/>
-      <c r="B19" s="45"/>
-      <c r="C19" s="45"/>
-      <c r="D19" s="45"/>
-      <c r="E19" s="45"/>
-      <c r="F19" s="45"/>
-      <c r="G19" s="45"/>
-      <c r="H19" s="45"/>
-      <c r="I19" s="45"/>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" s="32" t="s">
+    <row r="18" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="24" t="str">
+        <f>GithubIssues!A18</f>
+        <v>https://github.com/i-adopt/users_stories/issues/18</v>
+      </c>
+      <c r="B18" s="55">
+        <v>1</v>
+      </c>
+      <c r="C18" s="55"/>
+      <c r="D18" s="56">
+        <v>1</v>
+      </c>
+      <c r="E18" s="56"/>
+      <c r="F18" s="56"/>
+      <c r="G18" s="56">
+        <v>1</v>
+      </c>
+      <c r="H18" s="56">
+        <v>1</v>
+      </c>
+      <c r="I18" s="56"/>
+    </row>
+    <row r="19" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="24" t="str">
+        <f>GithubIssues!A19</f>
+        <v>https://github.com/i-adopt/users_stories/issues/19</v>
+      </c>
+      <c r="B19" s="55"/>
+      <c r="C19" s="55">
+        <v>1</v>
+      </c>
+      <c r="D19" s="56"/>
+      <c r="E19" s="56"/>
+      <c r="F19" s="56"/>
+      <c r="G19" s="56">
+        <v>1</v>
+      </c>
+      <c r="H19" s="56"/>
+      <c r="I19" s="56"/>
+    </row>
+    <row r="20" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="24" t="str">
+        <f>GithubIssues!A20</f>
+        <v>https://github.com/i-adopt/users_stories/issues/20</v>
+      </c>
+      <c r="B20" s="55"/>
+      <c r="C20" s="55">
+        <v>1</v>
+      </c>
+      <c r="D20" s="56">
+        <v>1</v>
+      </c>
+      <c r="E20" s="56"/>
+      <c r="F20" s="56"/>
+      <c r="G20" s="56"/>
+      <c r="H20" s="56"/>
+      <c r="I20" s="56"/>
+    </row>
+    <row r="21" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="24" t="str">
+        <f>GithubIssues!A21</f>
+        <v xml:space="preserve">https://github.com/i-adopt/users_stories/issues/21 </v>
+      </c>
+      <c r="B21" s="54">
+        <f>Analysis_Coding!G21</f>
+        <v>0</v>
+      </c>
+      <c r="C21" s="54">
+        <f>Analysis_Coding!H21</f>
+        <v>1</v>
+      </c>
+      <c r="D21" s="54">
+        <f>Analysis_Coding!I21</f>
+        <v>1</v>
+      </c>
+      <c r="E21" s="54">
+        <f>Analysis_Coding!J21</f>
+        <v>0</v>
+      </c>
+      <c r="F21" s="54">
+        <f>Analysis_Coding!K21</f>
+        <v>0</v>
+      </c>
+      <c r="G21" s="54">
+        <f>Analysis_Coding!L21</f>
+        <v>1</v>
+      </c>
+      <c r="H21" s="54">
+        <f>Analysis_Coding!M21</f>
+        <v>0</v>
+      </c>
+      <c r="I21" s="54">
+        <f>Analysis_Coding!N21</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="42"/>
+      <c r="B22" s="57"/>
+      <c r="C22" s="57"/>
+      <c r="D22" s="57"/>
+      <c r="E22" s="57"/>
+      <c r="F22" s="57"/>
+      <c r="G22" s="57"/>
+      <c r="H22" s="57"/>
+      <c r="I22" s="57"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A23" s="31" t="s">
         <v>168</v>
       </c>
-      <c r="B20" s="33">
-        <f>SUM(B2:B17)</f>
+      <c r="B23" s="58">
+        <f>SUM(B2:B21)</f>
+        <v>3</v>
+      </c>
+      <c r="C23" s="58">
+        <f>SUM(C2:C21)</f>
+        <v>11</v>
+      </c>
+      <c r="D23" s="58">
+        <f>SUM(D2:D21)</f>
+        <v>12</v>
+      </c>
+      <c r="E23" s="58">
+        <f>SUM(E2:E21)</f>
+        <v>3</v>
+      </c>
+      <c r="F23" s="58">
+        <f>SUM(F2:F21)</f>
+        <v>1</v>
+      </c>
+      <c r="G23" s="58">
+        <f>SUM(G2:G21)</f>
+        <v>8</v>
+      </c>
+      <c r="H23" s="58">
+        <f>SUM(H2:H21)</f>
+        <v>3</v>
+      </c>
+      <c r="I23" s="58">
+        <f>SUM(I2:I21)</f>
         <v>2</v>
       </c>
-      <c r="C20" s="33">
-        <f t="shared" ref="C20:I20" si="0">SUM(C2:C17)</f>
-        <v>8</v>
-      </c>
-      <c r="D20" s="33">
-        <f t="shared" si="0"/>
-        <v>9</v>
-      </c>
-      <c r="E20" s="33">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="F20" s="33">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="G20" s="33">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="H20" s="33">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="I20" s="33">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>169</v>
-      </c>
-      <c r="B21">
-        <v>16</v>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>201</v>
+      </c>
+      <c r="B24">
+        <f>SUM(B23:I23)</f>
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>